<commit_message>
senescence warm fall and budset
</commit_message>
<xml_diff>
--- a/data/monitoring_phenology/2024_budburst_to_budset.xlsx
+++ b/data/monitoring_phenology/2024_budburst_to_budset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/data/monitoring_phenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEA18F0-3D0F-DC4E-AB03-E9773386FFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB36AE50-0B81-CB49-AF79-8733B90D2464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phenological_monitoring" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5171" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5179" uniqueCount="740">
   <si>
     <t>tree_ID</t>
   </si>
@@ -2252,6 +2252,12 @@
   <si>
     <t>doy255: apical shoot dead</t>
   </si>
+  <si>
+    <t>doy262:bud eaten</t>
+  </si>
+  <si>
+    <t>doy262:bud bursting again</t>
+  </si>
 </sst>
 </file>
 
@@ -2755,12 +2761,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -3515,11 +3520,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM631"/>
+  <dimension ref="A1:AN631"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM542" sqref="AM542:AM631"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AN115" sqref="AN115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3531,7 +3536,7 @@
     <col min="30" max="30" width="4.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3649,8 +3654,11 @@
       <c r="AM1" s="3">
         <v>256</v>
       </c>
+      <c r="AN1" s="3">
+        <v>262</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3768,8 +3776,11 @@
       <c r="AM2">
         <v>5</v>
       </c>
+      <c r="AN2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3884,8 +3895,11 @@
       <c r="AM3">
         <v>5</v>
       </c>
+      <c r="AN3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4000,8 +4014,11 @@
       <c r="AM4">
         <v>5</v>
       </c>
+      <c r="AN4">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -4116,8 +4133,11 @@
       <c r="AM5">
         <v>5</v>
       </c>
+      <c r="AN5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -4232,8 +4252,11 @@
       <c r="AM6">
         <v>5</v>
       </c>
+      <c r="AN6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -4348,8 +4371,11 @@
       <c r="AM7">
         <v>6</v>
       </c>
+      <c r="AN7">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -4464,8 +4490,11 @@
       <c r="AM8">
         <v>6</v>
       </c>
+      <c r="AN8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -4580,8 +4609,11 @@
       <c r="AM9">
         <v>6</v>
       </c>
+      <c r="AN9">
+        <v>6</v>
+      </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -4696,8 +4728,11 @@
       <c r="AM10">
         <v>6</v>
       </c>
+      <c r="AN10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -4815,8 +4850,11 @@
       <c r="AM11">
         <v>6</v>
       </c>
+      <c r="AN11">
+        <v>6</v>
+      </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -4931,8 +4969,11 @@
       <c r="AM12">
         <v>5</v>
       </c>
+      <c r="AN12">
+        <v>5</v>
+      </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -5047,8 +5088,11 @@
       <c r="AM13">
         <v>5</v>
       </c>
+      <c r="AN13">
+        <v>5</v>
+      </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -5163,8 +5207,11 @@
       <c r="AM14">
         <v>5</v>
       </c>
+      <c r="AN14">
+        <v>5</v>
+      </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -5279,8 +5326,11 @@
       <c r="AM15">
         <v>5</v>
       </c>
+      <c r="AN15">
+        <v>5</v>
+      </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -5395,8 +5445,11 @@
       <c r="AM16">
         <v>5</v>
       </c>
+      <c r="AN16">
+        <v>5</v>
+      </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -5511,8 +5564,11 @@
       <c r="AM17">
         <v>5</v>
       </c>
+      <c r="AN17">
+        <v>6</v>
+      </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -5627,8 +5683,11 @@
       <c r="AM18">
         <v>5</v>
       </c>
+      <c r="AN18">
+        <v>6</v>
+      </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -5743,8 +5802,11 @@
       <c r="AM19">
         <v>6</v>
       </c>
+      <c r="AN19">
+        <v>6</v>
+      </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -5859,8 +5921,11 @@
       <c r="AM20">
         <v>5</v>
       </c>
+      <c r="AN20">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -5975,8 +6040,11 @@
       <c r="AM21">
         <v>5</v>
       </c>
+      <c r="AN21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -6094,8 +6162,11 @@
       <c r="AM22">
         <v>6</v>
       </c>
+      <c r="AN22">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -6210,8 +6281,11 @@
       <c r="AM23">
         <v>6</v>
       </c>
+      <c r="AN23">
+        <v>6</v>
+      </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -6326,8 +6400,11 @@
       <c r="AM24">
         <v>5</v>
       </c>
+      <c r="AN24">
+        <v>5</v>
+      </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -6442,8 +6519,11 @@
       <c r="AM25">
         <v>6</v>
       </c>
+      <c r="AN25">
+        <v>6</v>
+      </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -6558,8 +6638,11 @@
       <c r="AM26">
         <v>5</v>
       </c>
+      <c r="AN26">
+        <v>5</v>
+      </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -6674,8 +6757,11 @@
       <c r="AM27">
         <v>5</v>
       </c>
+      <c r="AN27">
+        <v>5</v>
+      </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -6793,8 +6879,11 @@
       <c r="AM28">
         <v>5</v>
       </c>
+      <c r="AN28">
+        <v>6</v>
+      </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -6810,6 +6899,9 @@
       <c r="E29" t="s">
         <v>9</v>
       </c>
+      <c r="F29" t="s">
+        <v>738</v>
+      </c>
       <c r="G29">
         <v>4</v>
       </c>
@@ -6909,8 +7001,11 @@
       <c r="AM29">
         <v>4</v>
       </c>
+      <c r="AN29" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -7025,8 +7120,11 @@
       <c r="AM30">
         <v>5</v>
       </c>
+      <c r="AN30">
+        <v>5</v>
+      </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -7141,8 +7239,11 @@
       <c r="AM31">
         <v>6</v>
       </c>
+      <c r="AN31">
+        <v>6</v>
+      </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -7258,7 +7359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -7374,7 +7475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -7490,7 +7591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -7606,7 +7707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -7722,7 +7823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -7838,7 +7939,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -7954,7 +8055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -8070,7 +8171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -8186,7 +8287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -8302,7 +8403,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -8421,7 +8522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -8537,7 +8638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -8653,7 +8754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -8769,7 +8870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -8885,7 +8986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -9000,8 +9101,11 @@
       <c r="AM47">
         <v>6</v>
       </c>
+      <c r="AN47">
+        <v>6</v>
+      </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -9116,8 +9220,11 @@
       <c r="AM48">
         <v>5</v>
       </c>
+      <c r="AN48">
+        <v>5</v>
+      </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -9232,8 +9339,11 @@
       <c r="AM49">
         <v>4</v>
       </c>
+      <c r="AN49">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -9348,8 +9458,11 @@
       <c r="AM50">
         <v>6</v>
       </c>
+      <c r="AN50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -9464,8 +9577,11 @@
       <c r="AM51">
         <v>6</v>
       </c>
+      <c r="AN51">
+        <v>6</v>
+      </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -9580,8 +9696,11 @@
       <c r="AM52">
         <v>0</v>
       </c>
+      <c r="AN52">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -9696,8 +9815,11 @@
       <c r="AM53">
         <v>6</v>
       </c>
+      <c r="AN53">
+        <v>6</v>
+      </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -9812,8 +9934,11 @@
       <c r="AM54">
         <v>6</v>
       </c>
+      <c r="AN54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -9931,8 +10056,11 @@
       <c r="AM55">
         <v>6</v>
       </c>
+      <c r="AN55">
+        <v>6</v>
+      </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -10050,8 +10178,11 @@
       <c r="AM56">
         <v>0</v>
       </c>
+      <c r="AN56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -10169,8 +10300,11 @@
       <c r="AM57">
         <v>6</v>
       </c>
+      <c r="AN57">
+        <v>6</v>
+      </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -10285,8 +10419,11 @@
       <c r="AM58">
         <v>6</v>
       </c>
+      <c r="AN58">
+        <v>6</v>
+      </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -10401,8 +10538,11 @@
       <c r="AM59" t="s">
         <v>308</v>
       </c>
+      <c r="AN59" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -10517,8 +10657,11 @@
       <c r="AM60">
         <v>6</v>
       </c>
+      <c r="AN60">
+        <v>6</v>
+      </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -10633,8 +10776,11 @@
       <c r="AM61">
         <v>6</v>
       </c>
+      <c r="AN61">
+        <v>6</v>
+      </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -10750,7 +10896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -10866,7 +11012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -12841,7 +12987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>94</v>
       </c>
@@ -12957,7 +13103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>95</v>
       </c>
@@ -13073,7 +13219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>96</v>
       </c>
@@ -13189,7 +13335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>97</v>
       </c>
@@ -13305,7 +13451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>98</v>
       </c>
@@ -13421,7 +13567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>99</v>
       </c>
@@ -13537,7 +13683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>100</v>
       </c>
@@ -13653,7 +13799,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>101</v>
       </c>
@@ -13769,7 +13915,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>102</v>
       </c>
@@ -13885,7 +14031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>103</v>
       </c>
@@ -14001,7 +14147,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>104</v>
       </c>
@@ -14117,7 +14263,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>105</v>
       </c>
@@ -14232,8 +14378,11 @@
       <c r="AM92">
         <v>6</v>
       </c>
+      <c r="AN92">
+        <v>6</v>
+      </c>
     </row>
-    <row r="93" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -14348,8 +14497,11 @@
       <c r="AM93">
         <v>6</v>
       </c>
+      <c r="AN93">
+        <v>6</v>
+      </c>
     </row>
-    <row r="94" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -14464,8 +14616,11 @@
       <c r="AM94">
         <v>6</v>
       </c>
+      <c r="AN94">
+        <v>6</v>
+      </c>
     </row>
-    <row r="95" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -14583,8 +14738,11 @@
       <c r="AM95">
         <v>6</v>
       </c>
+      <c r="AN95">
+        <v>6</v>
+      </c>
     </row>
-    <row r="96" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>112</v>
       </c>
@@ -14699,8 +14857,11 @@
       <c r="AM96">
         <v>6</v>
       </c>
+      <c r="AN96">
+        <v>6</v>
+      </c>
     </row>
-    <row r="97" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>113</v>
       </c>
@@ -14815,8 +14976,11 @@
       <c r="AM97">
         <v>6</v>
       </c>
+      <c r="AN97" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="98" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>114</v>
       </c>
@@ -14931,8 +15095,11 @@
       <c r="AM98">
         <v>6</v>
       </c>
+      <c r="AN98" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="99" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>115</v>
       </c>
@@ -15047,8 +15214,11 @@
       <c r="AM99">
         <v>6</v>
       </c>
+      <c r="AN99" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="100" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>116</v>
       </c>
@@ -15163,8 +15333,11 @@
       <c r="AM100">
         <v>6</v>
       </c>
+      <c r="AN100" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="101" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>117</v>
       </c>
@@ -15279,8 +15452,11 @@
       <c r="AM101">
         <v>6</v>
       </c>
+      <c r="AN101" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="102" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>118</v>
       </c>
@@ -15395,8 +15571,11 @@
       <c r="AM102">
         <v>6</v>
       </c>
+      <c r="AN102" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="103" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>119</v>
       </c>
@@ -15511,8 +15690,11 @@
       <c r="AM103">
         <v>6</v>
       </c>
+      <c r="AN103" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="104" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>120</v>
       </c>
@@ -15627,8 +15809,11 @@
       <c r="AM104">
         <v>6</v>
       </c>
+      <c r="AN104" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="105" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>121</v>
       </c>
@@ -15743,8 +15928,11 @@
       <c r="AM105">
         <v>6</v>
       </c>
+      <c r="AN105" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="106" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>122</v>
       </c>
@@ -15859,8 +16047,11 @@
       <c r="AM106">
         <v>6</v>
       </c>
+      <c r="AN106" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="107" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -15975,8 +16166,11 @@
       <c r="AM107" s="2">
         <v>6</v>
       </c>
+      <c r="AN107" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="108" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>124</v>
       </c>
@@ -16091,8 +16285,11 @@
       <c r="AM108" s="2">
         <v>6</v>
       </c>
+      <c r="AN108" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="109" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>125</v>
       </c>
@@ -16210,8 +16407,11 @@
       <c r="AM109" s="2">
         <v>6</v>
       </c>
+      <c r="AN109" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="110" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -16326,8 +16526,11 @@
       <c r="AM110" s="2">
         <v>0</v>
       </c>
+      <c r="AN110" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="111" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>127</v>
       </c>
@@ -16343,6 +16546,9 @@
       <c r="E111" t="s">
         <v>107</v>
       </c>
+      <c r="F111" t="s">
+        <v>739</v>
+      </c>
       <c r="G111">
         <v>4</v>
       </c>
@@ -16442,8 +16648,11 @@
       <c r="AM111" s="2">
         <v>6</v>
       </c>
+      <c r="AN111" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="112" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>128</v>
       </c>
@@ -16558,8 +16767,11 @@
       <c r="AM112">
         <v>6</v>
       </c>
+      <c r="AN112" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="113" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -16674,8 +16886,11 @@
       <c r="AM113" t="s">
         <v>308</v>
       </c>
+      <c r="AN113" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="114" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -16790,8 +17005,11 @@
       <c r="AM114">
         <v>6</v>
       </c>
+      <c r="AN114" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="115" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>131</v>
       </c>
@@ -16906,8 +17124,11 @@
       <c r="AM115">
         <v>6</v>
       </c>
+      <c r="AN115" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="116" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>132</v>
       </c>
@@ -17022,8 +17243,11 @@
       <c r="AM116">
         <v>6</v>
       </c>
+      <c r="AN116" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="117" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>133</v>
       </c>
@@ -17138,8 +17362,11 @@
       <c r="AM117">
         <v>6</v>
       </c>
+      <c r="AN117" s="2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="118" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>134</v>
       </c>
@@ -17254,8 +17481,11 @@
       <c r="AM118">
         <v>6</v>
       </c>
+      <c r="AN118">
+        <v>6</v>
+      </c>
     </row>
-    <row r="119" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -17370,8 +17600,11 @@
       <c r="AM119">
         <v>6</v>
       </c>
+      <c r="AN119">
+        <v>6</v>
+      </c>
     </row>
-    <row r="120" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>136</v>
       </c>
@@ -17486,8 +17719,11 @@
       <c r="AM120">
         <v>6</v>
       </c>
+      <c r="AN120">
+        <v>6</v>
+      </c>
     </row>
-    <row r="121" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>137</v>
       </c>
@@ -17605,8 +17841,11 @@
       <c r="AM121">
         <v>6</v>
       </c>
+      <c r="AN121">
+        <v>6</v>
+      </c>
     </row>
-    <row r="122" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>138</v>
       </c>
@@ -17722,7 +17961,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>139</v>
       </c>
@@ -17838,7 +18077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>140</v>
       </c>
@@ -17954,7 +18193,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>141</v>
       </c>
@@ -18070,7 +18309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>142</v>
       </c>
@@ -18186,7 +18425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="127" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>143</v>
       </c>
@@ -18302,7 +18541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>144</v>
       </c>
@@ -18418,7 +18657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>145</v>
       </c>
@@ -18534,7 +18773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="130" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>146</v>
       </c>
@@ -18650,7 +18889,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="131" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>147</v>
       </c>
@@ -18769,7 +19008,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="132" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>148</v>
       </c>
@@ -18885,7 +19124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>149</v>
       </c>
@@ -19001,7 +19240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>150</v>
       </c>
@@ -19117,7 +19356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>151</v>
       </c>
@@ -19233,7 +19472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>152</v>
       </c>
@@ -19349,7 +19588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>153</v>
       </c>
@@ -19365,6 +19604,9 @@
       <c r="E137" t="s">
         <v>107</v>
       </c>
+      <c r="F137" t="s">
+        <v>739</v>
+      </c>
       <c r="G137" t="s">
         <v>10</v>
       </c>
@@ -19464,8 +19706,11 @@
       <c r="AM137">
         <v>6</v>
       </c>
+      <c r="AN137" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="138" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>154</v>
       </c>
@@ -19580,8 +19825,11 @@
       <c r="AM138">
         <v>6</v>
       </c>
+      <c r="AN138" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="139" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>155</v>
       </c>
@@ -19696,8 +19944,11 @@
       <c r="AM139">
         <v>6</v>
       </c>
+      <c r="AN139" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="140" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>156</v>
       </c>
@@ -19812,8 +20063,11 @@
       <c r="AM140">
         <v>0</v>
       </c>
+      <c r="AN140" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="141" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>157</v>
       </c>
@@ -19928,8 +20182,11 @@
       <c r="AM141">
         <v>6</v>
       </c>
+      <c r="AN141" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="142" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>158</v>
       </c>
@@ -20044,8 +20301,11 @@
       <c r="AM142">
         <v>6</v>
       </c>
+      <c r="AN142" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="143" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>159</v>
       </c>
@@ -20160,8 +20420,11 @@
       <c r="AM143">
         <v>6</v>
       </c>
+      <c r="AN143" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="144" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>160</v>
       </c>
@@ -20276,8 +20539,11 @@
       <c r="AM144">
         <v>6</v>
       </c>
+      <c r="AN144" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="145" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>161</v>
       </c>
@@ -20392,8 +20658,11 @@
       <c r="AM145">
         <v>6</v>
       </c>
+      <c r="AN145" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="146" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>162</v>
       </c>
@@ -20508,8 +20777,11 @@
       <c r="AM146">
         <v>6</v>
       </c>
+      <c r="AN146" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="147" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>163</v>
       </c>
@@ -20624,8 +20896,11 @@
       <c r="AM147">
         <v>6</v>
       </c>
+      <c r="AN147" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="148" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>164</v>
       </c>
@@ -20641,6 +20916,9 @@
       <c r="E148" t="s">
         <v>107</v>
       </c>
+      <c r="F148" t="s">
+        <v>739</v>
+      </c>
       <c r="G148" t="s">
         <v>10</v>
       </c>
@@ -20740,8 +21018,11 @@
       <c r="AM148">
         <v>6</v>
       </c>
+      <c r="AN148" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="149" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>165</v>
       </c>
@@ -20856,8 +21137,11 @@
       <c r="AM149">
         <v>6</v>
       </c>
+      <c r="AN149" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="150" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>166</v>
       </c>
@@ -20873,6 +21157,9 @@
       <c r="E150" t="s">
         <v>107</v>
       </c>
+      <c r="F150" t="s">
+        <v>739</v>
+      </c>
       <c r="G150" t="s">
         <v>10</v>
       </c>
@@ -20972,8 +21259,11 @@
       <c r="AM150">
         <v>6</v>
       </c>
+      <c r="AN150" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="151" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>167</v>
       </c>
@@ -21088,8 +21378,11 @@
       <c r="AM151">
         <v>0</v>
       </c>
+      <c r="AN151" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="152" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>168</v>
       </c>
@@ -21205,7 +21498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>169</v>
       </c>
@@ -21321,7 +21614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>170</v>
       </c>
@@ -21437,7 +21730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>171</v>
       </c>
@@ -21553,7 +21846,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:40" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>172</v>
       </c>
@@ -21669,7 +21962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>173</v>
       </c>
@@ -21785,7 +22078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>174</v>
       </c>
@@ -21901,7 +22194,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>175</v>
       </c>
@@ -22017,7 +22310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>176</v>
       </c>
@@ -46753,7 +47046,7 @@
       <c r="AL373">
         <v>6</v>
       </c>
-      <c r="AM373" s="4">
+      <c r="AM373">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding missing pheno data
</commit_message>
<xml_diff>
--- a/data/monitoring_phenology/2024_budburst_to_budset.xlsx
+++ b/data/monitoring_phenology/2024_budburst_to_budset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/data/monitoring_phenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3308EF6-D5B8-444D-BFA7-D5B111F5FE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5BE840-56CC-234F-AD08-85F111EC012E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phenological_monitoring" sheetId="1" r:id="rId1"/>
@@ -2773,13 +2773,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -3536,8 +3534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN631"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AN467" sqref="AN467"/>
     </sheetView>
   </sheetViews>
@@ -22901,7 +22899,6 @@
       <c r="E163" t="s">
         <v>107</v>
       </c>
-      <c r="F163" s="4"/>
       <c r="G163" t="s">
         <v>10</v>
       </c>
@@ -42653,7 +42650,7 @@
       <c r="AM329">
         <v>5</v>
       </c>
-      <c r="AN329" s="5">
+      <c r="AN329">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
budset and sensesncence in climate chambers
</commit_message>
<xml_diff>
--- a/data/monitoring_phenology/2024_budburst_to_budset.xlsx
+++ b/data/monitoring_phenology/2024_budburst_to_budset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/data/monitoring_phenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5BE840-56CC-234F-AD08-85F111EC012E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEF62B8-BB03-754F-96E3-FB434113EFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phenological_monitoring" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5317" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5333" uniqueCount="745">
   <si>
     <t>tree_ID</t>
   </si>
@@ -2270,6 +2270,9 @@
   <si>
     <t>doy262: bud bursting again. Leaf unfolding</t>
   </si>
+  <si>
+    <t>doy276: seems like it flushed and starts to set bud again</t>
+  </si>
 </sst>
 </file>
 
@@ -3532,11 +3535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN631"/>
+  <dimension ref="A1:AO631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AN467" sqref="AN467"/>
+    <sheetView tabSelected="1" topLeftCell="A256" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AO267" sqref="AO267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3548,7 +3551,7 @@
     <col min="30" max="30" width="4.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3669,8 +3672,11 @@
       <c r="AN1" s="3">
         <v>262</v>
       </c>
+      <c r="AO1" s="3">
+        <v>276</v>
+      </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3792,7 +3798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3911,7 +3917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4030,7 +4036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -4149,7 +4155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -4268,7 +4274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -4387,7 +4393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -4506,7 +4512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -4625,7 +4631,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -4744,7 +4750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -4866,7 +4872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -4985,7 +4991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -5104,7 +5110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -5223,7 +5229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -5342,7 +5348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -5461,7 +5467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -5580,7 +5586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -5699,7 +5705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -5818,7 +5824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -5937,7 +5943,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -6056,7 +6062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -6178,7 +6184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -6297,7 +6303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -6416,7 +6422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -6535,7 +6541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -6654,7 +6660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -6773,7 +6779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -6895,7 +6901,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -7017,7 +7023,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -7136,7 +7142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -7255,7 +7261,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -7373,8 +7379,11 @@
       <c r="AN32">
         <v>4</v>
       </c>
+      <c r="AO32">
+        <v>6</v>
+      </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -7492,8 +7501,11 @@
       <c r="AN33">
         <v>6</v>
       </c>
+      <c r="AO33">
+        <v>6</v>
+      </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -7611,8 +7623,11 @@
       <c r="AN34">
         <v>5</v>
       </c>
+      <c r="AO34">
+        <v>5</v>
+      </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -7730,8 +7745,11 @@
       <c r="AN35">
         <v>6</v>
       </c>
+      <c r="AO35">
+        <v>6</v>
+      </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -7849,8 +7867,11 @@
       <c r="AN36">
         <v>5</v>
       </c>
+      <c r="AO36">
+        <v>6</v>
+      </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -7968,8 +7989,11 @@
       <c r="AN37">
         <v>6</v>
       </c>
+      <c r="AO37">
+        <v>6</v>
+      </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -8087,8 +8111,11 @@
       <c r="AN38">
         <v>6</v>
       </c>
+      <c r="AO38">
+        <v>6</v>
+      </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -8206,8 +8233,11 @@
       <c r="AN39">
         <v>6</v>
       </c>
+      <c r="AO39">
+        <v>6</v>
+      </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -8325,8 +8355,11 @@
       <c r="AN40">
         <v>5</v>
       </c>
+      <c r="AO40">
+        <v>6</v>
+      </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -8444,8 +8477,11 @@
       <c r="AN41">
         <v>6</v>
       </c>
+      <c r="AO41">
+        <v>6</v>
+      </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -8566,8 +8602,11 @@
       <c r="AN42">
         <v>5</v>
       </c>
+      <c r="AO42">
+        <v>6</v>
+      </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -8685,8 +8724,11 @@
       <c r="AN43">
         <v>6</v>
       </c>
+      <c r="AO43">
+        <v>6</v>
+      </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -8804,8 +8846,11 @@
       <c r="AN44">
         <v>6</v>
       </c>
+      <c r="AO44">
+        <v>6</v>
+      </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -8923,8 +8968,11 @@
       <c r="AN45">
         <v>6</v>
       </c>
+      <c r="AO45">
+        <v>6</v>
+      </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -9042,8 +9090,11 @@
       <c r="AN46">
         <v>5</v>
       </c>
+      <c r="AO46">
+        <v>6</v>
+      </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -9162,7 +9213,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -9281,7 +9332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -9400,7 +9451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -9519,7 +9570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -9638,7 +9689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -9757,7 +9808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -9876,7 +9927,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -9995,7 +10046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -10117,7 +10168,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -10239,7 +10290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -10361,7 +10412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -10480,7 +10531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -10599,7 +10650,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -10718,7 +10769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -10837,7 +10888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -10955,8 +11006,11 @@
       <c r="AN62">
         <v>6</v>
       </c>
+      <c r="AO62">
+        <v>6</v>
+      </c>
     </row>
-    <row r="63" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -11074,8 +11128,11 @@
       <c r="AN63">
         <v>6</v>
       </c>
+      <c r="AO63">
+        <v>6</v>
+      </c>
     </row>
-    <row r="64" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -11193,8 +11250,11 @@
       <c r="AN64">
         <v>6</v>
       </c>
+      <c r="AO64">
+        <v>6</v>
+      </c>
     </row>
-    <row r="65" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -11312,8 +11372,11 @@
       <c r="AN65">
         <v>6</v>
       </c>
+      <c r="AO65">
+        <v>6</v>
+      </c>
     </row>
-    <row r="66" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -11431,8 +11494,11 @@
       <c r="AN66">
         <v>4</v>
       </c>
+      <c r="AO66">
+        <v>5</v>
+      </c>
     </row>
-    <row r="67" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -11550,8 +11616,11 @@
       <c r="AN67">
         <v>6</v>
       </c>
+      <c r="AO67">
+        <v>6</v>
+      </c>
     </row>
-    <row r="68" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -11669,8 +11738,11 @@
       <c r="AN68">
         <v>6</v>
       </c>
+      <c r="AO68">
+        <v>6</v>
+      </c>
     </row>
-    <row r="69" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>81</v>
       </c>
@@ -11788,8 +11860,11 @@
       <c r="AN69">
         <v>6</v>
       </c>
+      <c r="AO69">
+        <v>6</v>
+      </c>
     </row>
-    <row r="70" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -11907,8 +11982,11 @@
       <c r="AN70">
         <v>6</v>
       </c>
+      <c r="AO70">
+        <v>6</v>
+      </c>
     </row>
-    <row r="71" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -12029,8 +12107,11 @@
       <c r="AN71" t="s">
         <v>308</v>
       </c>
+      <c r="AO71" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="72" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>84</v>
       </c>
@@ -12148,8 +12229,11 @@
       <c r="AN72" s="2">
         <v>6</v>
       </c>
+      <c r="AO72">
+        <v>6</v>
+      </c>
     </row>
-    <row r="73" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -12267,8 +12351,11 @@
       <c r="AN73" s="2">
         <v>6</v>
       </c>
+      <c r="AO73">
+        <v>6</v>
+      </c>
     </row>
-    <row r="74" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>86</v>
       </c>
@@ -12386,8 +12473,11 @@
       <c r="AN74" s="2">
         <v>6</v>
       </c>
+      <c r="AO74">
+        <v>6</v>
+      </c>
     </row>
-    <row r="75" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -12505,8 +12595,11 @@
       <c r="AN75" s="2">
         <v>6</v>
       </c>
+      <c r="AO75">
+        <v>6</v>
+      </c>
     </row>
-    <row r="76" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -12624,8 +12717,11 @@
       <c r="AN76" s="2">
         <v>6</v>
       </c>
+      <c r="AO76">
+        <v>6</v>
+      </c>
     </row>
-    <row r="77" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>89</v>
       </c>
@@ -12743,8 +12839,11 @@
       <c r="AN77" s="2">
         <v>6</v>
       </c>
+      <c r="AO77" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="78" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>91</v>
       </c>
@@ -12862,8 +12961,11 @@
       <c r="AN78" s="2">
         <v>6</v>
       </c>
+      <c r="AO78" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="79" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>92</v>
       </c>
@@ -12981,8 +13083,11 @@
       <c r="AN79" s="2">
         <v>6</v>
       </c>
+      <c r="AO79" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="80" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>93</v>
       </c>
@@ -13100,8 +13205,11 @@
       <c r="AN80" s="2">
         <v>6</v>
       </c>
+      <c r="AO80" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="81" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>94</v>
       </c>
@@ -13219,8 +13327,11 @@
       <c r="AN81" s="2">
         <v>6</v>
       </c>
+      <c r="AO81" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="82" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>95</v>
       </c>
@@ -13338,8 +13449,11 @@
       <c r="AN82" s="2">
         <v>6</v>
       </c>
+      <c r="AO82" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="83" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>96</v>
       </c>
@@ -13457,8 +13571,11 @@
       <c r="AN83" s="2">
         <v>6</v>
       </c>
+      <c r="AO83" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="84" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>97</v>
       </c>
@@ -13576,8 +13693,11 @@
       <c r="AN84" s="2">
         <v>6</v>
       </c>
+      <c r="AO84" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="85" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>98</v>
       </c>
@@ -13695,8 +13815,11 @@
       <c r="AN85" s="2">
         <v>6</v>
       </c>
+      <c r="AO85" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="86" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>99</v>
       </c>
@@ -13814,8 +13937,11 @@
       <c r="AN86" s="2">
         <v>6</v>
       </c>
+      <c r="AO86" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="87" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>100</v>
       </c>
@@ -13933,8 +14059,11 @@
       <c r="AN87" s="2">
         <v>6</v>
       </c>
+      <c r="AO87" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="88" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>101</v>
       </c>
@@ -14052,8 +14181,11 @@
       <c r="AN88" s="2">
         <v>6</v>
       </c>
+      <c r="AO88" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="89" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>102</v>
       </c>
@@ -14171,8 +14303,11 @@
       <c r="AN89" s="2">
         <v>6</v>
       </c>
+      <c r="AO89" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="90" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>103</v>
       </c>
@@ -14290,8 +14425,11 @@
       <c r="AN90" s="2">
         <v>6</v>
       </c>
+      <c r="AO90" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="91" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>104</v>
       </c>
@@ -14409,8 +14547,11 @@
       <c r="AN91" s="2">
         <v>6</v>
       </c>
+      <c r="AO91" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="92" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>105</v>
       </c>
@@ -14529,7 +14670,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -14648,7 +14789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -14767,7 +14908,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -14889,7 +15030,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>112</v>
       </c>
@@ -16918,7 +17059,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -17037,7 +17178,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="114" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -17156,7 +17297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>131</v>
       </c>
@@ -17275,7 +17416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>132</v>
       </c>
@@ -17394,7 +17535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>133</v>
       </c>
@@ -17513,7 +17654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>134</v>
       </c>
@@ -17632,7 +17773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -17751,7 +17892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>136</v>
       </c>
@@ -17870,7 +18011,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>137</v>
       </c>
@@ -17992,7 +18133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>138</v>
       </c>
@@ -18110,8 +18251,11 @@
       <c r="AN122">
         <v>6</v>
       </c>
+      <c r="AO122">
+        <v>6</v>
+      </c>
     </row>
-    <row r="123" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>139</v>
       </c>
@@ -18229,8 +18373,11 @@
       <c r="AN123">
         <v>6</v>
       </c>
+      <c r="AO123">
+        <v>6</v>
+      </c>
     </row>
-    <row r="124" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>140</v>
       </c>
@@ -18348,8 +18495,11 @@
       <c r="AN124">
         <v>6</v>
       </c>
+      <c r="AO124">
+        <v>6</v>
+      </c>
     </row>
-    <row r="125" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>141</v>
       </c>
@@ -18467,8 +18617,11 @@
       <c r="AN125">
         <v>6</v>
       </c>
+      <c r="AO125">
+        <v>6</v>
+      </c>
     </row>
-    <row r="126" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>142</v>
       </c>
@@ -18586,8 +18739,11 @@
       <c r="AN126">
         <v>6</v>
       </c>
+      <c r="AO126">
+        <v>6</v>
+      </c>
     </row>
-    <row r="127" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>143</v>
       </c>
@@ -18705,8 +18861,11 @@
       <c r="AN127">
         <v>6</v>
       </c>
+      <c r="AO127">
+        <v>6</v>
+      </c>
     </row>
-    <row r="128" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>144</v>
       </c>
@@ -18824,8 +18983,11 @@
       <c r="AN128">
         <v>6</v>
       </c>
+      <c r="AO128">
+        <v>6</v>
+      </c>
     </row>
-    <row r="129" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>145</v>
       </c>
@@ -18943,8 +19105,11 @@
       <c r="AN129">
         <v>6</v>
       </c>
+      <c r="AO129">
+        <v>0</v>
+      </c>
     </row>
-    <row r="130" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>146</v>
       </c>
@@ -19062,8 +19227,11 @@
       <c r="AN130">
         <v>6</v>
       </c>
+      <c r="AO130">
+        <v>6</v>
+      </c>
     </row>
-    <row r="131" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>147</v>
       </c>
@@ -19184,8 +19352,11 @@
       <c r="AN131" t="s">
         <v>308</v>
       </c>
+      <c r="AO131" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="132" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>148</v>
       </c>
@@ -19303,8 +19474,11 @@
       <c r="AN132">
         <v>6</v>
       </c>
+      <c r="AO132">
+        <v>6</v>
+      </c>
     </row>
-    <row r="133" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>149</v>
       </c>
@@ -19422,8 +19596,11 @@
       <c r="AN133">
         <v>6</v>
       </c>
+      <c r="AO133">
+        <v>6</v>
+      </c>
     </row>
-    <row r="134" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>150</v>
       </c>
@@ -19541,8 +19718,11 @@
       <c r="AN134">
         <v>6</v>
       </c>
+      <c r="AO134">
+        <v>6</v>
+      </c>
     </row>
-    <row r="135" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>151</v>
       </c>
@@ -19660,8 +19840,11 @@
       <c r="AN135">
         <v>6</v>
       </c>
+      <c r="AO135">
+        <v>6</v>
+      </c>
     </row>
-    <row r="136" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>152</v>
       </c>
@@ -19779,8 +19962,11 @@
       <c r="AN136">
         <v>6</v>
       </c>
+      <c r="AO136">
+        <v>6</v>
+      </c>
     </row>
-    <row r="137" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>153</v>
       </c>
@@ -19902,7 +20088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>154</v>
       </c>
@@ -20021,7 +20207,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>155</v>
       </c>
@@ -20140,7 +20326,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>156</v>
       </c>
@@ -20259,7 +20445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>157</v>
       </c>
@@ -20378,7 +20564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>158</v>
       </c>
@@ -20497,7 +20683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>159</v>
       </c>
@@ -20616,7 +20802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>160</v>
       </c>
@@ -20735,7 +20921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>161</v>
       </c>
@@ -20854,7 +21040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>162</v>
       </c>
@@ -20973,7 +21159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="147" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>163</v>
       </c>
@@ -21092,7 +21278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>164</v>
       </c>
@@ -21214,7 +21400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>165</v>
       </c>
@@ -21333,7 +21519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="150" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>166</v>
       </c>
@@ -21455,7 +21641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>167</v>
       </c>
@@ -21574,7 +21760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>168</v>
       </c>
@@ -21692,8 +21878,11 @@
       <c r="AN152" s="2">
         <v>6</v>
       </c>
+      <c r="AO152">
+        <v>0</v>
+      </c>
     </row>
-    <row r="153" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>169</v>
       </c>
@@ -21811,8 +22000,11 @@
       <c r="AN153" s="2">
         <v>0</v>
       </c>
+      <c r="AO153">
+        <v>0</v>
+      </c>
     </row>
-    <row r="154" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>170</v>
       </c>
@@ -21930,8 +22122,11 @@
       <c r="AN154" s="2">
         <v>6</v>
       </c>
+      <c r="AO154">
+        <v>6</v>
+      </c>
     </row>
-    <row r="155" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>171</v>
       </c>
@@ -22049,8 +22244,11 @@
       <c r="AN155" s="2">
         <v>6</v>
       </c>
+      <c r="AO155">
+        <v>6</v>
+      </c>
     </row>
-    <row r="156" spans="1:40" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:41" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>172</v>
       </c>
@@ -22168,8 +22366,11 @@
       <c r="AN156" s="2">
         <v>6</v>
       </c>
+      <c r="AO156">
+        <v>6</v>
+      </c>
     </row>
-    <row r="157" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>173</v>
       </c>
@@ -22287,8 +22488,11 @@
       <c r="AN157">
         <v>0</v>
       </c>
+      <c r="AO157">
+        <v>0</v>
+      </c>
     </row>
-    <row r="158" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>174</v>
       </c>
@@ -22406,8 +22610,11 @@
       <c r="AN158" s="2">
         <v>6</v>
       </c>
+      <c r="AO158">
+        <v>6</v>
+      </c>
     </row>
-    <row r="159" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>175</v>
       </c>
@@ -22525,8 +22732,11 @@
       <c r="AN159" s="2">
         <v>6</v>
       </c>
+      <c r="AO159">
+        <v>6</v>
+      </c>
     </row>
-    <row r="160" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>176</v>
       </c>
@@ -22644,8 +22854,11 @@
       <c r="AN160" s="2">
         <v>6</v>
       </c>
+      <c r="AO160">
+        <v>0</v>
+      </c>
     </row>
-    <row r="161" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>177</v>
       </c>
@@ -22763,8 +22976,11 @@
       <c r="AN161" s="2">
         <v>0</v>
       </c>
+      <c r="AO161">
+        <v>0</v>
+      </c>
     </row>
-    <row r="162" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>178</v>
       </c>
@@ -22780,6 +22996,9 @@
       <c r="E162" t="s">
         <v>107</v>
       </c>
+      <c r="F162" t="s">
+        <v>744</v>
+      </c>
       <c r="G162" t="s">
         <v>10</v>
       </c>
@@ -22882,8 +23101,11 @@
       <c r="AN162" s="2">
         <v>6</v>
       </c>
+      <c r="AO162">
+        <v>5</v>
+      </c>
     </row>
-    <row r="163" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>179</v>
       </c>
@@ -23001,8 +23223,11 @@
       <c r="AN163" s="2">
         <v>6</v>
       </c>
+      <c r="AO163">
+        <v>6</v>
+      </c>
     </row>
-    <row r="164" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>180</v>
       </c>
@@ -23123,8 +23348,11 @@
       <c r="AN164" s="2">
         <v>2</v>
       </c>
+      <c r="AO164">
+        <v>4</v>
+      </c>
     </row>
-    <row r="165" spans="1:40" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>181</v>
       </c>
@@ -23242,8 +23470,11 @@
       <c r="AN165" s="2">
         <v>6</v>
       </c>
+      <c r="AO165">
+        <v>6</v>
+      </c>
     </row>
-    <row r="166" spans="1:40" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:41" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>182</v>
       </c>
@@ -23361,8 +23592,11 @@
       <c r="AN166" s="2">
         <v>6</v>
       </c>
+      <c r="AO166">
+        <v>6</v>
+      </c>
     </row>
-    <row r="167" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>183</v>
       </c>
@@ -23480,8 +23714,11 @@
       <c r="AN167">
         <v>6</v>
       </c>
+      <c r="AO167">
+        <v>6</v>
+      </c>
     </row>
-    <row r="168" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>184</v>
       </c>
@@ -23599,8 +23836,11 @@
       <c r="AN168">
         <v>6</v>
       </c>
+      <c r="AO168">
+        <v>6</v>
+      </c>
     </row>
-    <row r="169" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>185</v>
       </c>
@@ -23718,8 +23958,11 @@
       <c r="AN169">
         <v>6</v>
       </c>
+      <c r="AO169">
+        <v>6</v>
+      </c>
     </row>
-    <row r="170" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>186</v>
       </c>
@@ -23837,8 +24080,11 @@
       <c r="AN170">
         <v>6</v>
       </c>
+      <c r="AO170">
+        <v>6</v>
+      </c>
     </row>
-    <row r="171" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>187</v>
       </c>
@@ -23956,8 +24202,11 @@
       <c r="AN171">
         <v>6</v>
       </c>
+      <c r="AO171">
+        <v>6</v>
+      </c>
     </row>
-    <row r="172" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>188</v>
       </c>
@@ -24075,8 +24324,11 @@
       <c r="AN172">
         <v>6</v>
       </c>
+      <c r="AO172">
+        <v>6</v>
+      </c>
     </row>
-    <row r="173" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>189</v>
       </c>
@@ -24194,8 +24446,11 @@
       <c r="AN173">
         <v>6</v>
       </c>
+      <c r="AO173">
+        <v>6</v>
+      </c>
     </row>
-    <row r="174" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>190</v>
       </c>
@@ -24313,8 +24568,11 @@
       <c r="AN174">
         <v>6</v>
       </c>
+      <c r="AO174">
+        <v>6</v>
+      </c>
     </row>
-    <row r="175" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>191</v>
       </c>
@@ -24432,8 +24690,11 @@
       <c r="AN175">
         <v>0</v>
       </c>
+      <c r="AO175">
+        <v>0</v>
+      </c>
     </row>
-    <row r="176" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>192</v>
       </c>
@@ -24551,8 +24812,11 @@
       <c r="AN176">
         <v>6</v>
       </c>
+      <c r="AO176">
+        <v>6</v>
+      </c>
     </row>
-    <row r="177" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>193</v>
       </c>
@@ -24670,8 +24934,11 @@
       <c r="AN177">
         <v>6</v>
       </c>
+      <c r="AO177">
+        <v>6</v>
+      </c>
     </row>
-    <row r="178" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>194</v>
       </c>
@@ -24789,8 +25056,11 @@
       <c r="AN178">
         <v>0</v>
       </c>
+      <c r="AO178">
+        <v>0</v>
+      </c>
     </row>
-    <row r="179" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>195</v>
       </c>
@@ -24908,8 +25178,11 @@
       <c r="AN179">
         <v>6</v>
       </c>
+      <c r="AO179">
+        <v>6</v>
+      </c>
     </row>
-    <row r="180" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>196</v>
       </c>
@@ -25027,8 +25300,11 @@
       <c r="AN180">
         <v>0</v>
       </c>
+      <c r="AO180">
+        <v>0</v>
+      </c>
     </row>
-    <row r="181" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>197</v>
       </c>
@@ -25146,8 +25422,11 @@
       <c r="AN181">
         <v>6</v>
       </c>
+      <c r="AO181">
+        <v>6</v>
+      </c>
     </row>
-    <row r="182" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>198</v>
       </c>
@@ -25264,7 +25543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>201</v>
       </c>
@@ -25381,7 +25660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>202</v>
       </c>
@@ -25498,7 +25777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>203</v>
       </c>
@@ -25615,7 +25894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>204</v>
       </c>
@@ -25735,7 +26014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>206</v>
       </c>
@@ -25852,7 +26131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>207</v>
       </c>
@@ -25969,7 +26248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>208</v>
       </c>
@@ -26086,7 +26365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>209</v>
       </c>
@@ -26206,7 +26485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>210</v>
       </c>
@@ -26323,7 +26602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>211</v>
       </c>
@@ -28327,7 +28606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>230</v>
       </c>
@@ -28444,7 +28723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>231</v>
       </c>
@@ -28561,7 +28840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>232</v>
       </c>
@@ -28681,7 +28960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>233</v>
       </c>
@@ -28797,8 +29076,11 @@
       <c r="AN212">
         <v>6</v>
       </c>
+      <c r="AO212">
+        <v>0</v>
+      </c>
     </row>
-    <row r="213" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>234</v>
       </c>
@@ -28914,8 +29196,11 @@
       <c r="AN213">
         <v>0</v>
       </c>
+      <c r="AO213">
+        <v>0</v>
+      </c>
     </row>
-    <row r="214" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>235</v>
       </c>
@@ -29031,8 +29316,11 @@
       <c r="AN214">
         <v>0</v>
       </c>
+      <c r="AO214">
+        <v>0</v>
+      </c>
     </row>
-    <row r="215" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>236</v>
       </c>
@@ -29148,8 +29436,11 @@
       <c r="AN215">
         <v>0</v>
       </c>
+      <c r="AO215">
+        <v>0</v>
+      </c>
     </row>
-    <row r="216" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>237</v>
       </c>
@@ -29268,8 +29559,11 @@
       <c r="AN216">
         <v>6</v>
       </c>
+      <c r="AO216">
+        <v>0</v>
+      </c>
     </row>
-    <row r="217" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>238</v>
       </c>
@@ -29385,8 +29679,11 @@
       <c r="AN217">
         <v>0</v>
       </c>
+      <c r="AO217">
+        <v>0</v>
+      </c>
     </row>
-    <row r="218" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>239</v>
       </c>
@@ -29502,8 +29799,11 @@
       <c r="AN218">
         <v>0</v>
       </c>
+      <c r="AO218">
+        <v>0</v>
+      </c>
     </row>
-    <row r="219" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>240</v>
       </c>
@@ -29619,8 +29919,11 @@
       <c r="AN219">
         <v>6</v>
       </c>
+      <c r="AO219">
+        <v>0</v>
+      </c>
     </row>
-    <row r="220" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>241</v>
       </c>
@@ -29736,8 +30039,11 @@
       <c r="AN220">
         <v>6</v>
       </c>
+      <c r="AO220">
+        <v>0</v>
+      </c>
     </row>
-    <row r="221" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>242</v>
       </c>
@@ -29853,8 +30159,11 @@
       <c r="AN221" t="s">
         <v>308</v>
       </c>
+      <c r="AO221" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="222" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>243</v>
       </c>
@@ -29970,8 +30279,11 @@
       <c r="AN222">
         <v>0</v>
       </c>
+      <c r="AO222">
+        <v>0</v>
+      </c>
     </row>
-    <row r="223" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>244</v>
       </c>
@@ -30090,8 +30402,11 @@
       <c r="AN223">
         <v>0</v>
       </c>
+      <c r="AO223">
+        <v>0</v>
+      </c>
     </row>
-    <row r="224" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>245</v>
       </c>
@@ -30207,8 +30522,11 @@
       <c r="AN224">
         <v>0</v>
       </c>
+      <c r="AO224">
+        <v>0</v>
+      </c>
     </row>
-    <row r="225" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>246</v>
       </c>
@@ -30327,8 +30645,11 @@
       <c r="AN225">
         <v>0</v>
       </c>
+      <c r="AO225">
+        <v>0</v>
+      </c>
     </row>
-    <row r="226" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>247</v>
       </c>
@@ -30444,8 +30765,11 @@
       <c r="AN226">
         <v>0</v>
       </c>
+      <c r="AO226">
+        <v>0</v>
+      </c>
     </row>
-    <row r="227" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>248</v>
       </c>
@@ -30562,7 +30886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>249</v>
       </c>
@@ -30679,7 +31003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>250</v>
       </c>
@@ -30796,7 +31120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>251</v>
       </c>
@@ -30913,7 +31237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>252</v>
       </c>
@@ -31030,7 +31354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>253</v>
       </c>
@@ -31147,7 +31471,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="233" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>254</v>
       </c>
@@ -31264,7 +31588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>255</v>
       </c>
@@ -31381,7 +31705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>256</v>
       </c>
@@ -31498,7 +31822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>257</v>
       </c>
@@ -31615,7 +31939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>258</v>
       </c>
@@ -31732,7 +32056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>259</v>
       </c>
@@ -31849,7 +32173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>260</v>
       </c>
@@ -31966,7 +32290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>261</v>
       </c>
@@ -32083,7 +32407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>262</v>
       </c>
@@ -32200,7 +32524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>263</v>
       </c>
@@ -32316,8 +32640,11 @@
       <c r="AN242">
         <v>6</v>
       </c>
+      <c r="AO242">
+        <v>0</v>
+      </c>
     </row>
-    <row r="243" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>264</v>
       </c>
@@ -32433,8 +32760,11 @@
       <c r="AN243">
         <v>6</v>
       </c>
+      <c r="AO243">
+        <v>0</v>
+      </c>
     </row>
-    <row r="244" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>265</v>
       </c>
@@ -32550,8 +32880,11 @@
       <c r="AN244">
         <v>0</v>
       </c>
+      <c r="AO244">
+        <v>0</v>
+      </c>
     </row>
-    <row r="245" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>266</v>
       </c>
@@ -32667,8 +33000,11 @@
       <c r="AN245">
         <v>0</v>
       </c>
+      <c r="AO245">
+        <v>0</v>
+      </c>
     </row>
-    <row r="246" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>267</v>
       </c>
@@ -32784,8 +33120,11 @@
       <c r="AN246">
         <v>0</v>
       </c>
+      <c r="AO246">
+        <v>0</v>
+      </c>
     </row>
-    <row r="247" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>268</v>
       </c>
@@ -32901,8 +33240,11 @@
       <c r="AN247">
         <v>0</v>
       </c>
+      <c r="AO247">
+        <v>0</v>
+      </c>
     </row>
-    <row r="248" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>269</v>
       </c>
@@ -33018,8 +33360,11 @@
       <c r="AN248">
         <v>0</v>
       </c>
+      <c r="AO248">
+        <v>0</v>
+      </c>
     </row>
-    <row r="249" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>270</v>
       </c>
@@ -33135,8 +33480,11 @@
       <c r="AN249">
         <v>0</v>
       </c>
+      <c r="AO249">
+        <v>0</v>
+      </c>
     </row>
-    <row r="250" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>271</v>
       </c>
@@ -33252,8 +33600,11 @@
       <c r="AN250">
         <v>6</v>
       </c>
+      <c r="AO250">
+        <v>0</v>
+      </c>
     </row>
-    <row r="251" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>272</v>
       </c>
@@ -33369,8 +33720,11 @@
       <c r="AN251">
         <v>0</v>
       </c>
+      <c r="AO251">
+        <v>0</v>
+      </c>
     </row>
-    <row r="252" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>273</v>
       </c>
@@ -33486,8 +33840,11 @@
       <c r="AN252">
         <v>0</v>
       </c>
+      <c r="AO252">
+        <v>0</v>
+      </c>
     </row>
-    <row r="253" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>274</v>
       </c>
@@ -33603,8 +33960,11 @@
       <c r="AN253">
         <v>0</v>
       </c>
+      <c r="AO253">
+        <v>0</v>
+      </c>
     </row>
-    <row r="254" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>275</v>
       </c>
@@ -33720,8 +34080,11 @@
       <c r="AN254">
         <v>0</v>
       </c>
+      <c r="AO254">
+        <v>0</v>
+      </c>
     </row>
-    <row r="255" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>276</v>
       </c>
@@ -33837,8 +34200,11 @@
       <c r="AN255">
         <v>0</v>
       </c>
+      <c r="AO255">
+        <v>0</v>
+      </c>
     </row>
-    <row r="256" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>277</v>
       </c>
@@ -33954,8 +34320,11 @@
       <c r="AN256">
         <v>0</v>
       </c>
+      <c r="AO256">
+        <v>0</v>
+      </c>
     </row>
-    <row r="257" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>278</v>
       </c>
@@ -34071,8 +34440,11 @@
       <c r="AN257">
         <v>0</v>
       </c>
+      <c r="AO257">
+        <v>0</v>
+      </c>
     </row>
-    <row r="258" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>279</v>
       </c>
@@ -34188,8 +34560,11 @@
       <c r="AN258">
         <v>0</v>
       </c>
+      <c r="AO258">
+        <v>0</v>
+      </c>
     </row>
-    <row r="259" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>280</v>
       </c>
@@ -34305,8 +34680,11 @@
       <c r="AN259">
         <v>0</v>
       </c>
+      <c r="AO259">
+        <v>0</v>
+      </c>
     </row>
-    <row r="260" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>281</v>
       </c>
@@ -34422,8 +34800,11 @@
       <c r="AN260">
         <v>0</v>
       </c>
+      <c r="AO260">
+        <v>0</v>
+      </c>
     </row>
-    <row r="261" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>282</v>
       </c>
@@ -34539,8 +34920,11 @@
       <c r="AN261">
         <v>0</v>
       </c>
+      <c r="AO261">
+        <v>0</v>
+      </c>
     </row>
-    <row r="262" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>283</v>
       </c>
@@ -34656,8 +35040,11 @@
       <c r="AN262">
         <v>0</v>
       </c>
+      <c r="AO262">
+        <v>0</v>
+      </c>
     </row>
-    <row r="263" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>284</v>
       </c>
@@ -34773,8 +35160,11 @@
       <c r="AN263">
         <v>0</v>
       </c>
+      <c r="AO263">
+        <v>0</v>
+      </c>
     </row>
-    <row r="264" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>285</v>
       </c>
@@ -34890,8 +35280,11 @@
       <c r="AN264">
         <v>0</v>
       </c>
+      <c r="AO264">
+        <v>0</v>
+      </c>
     </row>
-    <row r="265" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>286</v>
       </c>
@@ -35007,8 +35400,11 @@
       <c r="AN265">
         <v>0</v>
       </c>
+      <c r="AO265">
+        <v>0</v>
+      </c>
     </row>
-    <row r="266" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>287</v>
       </c>
@@ -35124,8 +35520,11 @@
       <c r="AN266">
         <v>6</v>
       </c>
+      <c r="AO266">
+        <v>0</v>
+      </c>
     </row>
-    <row r="267" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>288</v>
       </c>
@@ -35241,8 +35640,11 @@
       <c r="AN267">
         <v>0</v>
       </c>
+      <c r="AO267">
+        <v>0</v>
+      </c>
     </row>
-    <row r="268" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>289</v>
       </c>
@@ -35358,8 +35760,11 @@
       <c r="AN268">
         <v>0</v>
       </c>
+      <c r="AO268">
+        <v>0</v>
+      </c>
     </row>
-    <row r="269" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>290</v>
       </c>
@@ -35475,8 +35880,11 @@
       <c r="AN269">
         <v>0</v>
       </c>
+      <c r="AO269">
+        <v>0</v>
+      </c>
     </row>
-    <row r="270" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>291</v>
       </c>
@@ -35592,8 +36000,11 @@
       <c r="AN270">
         <v>0</v>
       </c>
+      <c r="AO270">
+        <v>0</v>
+      </c>
     </row>
-    <row r="271" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>292</v>
       </c>
@@ -35709,8 +36120,11 @@
       <c r="AN271">
         <v>0</v>
       </c>
+      <c r="AO271">
+        <v>0</v>
+      </c>
     </row>
-    <row r="272" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>293</v>
       </c>
@@ -37751,7 +38165,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="289" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>314</v>
       </c>
@@ -37870,7 +38284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>315</v>
       </c>
@@ -37989,7 +38403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>316</v>
       </c>
@@ -38108,7 +38522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>317</v>
       </c>
@@ -38227,7 +38641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>318</v>
       </c>
@@ -38346,7 +38760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>319</v>
       </c>
@@ -38468,7 +38882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>321</v>
       </c>
@@ -38587,7 +39001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>322</v>
       </c>
@@ -38706,7 +39120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>323</v>
       </c>
@@ -38828,7 +39242,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="298" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>324</v>
       </c>
@@ -38947,7 +39361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>325</v>
       </c>
@@ -39069,7 +39483,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="300" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>326</v>
       </c>
@@ -39188,7 +39602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>327</v>
       </c>
@@ -39307,7 +39721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="302" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>328</v>
       </c>
@@ -39425,8 +39839,11 @@
       <c r="AN302">
         <v>0</v>
       </c>
+      <c r="AO302">
+        <v>0</v>
+      </c>
     </row>
-    <row r="303" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>329</v>
       </c>
@@ -39544,8 +39961,11 @@
       <c r="AN303">
         <v>0</v>
       </c>
+      <c r="AO303">
+        <v>0</v>
+      </c>
     </row>
-    <row r="304" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>330</v>
       </c>
@@ -39663,8 +40083,11 @@
       <c r="AN304">
         <v>0</v>
       </c>
+      <c r="AO304">
+        <v>0</v>
+      </c>
     </row>
-    <row r="305" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>331</v>
       </c>
@@ -39782,8 +40205,11 @@
       <c r="AN305">
         <v>0</v>
       </c>
+      <c r="AO305">
+        <v>0</v>
+      </c>
     </row>
-    <row r="306" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>332</v>
       </c>
@@ -39901,8 +40327,11 @@
       <c r="AN306">
         <v>6</v>
       </c>
+      <c r="AO306">
+        <v>0</v>
+      </c>
     </row>
-    <row r="307" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>333</v>
       </c>
@@ -40020,8 +40449,11 @@
       <c r="AN307">
         <v>0</v>
       </c>
+      <c r="AO307">
+        <v>0</v>
+      </c>
     </row>
-    <row r="308" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>334</v>
       </c>
@@ -40139,8 +40571,11 @@
       <c r="AN308">
         <v>0</v>
       </c>
+      <c r="AO308">
+        <v>0</v>
+      </c>
     </row>
-    <row r="309" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>335</v>
       </c>
@@ -40258,8 +40693,11 @@
       <c r="AN309">
         <v>0</v>
       </c>
+      <c r="AO309">
+        <v>0</v>
+      </c>
     </row>
-    <row r="310" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>336</v>
       </c>
@@ -40377,8 +40815,11 @@
       <c r="AN310">
         <v>0</v>
       </c>
+      <c r="AO310">
+        <v>0</v>
+      </c>
     </row>
-    <row r="311" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>337</v>
       </c>
@@ -40496,8 +40937,11 @@
       <c r="AN311">
         <v>6</v>
       </c>
+      <c r="AO311">
+        <v>0</v>
+      </c>
     </row>
-    <row r="312" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>338</v>
       </c>
@@ -40615,8 +41059,11 @@
       <c r="AN312">
         <v>6</v>
       </c>
+      <c r="AO312">
+        <v>0</v>
+      </c>
     </row>
-    <row r="313" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>339</v>
       </c>
@@ -40734,8 +41181,11 @@
       <c r="AN313">
         <v>0</v>
       </c>
+      <c r="AO313">
+        <v>0</v>
+      </c>
     </row>
-    <row r="314" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>340</v>
       </c>
@@ -40853,8 +41303,11 @@
       <c r="AN314">
         <v>6</v>
       </c>
+      <c r="AO314">
+        <v>0</v>
+      </c>
     </row>
-    <row r="315" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>341</v>
       </c>
@@ -40972,8 +41425,11 @@
       <c r="AN315">
         <v>0</v>
       </c>
+      <c r="AO315">
+        <v>0</v>
+      </c>
     </row>
-    <row r="316" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>342</v>
       </c>
@@ -41094,8 +41550,11 @@
       <c r="AN316">
         <v>0</v>
       </c>
+      <c r="AO316">
+        <v>0</v>
+      </c>
     </row>
-    <row r="317" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>343</v>
       </c>
@@ -41217,7 +41676,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="318" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>344</v>
       </c>
@@ -41336,7 +41795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>345</v>
       </c>
@@ -41455,7 +41914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="320" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>346</v>
       </c>
@@ -41574,7 +42033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="321" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>347</v>
       </c>
@@ -41693,7 +42152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="322" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>348</v>
       </c>
@@ -41815,7 +42274,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="323" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>350</v>
       </c>
@@ -41934,7 +42393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>351</v>
       </c>
@@ -42056,7 +42515,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="325" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>353</v>
       </c>
@@ -42175,7 +42634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="326" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>354</v>
       </c>
@@ -42294,7 +42753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="327" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>355</v>
       </c>
@@ -42413,7 +42872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>356</v>
       </c>
@@ -42535,7 +42994,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="329" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>357</v>
       </c>
@@ -42654,7 +43113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="330" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>358</v>
       </c>
@@ -42776,7 +43235,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="331" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>359</v>
       </c>
@@ -42895,7 +43354,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="332" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>360</v>
       </c>
@@ -43013,8 +43472,11 @@
       <c r="AN332">
         <v>6</v>
       </c>
+      <c r="AO332">
+        <v>0</v>
+      </c>
     </row>
-    <row r="333" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>361</v>
       </c>
@@ -43132,8 +43594,11 @@
       <c r="AN333">
         <v>6</v>
       </c>
+      <c r="AO333">
+        <v>0</v>
+      </c>
     </row>
-    <row r="334" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>362</v>
       </c>
@@ -43254,8 +43719,11 @@
       <c r="AN334" t="s">
         <v>308</v>
       </c>
+      <c r="AO334" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="335" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>363</v>
       </c>
@@ -43376,8 +43844,11 @@
       <c r="AN335" t="s">
         <v>308</v>
       </c>
+      <c r="AO335" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="336" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>364</v>
       </c>
@@ -43495,8 +43966,11 @@
       <c r="AN336">
         <v>6</v>
       </c>
+      <c r="AO336">
+        <v>0</v>
+      </c>
     </row>
-    <row r="337" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>365</v>
       </c>
@@ -43617,8 +44091,11 @@
       <c r="AN337" t="s">
         <v>308</v>
       </c>
+      <c r="AO337" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="338" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>366</v>
       </c>
@@ -43736,8 +44213,11 @@
       <c r="AN338">
         <v>6</v>
       </c>
+      <c r="AO338">
+        <v>0</v>
+      </c>
     </row>
-    <row r="339" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>367</v>
       </c>
@@ -43855,8 +44335,11 @@
       <c r="AN339">
         <v>6</v>
       </c>
+      <c r="AO339">
+        <v>0</v>
+      </c>
     </row>
-    <row r="340" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>368</v>
       </c>
@@ -43974,8 +44457,11 @@
       <c r="AN340">
         <v>0</v>
       </c>
+      <c r="AO340">
+        <v>0</v>
+      </c>
     </row>
-    <row r="341" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>369</v>
       </c>
@@ -44093,8 +44579,11 @@
       <c r="AN341">
         <v>6</v>
       </c>
+      <c r="AO341">
+        <v>0</v>
+      </c>
     </row>
-    <row r="342" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>370</v>
       </c>
@@ -44215,8 +44704,11 @@
       <c r="AN342" t="s">
         <v>308</v>
       </c>
+      <c r="AO342" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="343" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>371</v>
       </c>
@@ -44337,8 +44829,11 @@
       <c r="AN343" t="s">
         <v>308</v>
       </c>
+      <c r="AO343" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="344" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>372</v>
       </c>
@@ -44459,8 +44954,11 @@
       <c r="AN344">
         <v>0</v>
       </c>
+      <c r="AO344">
+        <v>0</v>
+      </c>
     </row>
-    <row r="345" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>373</v>
       </c>
@@ -44578,8 +45076,11 @@
       <c r="AN345" t="s">
         <v>308</v>
       </c>
+      <c r="AO345" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="346" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>374</v>
       </c>
@@ -44697,8 +45198,11 @@
       <c r="AN346">
         <v>0</v>
       </c>
+      <c r="AO346">
+        <v>0</v>
+      </c>
     </row>
-    <row r="347" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>375</v>
       </c>
@@ -44816,8 +45320,11 @@
       <c r="AN347">
         <v>6</v>
       </c>
+      <c r="AO347">
+        <v>6</v>
+      </c>
     </row>
-    <row r="348" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>376</v>
       </c>
@@ -44938,8 +45445,11 @@
       <c r="AN348">
         <v>1</v>
       </c>
+      <c r="AO348">
+        <v>5</v>
+      </c>
     </row>
-    <row r="349" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>377</v>
       </c>
@@ -45057,8 +45567,11 @@
       <c r="AN349">
         <v>0</v>
       </c>
+      <c r="AO349">
+        <v>0</v>
+      </c>
     </row>
-    <row r="350" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>378</v>
       </c>
@@ -45176,8 +45689,11 @@
       <c r="AN350" t="s">
         <v>308</v>
       </c>
+      <c r="AO350" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="351" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>379</v>
       </c>
@@ -45295,8 +45811,11 @@
       <c r="AN351">
         <v>0</v>
       </c>
+      <c r="AO351">
+        <v>0</v>
+      </c>
     </row>
-    <row r="352" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>380</v>
       </c>
@@ -45417,8 +45936,11 @@
       <c r="AN352">
         <v>1</v>
       </c>
+      <c r="AO352">
+        <v>5</v>
+      </c>
     </row>
-    <row r="353" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>381</v>
       </c>
@@ -45536,8 +46058,11 @@
       <c r="AN353">
         <v>6</v>
       </c>
+      <c r="AO353">
+        <v>6</v>
+      </c>
     </row>
-    <row r="354" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>382</v>
       </c>
@@ -45655,8 +46180,11 @@
       <c r="AN354">
         <v>0</v>
       </c>
+      <c r="AO354">
+        <v>0</v>
+      </c>
     </row>
-    <row r="355" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>383</v>
       </c>
@@ -45777,8 +46305,11 @@
       <c r="AN355" t="s">
         <v>308</v>
       </c>
+      <c r="AO355" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="356" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>384</v>
       </c>
@@ -45896,8 +46427,11 @@
       <c r="AN356">
         <v>0</v>
       </c>
+      <c r="AO356">
+        <v>0</v>
+      </c>
     </row>
-    <row r="357" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>385</v>
       </c>
@@ -46015,8 +46549,11 @@
       <c r="AN357">
         <v>6</v>
       </c>
+      <c r="AO357">
+        <v>0</v>
+      </c>
     </row>
-    <row r="358" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>386</v>
       </c>
@@ -46134,8 +46671,11 @@
       <c r="AN358">
         <v>0</v>
       </c>
+      <c r="AO358">
+        <v>0</v>
+      </c>
     </row>
-    <row r="359" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>387</v>
       </c>
@@ -46256,8 +46796,11 @@
       <c r="AN359" t="s">
         <v>308</v>
       </c>
+      <c r="AO359" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="360" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>388</v>
       </c>
@@ -46375,8 +46918,11 @@
       <c r="AN360">
         <v>6</v>
       </c>
+      <c r="AO360">
+        <v>0</v>
+      </c>
     </row>
-    <row r="361" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>389</v>
       </c>
@@ -46497,8 +47043,11 @@
       <c r="AN361">
         <v>1</v>
       </c>
+      <c r="AO361">
+        <v>5</v>
+      </c>
     </row>
-    <row r="362" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>390</v>
       </c>
@@ -46617,7 +47166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>393</v>
       </c>
@@ -46736,7 +47285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>394</v>
       </c>
@@ -46855,7 +47404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>395</v>
       </c>
@@ -46974,7 +47523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>396</v>
       </c>
@@ -47093,7 +47642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>397</v>
       </c>
@@ -47212,7 +47761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>398</v>
       </c>
@@ -60719,7 +61268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="481" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>518</v>
       </c>
@@ -60838,7 +61387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="482" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
         <v>519</v>
       </c>
@@ -60956,8 +61505,11 @@
       <c r="AN482">
         <v>0</v>
       </c>
+      <c r="AO482">
+        <v>0</v>
+      </c>
     </row>
-    <row r="483" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
         <v>520</v>
       </c>
@@ -61075,8 +61627,11 @@
       <c r="AN483">
         <v>6</v>
       </c>
+      <c r="AO483">
+        <v>0</v>
+      </c>
     </row>
-    <row r="484" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>521</v>
       </c>
@@ -61194,8 +61749,11 @@
       <c r="AN484">
         <v>0</v>
       </c>
+      <c r="AO484">
+        <v>0</v>
+      </c>
     </row>
-    <row r="485" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
         <v>522</v>
       </c>
@@ -61313,8 +61871,11 @@
       <c r="AN485">
         <v>0</v>
       </c>
+      <c r="AO485">
+        <v>0</v>
+      </c>
     </row>
-    <row r="486" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>523</v>
       </c>
@@ -61432,8 +61993,11 @@
       <c r="AN486">
         <v>0</v>
       </c>
+      <c r="AO486">
+        <v>0</v>
+      </c>
     </row>
-    <row r="487" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
         <v>524</v>
       </c>
@@ -61551,8 +62115,11 @@
       <c r="AN487">
         <v>0</v>
       </c>
+      <c r="AO487">
+        <v>0</v>
+      </c>
     </row>
-    <row r="488" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
         <v>525</v>
       </c>
@@ -61673,8 +62240,11 @@
       <c r="AN488">
         <v>0</v>
       </c>
+      <c r="AO488">
+        <v>0</v>
+      </c>
     </row>
-    <row r="489" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
         <v>526</v>
       </c>
@@ -61792,8 +62362,11 @@
       <c r="AN489">
         <v>0</v>
       </c>
+      <c r="AO489">
+        <v>0</v>
+      </c>
     </row>
-    <row r="490" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
         <v>527</v>
       </c>
@@ -61911,8 +62484,11 @@
       <c r="AN490">
         <v>0</v>
       </c>
+      <c r="AO490">
+        <v>0</v>
+      </c>
     </row>
-    <row r="491" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
         <v>528</v>
       </c>
@@ -62030,8 +62606,11 @@
       <c r="AN491">
         <v>0</v>
       </c>
+      <c r="AO491">
+        <v>0</v>
+      </c>
     </row>
-    <row r="492" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
         <v>529</v>
       </c>
@@ -62149,8 +62728,11 @@
       <c r="AN492">
         <v>0</v>
       </c>
+      <c r="AO492">
+        <v>0</v>
+      </c>
     </row>
-    <row r="493" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
         <v>530</v>
       </c>
@@ -62268,8 +62850,11 @@
       <c r="AN493">
         <v>0</v>
       </c>
+      <c r="AO493">
+        <v>0</v>
+      </c>
     </row>
-    <row r="494" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
         <v>531</v>
       </c>
@@ -62387,8 +62972,11 @@
       <c r="AN494">
         <v>0</v>
       </c>
+      <c r="AO494">
+        <v>0</v>
+      </c>
     </row>
-    <row r="495" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
         <v>532</v>
       </c>
@@ -62509,8 +63097,11 @@
       <c r="AN495" t="s">
         <v>308</v>
       </c>
+      <c r="AO495" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="496" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
         <v>533</v>
       </c>
@@ -62628,8 +63219,11 @@
       <c r="AN496">
         <v>0</v>
       </c>
+      <c r="AO496">
+        <v>0</v>
+      </c>
     </row>
-    <row r="497" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
         <v>534</v>
       </c>
@@ -62748,7 +63342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="498" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
         <v>535</v>
       </c>
@@ -62867,7 +63461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="499" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
         <v>536</v>
       </c>
@@ -62986,7 +63580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="500" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
         <v>537</v>
       </c>
@@ -63105,7 +63699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="501" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
         <v>538</v>
       </c>
@@ -63224,7 +63818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="502" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
         <v>539</v>
       </c>
@@ -63343,7 +63937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="503" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
         <v>540</v>
       </c>
@@ -63462,7 +64056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="504" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
         <v>541</v>
       </c>
@@ -63581,7 +64175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="505" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
         <v>542</v>
       </c>
@@ -63700,7 +64294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="506" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
         <v>543</v>
       </c>
@@ -63819,7 +64413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="507" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
         <v>544</v>
       </c>
@@ -63938,7 +64532,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="508" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A508" t="s">
         <v>545</v>
       </c>
@@ -64057,7 +64651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="509" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
         <v>546</v>
       </c>
@@ -64176,7 +64770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="510" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A510" t="s">
         <v>547</v>
       </c>
@@ -64295,7 +64889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="511" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
         <v>548</v>
       </c>
@@ -64414,7 +65008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="512" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A512" t="s">
         <v>549</v>
       </c>
@@ -64535,8 +65129,11 @@
       <c r="AN512">
         <v>0</v>
       </c>
+      <c r="AO512">
+        <v>0</v>
+      </c>
     </row>
-    <row r="513" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
         <v>550</v>
       </c>
@@ -64654,8 +65251,11 @@
       <c r="AN513">
         <v>6</v>
       </c>
+      <c r="AO513">
+        <v>0</v>
+      </c>
     </row>
-    <row r="514" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
         <v>551</v>
       </c>
@@ -64773,8 +65373,11 @@
       <c r="AN514">
         <v>6</v>
       </c>
+      <c r="AO514">
+        <v>0</v>
+      </c>
     </row>
-    <row r="515" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
         <v>552</v>
       </c>
@@ -64892,8 +65495,11 @@
       <c r="AN515">
         <v>0</v>
       </c>
+      <c r="AO515">
+        <v>0</v>
+      </c>
     </row>
-    <row r="516" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A516" t="s">
         <v>553</v>
       </c>
@@ -65011,8 +65617,11 @@
       <c r="AN516">
         <v>6</v>
       </c>
+      <c r="AO516">
+        <v>6</v>
+      </c>
     </row>
-    <row r="517" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
         <v>554</v>
       </c>
@@ -65133,8 +65742,11 @@
       <c r="AN517" t="s">
         <v>308</v>
       </c>
+      <c r="AO517" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="518" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A518" t="s">
         <v>555</v>
       </c>
@@ -65255,8 +65867,11 @@
       <c r="AN518" t="s">
         <v>308</v>
       </c>
+      <c r="AO518" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="519" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A519" t="s">
         <v>557</v>
       </c>
@@ -65374,8 +65989,11 @@
       <c r="AN519">
         <v>0</v>
       </c>
+      <c r="AO519">
+        <v>0</v>
+      </c>
     </row>
-    <row r="520" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A520" t="s">
         <v>558</v>
       </c>
@@ -65493,8 +66111,11 @@
       <c r="AN520">
         <v>6</v>
       </c>
+      <c r="AO520">
+        <v>0</v>
+      </c>
     </row>
-    <row r="521" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A521" t="s">
         <v>559</v>
       </c>
@@ -65612,8 +66233,11 @@
       <c r="AN521">
         <v>6</v>
       </c>
+      <c r="AO521">
+        <v>6</v>
+      </c>
     </row>
-    <row r="522" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
         <v>560</v>
       </c>
@@ -65731,8 +66355,11 @@
       <c r="AN522">
         <v>6</v>
       </c>
+      <c r="AO522">
+        <v>6</v>
+      </c>
     </row>
-    <row r="523" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
         <v>561</v>
       </c>
@@ -65850,8 +66477,11 @@
       <c r="AN523">
         <v>0</v>
       </c>
+      <c r="AO523">
+        <v>0</v>
+      </c>
     </row>
-    <row r="524" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
         <v>562</v>
       </c>
@@ -65969,8 +66599,11 @@
       <c r="AN524">
         <v>0</v>
       </c>
+      <c r="AO524">
+        <v>0</v>
+      </c>
     </row>
-    <row r="525" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
         <v>563</v>
       </c>
@@ -66088,8 +66721,11 @@
       <c r="AN525">
         <v>0</v>
       </c>
+      <c r="AO525">
+        <v>0</v>
+      </c>
     </row>
-    <row r="526" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="526" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A526" t="s">
         <v>564</v>
       </c>
@@ -66207,8 +66843,11 @@
       <c r="AN526">
         <v>0</v>
       </c>
+      <c r="AO526">
+        <v>0</v>
+      </c>
     </row>
-    <row r="527" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="527" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
         <v>565</v>
       </c>
@@ -66326,8 +66965,11 @@
       <c r="AN527">
         <v>0</v>
       </c>
+      <c r="AO527">
+        <v>0</v>
+      </c>
     </row>
-    <row r="528" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="528" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A528" t="s">
         <v>566</v>
       </c>
@@ -66448,8 +67090,11 @@
       <c r="AN528">
         <v>0</v>
       </c>
+      <c r="AO528">
+        <v>0</v>
+      </c>
     </row>
-    <row r="529" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>567</v>
       </c>
@@ -66567,8 +67212,11 @@
       <c r="AN529">
         <v>0</v>
       </c>
+      <c r="AO529">
+        <v>0</v>
+      </c>
     </row>
-    <row r="530" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A530" t="s">
         <v>568</v>
       </c>
@@ -66686,8 +67334,11 @@
       <c r="AN530">
         <v>0</v>
       </c>
+      <c r="AO530">
+        <v>0</v>
+      </c>
     </row>
-    <row r="531" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
         <v>569</v>
       </c>
@@ -66808,8 +67459,11 @@
       <c r="AN531">
         <v>6</v>
       </c>
+      <c r="AO531">
+        <v>0</v>
+      </c>
     </row>
-    <row r="532" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
         <v>570</v>
       </c>
@@ -66930,8 +67584,11 @@
       <c r="AN532">
         <v>0</v>
       </c>
+      <c r="AO532">
+        <v>0</v>
+      </c>
     </row>
-    <row r="533" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
         <v>571</v>
       </c>
@@ -67049,8 +67706,11 @@
       <c r="AN533">
         <v>0</v>
       </c>
+      <c r="AO533">
+        <v>0</v>
+      </c>
     </row>
-    <row r="534" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A534" t="s">
         <v>572</v>
       </c>
@@ -67168,8 +67828,11 @@
       <c r="AN534">
         <v>6</v>
       </c>
+      <c r="AO534">
+        <v>0</v>
+      </c>
     </row>
-    <row r="535" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
         <v>573</v>
       </c>
@@ -67287,8 +67950,11 @@
       <c r="AN535">
         <v>6</v>
       </c>
+      <c r="AO535">
+        <v>0</v>
+      </c>
     </row>
-    <row r="536" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>574</v>
       </c>
@@ -67406,8 +68072,11 @@
       <c r="AN536">
         <v>0</v>
       </c>
+      <c r="AO536">
+        <v>0</v>
+      </c>
     </row>
-    <row r="537" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
         <v>575</v>
       </c>
@@ -67525,8 +68194,11 @@
       <c r="AN537">
         <v>0</v>
       </c>
+      <c r="AO537">
+        <v>0</v>
+      </c>
     </row>
-    <row r="538" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
         <v>576</v>
       </c>
@@ -67644,8 +68316,11 @@
       <c r="AN538">
         <v>6</v>
       </c>
+      <c r="AO538">
+        <v>0</v>
+      </c>
     </row>
-    <row r="539" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
         <v>577</v>
       </c>
@@ -67763,8 +68438,11 @@
       <c r="AN539">
         <v>0</v>
       </c>
+      <c r="AO539">
+        <v>0</v>
+      </c>
     </row>
-    <row r="540" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>578</v>
       </c>
@@ -67882,8 +68560,11 @@
       <c r="AN540">
         <v>0</v>
       </c>
+      <c r="AO540">
+        <v>0</v>
+      </c>
     </row>
-    <row r="541" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
         <v>579</v>
       </c>
@@ -68001,8 +68682,11 @@
       <c r="AN541">
         <v>6</v>
       </c>
+      <c r="AO541">
+        <v>0</v>
+      </c>
     </row>
-    <row r="542" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>580</v>
       </c>
@@ -68124,7 +68808,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="543" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
         <v>583</v>
       </c>
@@ -68243,7 +68927,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="544" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>584</v>
       </c>

</xml_diff>

<commit_message>
addded missing data from yesterday from voice recording because it was raining
</commit_message>
<xml_diff>
--- a/data/monitoring_phenology/2024_budburst_to_budset.xlsx
+++ b/data/monitoring_phenology/2024_budburst_to_budset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/data/monitoring_phenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EFDC39-0789-464E-A620-436D84294FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED53541-5B4D-0346-80D6-94A16A039E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5385" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5404" uniqueCount="745">
   <si>
     <t>tree_ID</t>
   </si>
@@ -3181,15 +3181,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C09BEA22-6943-C148-893B-096C13910EF5}" name="Table1" displayName="Table1" ref="A1:AD631" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:AD631" xr:uid="{C09BEA22-6943-C148-893B-096C13910EF5}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="CoolS/WarmF"/>
-        <filter val="WarmS/WarmF"/>
-        <filter val="WarmS/WarmF_nitro"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AD631" xr:uid="{C09BEA22-6943-C148-893B-096C13910EF5}"/>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{6B7D526F-2D16-104C-916C-5A8D81E298F2}" name="tree_ID" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{E0C9A5F2-2115-B942-922F-AAB1B58E7971}" name="bloc" dataDxfId="28"/>
@@ -3545,9 +3537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A524" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP527" sqref="AP527:AP541"/>
+    <sheetView tabSelected="1" topLeftCell="A538" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AO547" sqref="AO547"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3687,7 +3679,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3811,8 +3803,11 @@
       <c r="AO2">
         <v>5</v>
       </c>
+      <c r="AP2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3933,8 +3928,11 @@
       <c r="AO3">
         <v>6</v>
       </c>
+      <c r="AP3">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4055,8 +4053,11 @@
       <c r="AO4">
         <v>6</v>
       </c>
+      <c r="AP4">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -4177,8 +4178,11 @@
       <c r="AO5">
         <v>6</v>
       </c>
+      <c r="AP5">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -4299,8 +4303,11 @@
       <c r="AO6">
         <v>6</v>
       </c>
+      <c r="AP6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="7" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -4421,8 +4428,11 @@
       <c r="AO7">
         <v>6</v>
       </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -4543,8 +4553,11 @@
       <c r="AO8">
         <v>6</v>
       </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -4665,8 +4678,11 @@
       <c r="AO9">
         <v>6</v>
       </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -4787,8 +4803,11 @@
       <c r="AO10">
         <v>6</v>
       </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -4912,8 +4931,11 @@
       <c r="AO11">
         <v>6</v>
       </c>
+      <c r="AP11">
+        <v>6</v>
+      </c>
     </row>
-    <row r="12" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -5034,8 +5056,11 @@
       <c r="AO12">
         <v>6</v>
       </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -5156,8 +5181,11 @@
       <c r="AO13">
         <v>6</v>
       </c>
+      <c r="AP13">
+        <v>6</v>
+      </c>
     </row>
-    <row r="14" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -5278,8 +5306,11 @@
       <c r="AO14">
         <v>6</v>
       </c>
+      <c r="AP14">
+        <v>6</v>
+      </c>
     </row>
-    <row r="15" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -5400,8 +5431,11 @@
       <c r="AO15">
         <v>6</v>
       </c>
+      <c r="AP15">
+        <v>6</v>
+      </c>
     </row>
-    <row r="16" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -5522,8 +5556,11 @@
       <c r="AO16">
         <v>6</v>
       </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -5644,8 +5681,11 @@
       <c r="AO17">
         <v>6</v>
       </c>
+      <c r="AP17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -5766,8 +5806,11 @@
       <c r="AO18">
         <v>6</v>
       </c>
+      <c r="AP18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -5888,8 +5931,11 @@
       <c r="AO19">
         <v>6</v>
       </c>
+      <c r="AP19">
+        <v>6</v>
+      </c>
     </row>
-    <row r="20" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -6010,8 +6056,11 @@
       <c r="AO20">
         <v>6</v>
       </c>
+      <c r="AP20">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -6132,8 +6181,11 @@
       <c r="AO21">
         <v>6</v>
       </c>
+      <c r="AP21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -6257,8 +6309,11 @@
       <c r="AO22">
         <v>6</v>
       </c>
+      <c r="AP22">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -6379,8 +6434,11 @@
       <c r="AO23">
         <v>6</v>
       </c>
+      <c r="AP23">
+        <v>6</v>
+      </c>
     </row>
-    <row r="24" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -6501,8 +6559,11 @@
       <c r="AO24">
         <v>6</v>
       </c>
+      <c r="AP24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -6623,8 +6684,11 @@
       <c r="AO25">
         <v>6</v>
       </c>
+      <c r="AP25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -6745,8 +6809,11 @@
       <c r="AO26">
         <v>6</v>
       </c>
+      <c r="AP26">
+        <v>6</v>
+      </c>
     </row>
-    <row r="27" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -6867,8 +6934,11 @@
       <c r="AO27">
         <v>5</v>
       </c>
+      <c r="AP27">
+        <v>6</v>
+      </c>
     </row>
-    <row r="28" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -6992,8 +7062,11 @@
       <c r="AO28">
         <v>0</v>
       </c>
+      <c r="AP28">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -7117,8 +7190,11 @@
       <c r="AO29" t="s">
         <v>308</v>
       </c>
+      <c r="AP29" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="30" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -7239,8 +7315,11 @@
       <c r="AO30">
         <v>6</v>
       </c>
+      <c r="AP30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -7360,6 +7439,9 @@
       </c>
       <c r="AO31">
         <v>6</v>
+      </c>
+      <c r="AP31">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:42" x14ac:dyDescent="0.2">
@@ -9240,7 +9322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -9361,8 +9443,11 @@
       <c r="AO47">
         <v>6</v>
       </c>
+      <c r="AP47">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -9483,8 +9568,11 @@
       <c r="AO48">
         <v>6</v>
       </c>
+      <c r="AP48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -9605,8 +9693,11 @@
       <c r="AO49">
         <v>5</v>
       </c>
+      <c r="AP49">
+        <v>6</v>
+      </c>
     </row>
-    <row r="50" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -9727,8 +9818,11 @@
       <c r="AO50">
         <v>6</v>
       </c>
+      <c r="AP50">
+        <v>6</v>
+      </c>
     </row>
-    <row r="51" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -9849,8 +9943,11 @@
       <c r="AO51">
         <v>6</v>
       </c>
+      <c r="AP51">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -9971,8 +10068,11 @@
       <c r="AO52">
         <v>0</v>
       </c>
+      <c r="AP52">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -10093,8 +10193,11 @@
       <c r="AO53">
         <v>6</v>
       </c>
+      <c r="AP53">
+        <v>6</v>
+      </c>
     </row>
-    <row r="54" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -10215,8 +10318,11 @@
       <c r="AO54">
         <v>0</v>
       </c>
+      <c r="AP54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -10340,8 +10446,11 @@
       <c r="AO55">
         <v>6</v>
       </c>
+      <c r="AP55">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -10465,8 +10574,11 @@
       <c r="AO56">
         <v>0</v>
       </c>
+      <c r="AP56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -10590,8 +10702,11 @@
       <c r="AO57">
         <v>6</v>
       </c>
+      <c r="AP57">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -10712,8 +10827,11 @@
       <c r="AO58">
         <v>6</v>
       </c>
+      <c r="AP58">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -10834,8 +10952,11 @@
       <c r="AO59" t="s">
         <v>308</v>
       </c>
+      <c r="AP59" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="60" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -10956,8 +11077,11 @@
       <c r="AO60">
         <v>0</v>
       </c>
+      <c r="AP60">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -11076,6 +11200,9 @@
         <v>6</v>
       </c>
       <c r="AO61">
+        <v>0</v>
+      </c>
+      <c r="AP61">
         <v>0</v>
       </c>
     </row>
@@ -14832,7 +14959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>105</v>
       </c>
@@ -14953,8 +15080,11 @@
       <c r="AO92" s="2">
         <v>6</v>
       </c>
+      <c r="AP92" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="93" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -15075,8 +15205,11 @@
       <c r="AO93" s="2">
         <v>6</v>
       </c>
+      <c r="AP93" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="94" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -15197,8 +15330,11 @@
       <c r="AO94" s="2">
         <v>0</v>
       </c>
+      <c r="AP94" s="2">
+        <v>9</v>
+      </c>
     </row>
-    <row r="95" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -15322,8 +15458,11 @@
       <c r="AO95" s="2">
         <v>6</v>
       </c>
+      <c r="AP95" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="96" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>112</v>
       </c>
@@ -15444,8 +15583,11 @@
       <c r="AO96" s="2">
         <v>6</v>
       </c>
+      <c r="AP96" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="97" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>113</v>
       </c>
@@ -15566,8 +15708,11 @@
       <c r="AO97" s="2">
         <v>6</v>
       </c>
+      <c r="AP97" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="98" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>114</v>
       </c>
@@ -15688,8 +15833,11 @@
       <c r="AO98" s="2">
         <v>6</v>
       </c>
+      <c r="AP98" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="99" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>115</v>
       </c>
@@ -15810,8 +15958,11 @@
       <c r="AO99" s="2">
         <v>6</v>
       </c>
+      <c r="AP99" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="100" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>116</v>
       </c>
@@ -15932,8 +16083,11 @@
       <c r="AO100" s="2">
         <v>0</v>
       </c>
+      <c r="AP100" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="101" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>117</v>
       </c>
@@ -16054,8 +16208,11 @@
       <c r="AO101" s="2">
         <v>6</v>
       </c>
+      <c r="AP101" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="102" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>118</v>
       </c>
@@ -16176,8 +16333,11 @@
       <c r="AO102" s="2">
         <v>6</v>
       </c>
+      <c r="AP102" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="103" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>119</v>
       </c>
@@ -16298,8 +16458,11 @@
       <c r="AO103" s="2">
         <v>6</v>
       </c>
+      <c r="AP103" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="104" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>120</v>
       </c>
@@ -16420,8 +16583,11 @@
       <c r="AO104" s="2">
         <v>6</v>
       </c>
+      <c r="AP104" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="105" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>121</v>
       </c>
@@ -16542,8 +16708,11 @@
       <c r="AO105" s="2">
         <v>6</v>
       </c>
+      <c r="AP105" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="106" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>122</v>
       </c>
@@ -16664,8 +16833,11 @@
       <c r="AO106" s="2">
         <v>6</v>
       </c>
+      <c r="AP106" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="107" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -16786,8 +16958,11 @@
       <c r="AO107" s="2">
         <v>6</v>
       </c>
+      <c r="AP107" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="108" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>124</v>
       </c>
@@ -16908,8 +17083,11 @@
       <c r="AO108" s="2">
         <v>6</v>
       </c>
+      <c r="AP108" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="109" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>125</v>
       </c>
@@ -17033,8 +17211,11 @@
       <c r="AO109" s="2">
         <v>6</v>
       </c>
+      <c r="AP109" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="110" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -17155,8 +17336,11 @@
       <c r="AO110" s="2">
         <v>6</v>
       </c>
+      <c r="AP110" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="111" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>127</v>
       </c>
@@ -17280,8 +17464,11 @@
       <c r="AO111" s="2">
         <v>5</v>
       </c>
+      <c r="AP111" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="112" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>128</v>
       </c>
@@ -17402,8 +17589,11 @@
       <c r="AO112" s="2">
         <v>0</v>
       </c>
+      <c r="AP112" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="113" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -17524,8 +17714,11 @@
       <c r="AO113" t="s">
         <v>308</v>
       </c>
+      <c r="AP113" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="114" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -17646,8 +17839,11 @@
       <c r="AO114" s="2">
         <v>6</v>
       </c>
+      <c r="AP114" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="115" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>131</v>
       </c>
@@ -17768,8 +17964,11 @@
       <c r="AO115" s="2">
         <v>6</v>
       </c>
+      <c r="AP115" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="116" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>132</v>
       </c>
@@ -17890,8 +18089,11 @@
       <c r="AO116" s="2">
         <v>0</v>
       </c>
+      <c r="AP116" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="117" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>133</v>
       </c>
@@ -18012,8 +18214,11 @@
       <c r="AO117" s="2">
         <v>6</v>
       </c>
+      <c r="AP117" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="118" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>134</v>
       </c>
@@ -18134,8 +18339,11 @@
       <c r="AO118" s="2">
         <v>6</v>
       </c>
+      <c r="AP118" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="119" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -18256,8 +18464,11 @@
       <c r="AO119" s="2">
         <v>0</v>
       </c>
+      <c r="AP119" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="120" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>136</v>
       </c>
@@ -18378,8 +18589,11 @@
       <c r="AO120" s="2">
         <v>6</v>
       </c>
+      <c r="AP120" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="121" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>137</v>
       </c>
@@ -18501,6 +18715,9 @@
         <v>6</v>
       </c>
       <c r="AO121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AP121" s="2">
         <v>6</v>
       </c>
     </row>
@@ -20382,7 +20599,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>153</v>
       </c>
@@ -20506,8 +20723,11 @@
       <c r="AO137">
         <v>5</v>
       </c>
+      <c r="AP137">
+        <v>6</v>
+      </c>
     </row>
-    <row r="138" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>154</v>
       </c>
@@ -20628,8 +20848,11 @@
       <c r="AO138">
         <v>6</v>
       </c>
+      <c r="AP138">
+        <v>6</v>
+      </c>
     </row>
-    <row r="139" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>155</v>
       </c>
@@ -20750,8 +20973,11 @@
       <c r="AO139">
         <v>6</v>
       </c>
+      <c r="AP139">
+        <v>6</v>
+      </c>
     </row>
-    <row r="140" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>156</v>
       </c>
@@ -20872,8 +21098,11 @@
       <c r="AO140">
         <v>0</v>
       </c>
+      <c r="AP140">
+        <v>0</v>
+      </c>
     </row>
-    <row r="141" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>157</v>
       </c>
@@ -20994,8 +21223,11 @@
       <c r="AO141">
         <v>0</v>
       </c>
+      <c r="AP141">
+        <v>0</v>
+      </c>
     </row>
-    <row r="142" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>158</v>
       </c>
@@ -21116,8 +21348,11 @@
       <c r="AO142">
         <v>0</v>
       </c>
+      <c r="AP142">
+        <v>0</v>
+      </c>
     </row>
-    <row r="143" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>159</v>
       </c>
@@ -21238,8 +21473,11 @@
       <c r="AO143">
         <v>0</v>
       </c>
+      <c r="AP143">
+        <v>0</v>
+      </c>
     </row>
-    <row r="144" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>160</v>
       </c>
@@ -21360,8 +21598,11 @@
       <c r="AO144">
         <v>0</v>
       </c>
+      <c r="AP144">
+        <v>0</v>
+      </c>
     </row>
-    <row r="145" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>161</v>
       </c>
@@ -21482,8 +21723,11 @@
       <c r="AO145">
         <v>0</v>
       </c>
+      <c r="AP145">
+        <v>0</v>
+      </c>
     </row>
-    <row r="146" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>162</v>
       </c>
@@ -21604,8 +21848,11 @@
       <c r="AO146">
         <v>6</v>
       </c>
+      <c r="AP146">
+        <v>6</v>
+      </c>
     </row>
-    <row r="147" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>163</v>
       </c>
@@ -21726,8 +21973,11 @@
       <c r="AO147">
         <v>0</v>
       </c>
+      <c r="AP147">
+        <v>0</v>
+      </c>
     </row>
-    <row r="148" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>164</v>
       </c>
@@ -21851,8 +22101,11 @@
       <c r="AO148">
         <v>5</v>
       </c>
+      <c r="AP148">
+        <v>6</v>
+      </c>
     </row>
-    <row r="149" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>165</v>
       </c>
@@ -21973,8 +22226,11 @@
       <c r="AO149">
         <v>0</v>
       </c>
+      <c r="AP149">
+        <v>0</v>
+      </c>
     </row>
-    <row r="150" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>166</v>
       </c>
@@ -22098,8 +22354,11 @@
       <c r="AO150">
         <v>5</v>
       </c>
+      <c r="AP150">
+        <v>6</v>
+      </c>
     </row>
-    <row r="151" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>167</v>
       </c>
@@ -22218,6 +22477,9 @@
         <v>0</v>
       </c>
       <c r="AO151">
+        <v>0</v>
+      </c>
+      <c r="AP151">
         <v>0</v>
       </c>
     </row>
@@ -25977,7 +26239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>198</v>
       </c>
@@ -26096,8 +26358,11 @@
       <c r="AO182">
         <v>0</v>
       </c>
+      <c r="AP182">
+        <v>0</v>
+      </c>
     </row>
-    <row r="183" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>201</v>
       </c>
@@ -26216,8 +26481,11 @@
       <c r="AO183">
         <v>0</v>
       </c>
+      <c r="AP183">
+        <v>0</v>
+      </c>
     </row>
-    <row r="184" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>202</v>
       </c>
@@ -26336,8 +26604,11 @@
       <c r="AO184">
         <v>0</v>
       </c>
+      <c r="AP184">
+        <v>0</v>
+      </c>
     </row>
-    <row r="185" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>203</v>
       </c>
@@ -26456,8 +26727,11 @@
       <c r="AO185">
         <v>0</v>
       </c>
+      <c r="AP185">
+        <v>0</v>
+      </c>
     </row>
-    <row r="186" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>204</v>
       </c>
@@ -26579,8 +26853,11 @@
       <c r="AO186">
         <v>0</v>
       </c>
+      <c r="AP186">
+        <v>0</v>
+      </c>
     </row>
-    <row r="187" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>206</v>
       </c>
@@ -26699,8 +26976,11 @@
       <c r="AO187">
         <v>0</v>
       </c>
+      <c r="AP187">
+        <v>0</v>
+      </c>
     </row>
-    <row r="188" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>207</v>
       </c>
@@ -26819,8 +27099,11 @@
       <c r="AO188">
         <v>0</v>
       </c>
+      <c r="AP188">
+        <v>0</v>
+      </c>
     </row>
-    <row r="189" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>208</v>
       </c>
@@ -26939,8 +27222,11 @@
       <c r="AO189">
         <v>0</v>
       </c>
+      <c r="AP189">
+        <v>0</v>
+      </c>
     </row>
-    <row r="190" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>209</v>
       </c>
@@ -27062,8 +27348,11 @@
       <c r="AO190">
         <v>0</v>
       </c>
+      <c r="AP190">
+        <v>0</v>
+      </c>
     </row>
-    <row r="191" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>210</v>
       </c>
@@ -27182,8 +27471,11 @@
       <c r="AO191">
         <v>0</v>
       </c>
+      <c r="AP191">
+        <v>0</v>
+      </c>
     </row>
-    <row r="192" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>211</v>
       </c>
@@ -27302,8 +27594,11 @@
       <c r="AO192">
         <v>0</v>
       </c>
+      <c r="AP192">
+        <v>0</v>
+      </c>
     </row>
-    <row r="193" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>212</v>
       </c>
@@ -27422,8 +27717,11 @@
       <c r="AO193">
         <v>0</v>
       </c>
+      <c r="AP193">
+        <v>0</v>
+      </c>
     </row>
-    <row r="194" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>213</v>
       </c>
@@ -27545,8 +27843,11 @@
       <c r="AO194">
         <v>0</v>
       </c>
+      <c r="AP194">
+        <v>0</v>
+      </c>
     </row>
-    <row r="195" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>215</v>
       </c>
@@ -27665,8 +27966,11 @@
       <c r="AO195">
         <v>0</v>
       </c>
+      <c r="AP195">
+        <v>0</v>
+      </c>
     </row>
-    <row r="196" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>216</v>
       </c>
@@ -27785,8 +28089,11 @@
       <c r="AO196">
         <v>0</v>
       </c>
+      <c r="AP196">
+        <v>0</v>
+      </c>
     </row>
-    <row r="197" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>217</v>
       </c>
@@ -27905,8 +28212,11 @@
       <c r="AO197">
         <v>0</v>
       </c>
+      <c r="AP197">
+        <v>0</v>
+      </c>
     </row>
-    <row r="198" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>218</v>
       </c>
@@ -28028,8 +28338,11 @@
       <c r="AO198">
         <v>0</v>
       </c>
+      <c r="AP198">
+        <v>0</v>
+      </c>
     </row>
-    <row r="199" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>220</v>
       </c>
@@ -28148,8 +28461,11 @@
       <c r="AO199">
         <v>0</v>
       </c>
+      <c r="AP199">
+        <v>0</v>
+      </c>
     </row>
-    <row r="200" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>221</v>
       </c>
@@ -28271,8 +28587,11 @@
       <c r="AO200">
         <v>0</v>
       </c>
+      <c r="AP200">
+        <v>0</v>
+      </c>
     </row>
-    <row r="201" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>222</v>
       </c>
@@ -28391,8 +28710,11 @@
       <c r="AO201">
         <v>0</v>
       </c>
+      <c r="AP201">
+        <v>0</v>
+      </c>
     </row>
-    <row r="202" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>223</v>
       </c>
@@ -28511,8 +28833,11 @@
       <c r="AO202">
         <v>0</v>
       </c>
+      <c r="AP202">
+        <v>0</v>
+      </c>
     </row>
-    <row r="203" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>224</v>
       </c>
@@ -28631,8 +28956,11 @@
       <c r="AO203">
         <v>0</v>
       </c>
+      <c r="AP203">
+        <v>0</v>
+      </c>
     </row>
-    <row r="204" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>225</v>
       </c>
@@ -28751,8 +29079,11 @@
       <c r="AO204">
         <v>0</v>
       </c>
+      <c r="AP204">
+        <v>0</v>
+      </c>
     </row>
-    <row r="205" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>226</v>
       </c>
@@ -28874,8 +29205,11 @@
       <c r="AO205">
         <v>0</v>
       </c>
+      <c r="AP205">
+        <v>0</v>
+      </c>
     </row>
-    <row r="206" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>227</v>
       </c>
@@ -28994,8 +29328,11 @@
       <c r="AO206">
         <v>0</v>
       </c>
+      <c r="AP206">
+        <v>0</v>
+      </c>
     </row>
-    <row r="207" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>228</v>
       </c>
@@ -29114,8 +29451,11 @@
       <c r="AO207">
         <v>0</v>
       </c>
+      <c r="AP207">
+        <v>0</v>
+      </c>
     </row>
-    <row r="208" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>229</v>
       </c>
@@ -29237,8 +29577,11 @@
       <c r="AO208">
         <v>0</v>
       </c>
+      <c r="AP208">
+        <v>0</v>
+      </c>
     </row>
-    <row r="209" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>230</v>
       </c>
@@ -29357,8 +29700,11 @@
       <c r="AO209">
         <v>0</v>
       </c>
+      <c r="AP209">
+        <v>0</v>
+      </c>
     </row>
-    <row r="210" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>231</v>
       </c>
@@ -29477,8 +29823,11 @@
       <c r="AO210">
         <v>0</v>
       </c>
+      <c r="AP210">
+        <v>0</v>
+      </c>
     </row>
-    <row r="211" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>232</v>
       </c>
@@ -29600,8 +29949,11 @@
       <c r="AO211">
         <v>0</v>
       </c>
+      <c r="AP211">
+        <v>0</v>
+      </c>
     </row>
-    <row r="212" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>233</v>
       </c>
@@ -29720,8 +30072,11 @@
       <c r="AO212">
         <v>0</v>
       </c>
+      <c r="AP212">
+        <v>0</v>
+      </c>
     </row>
-    <row r="213" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>234</v>
       </c>
@@ -29840,8 +30195,11 @@
       <c r="AO213">
         <v>0</v>
       </c>
+      <c r="AP213">
+        <v>0</v>
+      </c>
     </row>
-    <row r="214" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>235</v>
       </c>
@@ -29960,8 +30318,11 @@
       <c r="AO214">
         <v>0</v>
       </c>
+      <c r="AP214">
+        <v>0</v>
+      </c>
     </row>
-    <row r="215" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>236</v>
       </c>
@@ -30080,8 +30441,11 @@
       <c r="AO215">
         <v>0</v>
       </c>
+      <c r="AP215">
+        <v>0</v>
+      </c>
     </row>
-    <row r="216" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>237</v>
       </c>
@@ -30203,8 +30567,11 @@
       <c r="AO216">
         <v>0</v>
       </c>
+      <c r="AP216">
+        <v>0</v>
+      </c>
     </row>
-    <row r="217" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>238</v>
       </c>
@@ -30323,8 +30690,11 @@
       <c r="AO217">
         <v>0</v>
       </c>
+      <c r="AP217">
+        <v>0</v>
+      </c>
     </row>
-    <row r="218" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>239</v>
       </c>
@@ -30443,8 +30813,11 @@
       <c r="AO218">
         <v>0</v>
       </c>
+      <c r="AP218">
+        <v>0</v>
+      </c>
     </row>
-    <row r="219" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>240</v>
       </c>
@@ -30563,8 +30936,11 @@
       <c r="AO219">
         <v>0</v>
       </c>
+      <c r="AP219">
+        <v>0</v>
+      </c>
     </row>
-    <row r="220" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>241</v>
       </c>
@@ -30683,8 +31059,11 @@
       <c r="AO220">
         <v>0</v>
       </c>
+      <c r="AP220">
+        <v>0</v>
+      </c>
     </row>
-    <row r="221" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>242</v>
       </c>
@@ -30803,8 +31182,11 @@
       <c r="AO221" t="s">
         <v>308</v>
       </c>
+      <c r="AP221" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="222" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>243</v>
       </c>
@@ -30923,8 +31305,11 @@
       <c r="AO222">
         <v>0</v>
       </c>
+      <c r="AP222">
+        <v>0</v>
+      </c>
     </row>
-    <row r="223" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>244</v>
       </c>
@@ -31046,8 +31431,11 @@
       <c r="AO223">
         <v>0</v>
       </c>
+      <c r="AP223">
+        <v>0</v>
+      </c>
     </row>
-    <row r="224" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>245</v>
       </c>
@@ -31166,8 +31554,11 @@
       <c r="AO224">
         <v>0</v>
       </c>
+      <c r="AP224">
+        <v>0</v>
+      </c>
     </row>
-    <row r="225" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>246</v>
       </c>
@@ -31289,8 +31680,11 @@
       <c r="AO225">
         <v>0</v>
       </c>
+      <c r="AP225">
+        <v>0</v>
+      </c>
     </row>
-    <row r="226" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>247</v>
       </c>
@@ -31409,8 +31803,11 @@
       <c r="AO226">
         <v>0</v>
       </c>
+      <c r="AP226">
+        <v>0</v>
+      </c>
     </row>
-    <row r="227" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>248</v>
       </c>
@@ -31529,8 +31926,11 @@
       <c r="AO227">
         <v>0</v>
       </c>
+      <c r="AP227">
+        <v>0</v>
+      </c>
     </row>
-    <row r="228" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>249</v>
       </c>
@@ -31649,8 +32049,11 @@
       <c r="AO228">
         <v>0</v>
       </c>
+      <c r="AP228">
+        <v>0</v>
+      </c>
     </row>
-    <row r="229" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>250</v>
       </c>
@@ -31769,8 +32172,11 @@
       <c r="AO229">
         <v>0</v>
       </c>
+      <c r="AP229">
+        <v>0</v>
+      </c>
     </row>
-    <row r="230" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>251</v>
       </c>
@@ -31889,8 +32295,11 @@
       <c r="AO230">
         <v>0</v>
       </c>
+      <c r="AP230">
+        <v>0</v>
+      </c>
     </row>
-    <row r="231" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>252</v>
       </c>
@@ -32009,8 +32418,11 @@
       <c r="AO231">
         <v>0</v>
       </c>
+      <c r="AP231">
+        <v>0</v>
+      </c>
     </row>
-    <row r="232" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>253</v>
       </c>
@@ -32129,8 +32541,11 @@
       <c r="AO232">
         <v>0</v>
       </c>
+      <c r="AP232">
+        <v>0</v>
+      </c>
     </row>
-    <row r="233" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>254</v>
       </c>
@@ -32249,8 +32664,11 @@
       <c r="AO233">
         <v>0</v>
       </c>
+      <c r="AP233">
+        <v>0</v>
+      </c>
     </row>
-    <row r="234" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>255</v>
       </c>
@@ -32369,8 +32787,11 @@
       <c r="AO234">
         <v>0</v>
       </c>
+      <c r="AP234">
+        <v>0</v>
+      </c>
     </row>
-    <row r="235" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>256</v>
       </c>
@@ -32489,8 +32910,11 @@
       <c r="AO235">
         <v>0</v>
       </c>
+      <c r="AP235">
+        <v>0</v>
+      </c>
     </row>
-    <row r="236" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>257</v>
       </c>
@@ -32609,8 +33033,11 @@
       <c r="AO236">
         <v>0</v>
       </c>
+      <c r="AP236">
+        <v>0</v>
+      </c>
     </row>
-    <row r="237" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>258</v>
       </c>
@@ -32729,8 +33156,11 @@
       <c r="AO237">
         <v>0</v>
       </c>
+      <c r="AP237">
+        <v>0</v>
+      </c>
     </row>
-    <row r="238" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>259</v>
       </c>
@@ -32849,8 +33279,11 @@
       <c r="AO238">
         <v>0</v>
       </c>
+      <c r="AP238">
+        <v>0</v>
+      </c>
     </row>
-    <row r="239" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>260</v>
       </c>
@@ -32969,8 +33402,11 @@
       <c r="AO239">
         <v>0</v>
       </c>
+      <c r="AP239">
+        <v>0</v>
+      </c>
     </row>
-    <row r="240" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>261</v>
       </c>
@@ -33089,8 +33525,11 @@
       <c r="AO240">
         <v>0</v>
       </c>
+      <c r="AP240">
+        <v>0</v>
+      </c>
     </row>
-    <row r="241" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>262</v>
       </c>
@@ -33209,8 +33648,11 @@
       <c r="AO241">
         <v>0</v>
       </c>
+      <c r="AP241">
+        <v>0</v>
+      </c>
     </row>
-    <row r="242" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>263</v>
       </c>
@@ -33329,8 +33771,11 @@
       <c r="AO242">
         <v>0</v>
       </c>
+      <c r="AP242">
+        <v>0</v>
+      </c>
     </row>
-    <row r="243" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>264</v>
       </c>
@@ -33449,8 +33894,11 @@
       <c r="AO243">
         <v>0</v>
       </c>
+      <c r="AP243">
+        <v>0</v>
+      </c>
     </row>
-    <row r="244" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>265</v>
       </c>
@@ -33569,8 +34017,11 @@
       <c r="AO244">
         <v>0</v>
       </c>
+      <c r="AP244">
+        <v>0</v>
+      </c>
     </row>
-    <row r="245" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>266</v>
       </c>
@@ -33689,8 +34140,11 @@
       <c r="AO245">
         <v>0</v>
       </c>
+      <c r="AP245">
+        <v>0</v>
+      </c>
     </row>
-    <row r="246" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>267</v>
       </c>
@@ -33809,8 +34263,11 @@
       <c r="AO246">
         <v>0</v>
       </c>
+      <c r="AP246">
+        <v>0</v>
+      </c>
     </row>
-    <row r="247" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>268</v>
       </c>
@@ -33929,8 +34386,11 @@
       <c r="AO247">
         <v>0</v>
       </c>
+      <c r="AP247">
+        <v>0</v>
+      </c>
     </row>
-    <row r="248" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>269</v>
       </c>
@@ -34049,8 +34509,11 @@
       <c r="AO248">
         <v>0</v>
       </c>
+      <c r="AP248">
+        <v>0</v>
+      </c>
     </row>
-    <row r="249" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>270</v>
       </c>
@@ -34169,8 +34632,11 @@
       <c r="AO249">
         <v>0</v>
       </c>
+      <c r="AP249">
+        <v>0</v>
+      </c>
     </row>
-    <row r="250" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>271</v>
       </c>
@@ -34289,8 +34755,11 @@
       <c r="AO250">
         <v>0</v>
       </c>
+      <c r="AP250">
+        <v>0</v>
+      </c>
     </row>
-    <row r="251" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>272</v>
       </c>
@@ -34409,8 +34878,11 @@
       <c r="AO251">
         <v>0</v>
       </c>
+      <c r="AP251">
+        <v>0</v>
+      </c>
     </row>
-    <row r="252" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>273</v>
       </c>
@@ -34529,8 +35001,11 @@
       <c r="AO252">
         <v>0</v>
       </c>
+      <c r="AP252">
+        <v>0</v>
+      </c>
     </row>
-    <row r="253" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>274</v>
       </c>
@@ -34649,8 +35124,11 @@
       <c r="AO253">
         <v>0</v>
       </c>
+      <c r="AP253">
+        <v>0</v>
+      </c>
     </row>
-    <row r="254" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>275</v>
       </c>
@@ -34769,8 +35247,11 @@
       <c r="AO254">
         <v>0</v>
       </c>
+      <c r="AP254">
+        <v>0</v>
+      </c>
     </row>
-    <row r="255" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>276</v>
       </c>
@@ -34889,8 +35370,11 @@
       <c r="AO255">
         <v>0</v>
       </c>
+      <c r="AP255">
+        <v>0</v>
+      </c>
     </row>
-    <row r="256" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>277</v>
       </c>
@@ -35009,8 +35493,11 @@
       <c r="AO256">
         <v>0</v>
       </c>
+      <c r="AP256">
+        <v>0</v>
+      </c>
     </row>
-    <row r="257" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>278</v>
       </c>
@@ -35129,8 +35616,11 @@
       <c r="AO257">
         <v>0</v>
       </c>
+      <c r="AP257">
+        <v>0</v>
+      </c>
     </row>
-    <row r="258" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>279</v>
       </c>
@@ -35249,8 +35739,11 @@
       <c r="AO258">
         <v>0</v>
       </c>
+      <c r="AP258">
+        <v>0</v>
+      </c>
     </row>
-    <row r="259" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>280</v>
       </c>
@@ -35369,8 +35862,11 @@
       <c r="AO259">
         <v>0</v>
       </c>
+      <c r="AP259">
+        <v>0</v>
+      </c>
     </row>
-    <row r="260" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>281</v>
       </c>
@@ -35489,8 +35985,11 @@
       <c r="AO260">
         <v>0</v>
       </c>
+      <c r="AP260">
+        <v>0</v>
+      </c>
     </row>
-    <row r="261" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>282</v>
       </c>
@@ -35609,8 +36108,11 @@
       <c r="AO261">
         <v>0</v>
       </c>
+      <c r="AP261">
+        <v>0</v>
+      </c>
     </row>
-    <row r="262" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>283</v>
       </c>
@@ -35729,8 +36231,11 @@
       <c r="AO262">
         <v>0</v>
       </c>
+      <c r="AP262">
+        <v>0</v>
+      </c>
     </row>
-    <row r="263" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>284</v>
       </c>
@@ -35849,8 +36354,11 @@
       <c r="AO263">
         <v>0</v>
       </c>
+      <c r="AP263">
+        <v>0</v>
+      </c>
     </row>
-    <row r="264" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>285</v>
       </c>
@@ -35969,8 +36477,11 @@
       <c r="AO264">
         <v>0</v>
       </c>
+      <c r="AP264">
+        <v>0</v>
+      </c>
     </row>
-    <row r="265" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>286</v>
       </c>
@@ -36089,8 +36600,11 @@
       <c r="AO265">
         <v>0</v>
       </c>
+      <c r="AP265">
+        <v>0</v>
+      </c>
     </row>
-    <row r="266" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>287</v>
       </c>
@@ -36209,8 +36723,11 @@
       <c r="AO266">
         <v>0</v>
       </c>
+      <c r="AP266">
+        <v>0</v>
+      </c>
     </row>
-    <row r="267" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>288</v>
       </c>
@@ -36329,8 +36846,11 @@
       <c r="AO267">
         <v>0</v>
       </c>
+      <c r="AP267">
+        <v>0</v>
+      </c>
     </row>
-    <row r="268" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>289</v>
       </c>
@@ -36449,8 +36969,11 @@
       <c r="AO268">
         <v>0</v>
       </c>
+      <c r="AP268">
+        <v>0</v>
+      </c>
     </row>
-    <row r="269" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>290</v>
       </c>
@@ -36569,8 +37092,11 @@
       <c r="AO269">
         <v>0</v>
       </c>
+      <c r="AP269">
+        <v>0</v>
+      </c>
     </row>
-    <row r="270" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>291</v>
       </c>
@@ -36689,8 +37215,11 @@
       <c r="AO270">
         <v>0</v>
       </c>
+      <c r="AP270">
+        <v>0</v>
+      </c>
     </row>
-    <row r="271" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>292</v>
       </c>
@@ -36809,8 +37338,11 @@
       <c r="AO271">
         <v>0</v>
       </c>
+      <c r="AP271">
+        <v>0</v>
+      </c>
     </row>
-    <row r="272" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>293</v>
       </c>
@@ -36934,8 +37466,11 @@
       <c r="AO272" t="s">
         <v>308</v>
       </c>
+      <c r="AP272" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="273" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>296</v>
       </c>
@@ -37056,8 +37591,11 @@
       <c r="AO273">
         <v>0</v>
       </c>
+      <c r="AP273">
+        <v>0</v>
+      </c>
     </row>
-    <row r="274" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>297</v>
       </c>
@@ -37178,8 +37716,11 @@
       <c r="AO274">
         <v>0</v>
       </c>
+      <c r="AP274">
+        <v>0</v>
+      </c>
     </row>
-    <row r="275" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>298</v>
       </c>
@@ -37303,8 +37844,11 @@
       <c r="AO275" t="s">
         <v>308</v>
       </c>
+      <c r="AP275" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="276" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>299</v>
       </c>
@@ -37428,8 +37972,11 @@
       <c r="AO276">
         <v>0</v>
       </c>
+      <c r="AP276">
+        <v>0</v>
+      </c>
     </row>
-    <row r="277" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>300</v>
       </c>
@@ -37550,8 +38097,11 @@
       <c r="AO277">
         <v>0</v>
       </c>
+      <c r="AP277">
+        <v>0</v>
+      </c>
     </row>
-    <row r="278" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>301</v>
       </c>
@@ -37672,8 +38222,11 @@
       <c r="AO278">
         <v>0</v>
       </c>
+      <c r="AP278">
+        <v>0</v>
+      </c>
     </row>
-    <row r="279" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>302</v>
       </c>
@@ -37797,8 +38350,11 @@
       <c r="AO279" t="s">
         <v>308</v>
       </c>
+      <c r="AP279" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="280" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>303</v>
       </c>
@@ -37919,8 +38475,11 @@
       <c r="AO280">
         <v>0</v>
       </c>
+      <c r="AP280">
+        <v>0</v>
+      </c>
     </row>
-    <row r="281" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>304</v>
       </c>
@@ -38041,8 +38600,11 @@
       <c r="AO281">
         <v>0</v>
       </c>
+      <c r="AP281">
+        <v>0</v>
+      </c>
     </row>
-    <row r="282" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>305</v>
       </c>
@@ -38166,8 +38728,11 @@
       <c r="AO282" t="s">
         <v>308</v>
       </c>
+      <c r="AP282" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="283" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>306</v>
       </c>
@@ -38291,8 +38856,11 @@
       <c r="AO283" t="s">
         <v>308</v>
       </c>
+      <c r="AP283" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="284" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>309</v>
       </c>
@@ -38413,8 +38981,11 @@
       <c r="AO284">
         <v>0</v>
       </c>
+      <c r="AP284">
+        <v>0</v>
+      </c>
     </row>
-    <row r="285" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>310</v>
       </c>
@@ -38535,8 +39106,11 @@
       <c r="AO285">
         <v>0</v>
       </c>
+      <c r="AP285">
+        <v>0</v>
+      </c>
     </row>
-    <row r="286" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>311</v>
       </c>
@@ -38657,8 +39231,11 @@
       <c r="AO286">
         <v>0</v>
       </c>
+      <c r="AP286">
+        <v>0</v>
+      </c>
     </row>
-    <row r="287" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>312</v>
       </c>
@@ -38779,8 +39356,11 @@
       <c r="AO287">
         <v>0</v>
       </c>
+      <c r="AP287">
+        <v>0</v>
+      </c>
     </row>
-    <row r="288" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>313</v>
       </c>
@@ -38901,8 +39481,11 @@
       <c r="AO288">
         <v>0</v>
       </c>
+      <c r="AP288">
+        <v>0</v>
+      </c>
     </row>
-    <row r="289" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>314</v>
       </c>
@@ -39023,8 +39606,11 @@
       <c r="AO289">
         <v>0</v>
       </c>
+      <c r="AP289">
+        <v>0</v>
+      </c>
     </row>
-    <row r="290" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>315</v>
       </c>
@@ -39145,8 +39731,11 @@
       <c r="AO290">
         <v>0</v>
       </c>
+      <c r="AP290">
+        <v>0</v>
+      </c>
     </row>
-    <row r="291" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>316</v>
       </c>
@@ -39267,8 +39856,11 @@
       <c r="AO291">
         <v>0</v>
       </c>
+      <c r="AP291">
+        <v>0</v>
+      </c>
     </row>
-    <row r="292" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>317</v>
       </c>
@@ -39389,8 +39981,11 @@
       <c r="AO292">
         <v>0</v>
       </c>
+      <c r="AP292">
+        <v>0</v>
+      </c>
     </row>
-    <row r="293" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>318</v>
       </c>
@@ -39511,8 +40106,11 @@
       <c r="AO293">
         <v>0</v>
       </c>
+      <c r="AP293">
+        <v>0</v>
+      </c>
     </row>
-    <row r="294" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>319</v>
       </c>
@@ -39636,8 +40234,11 @@
       <c r="AO294">
         <v>0</v>
       </c>
+      <c r="AP294">
+        <v>0</v>
+      </c>
     </row>
-    <row r="295" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>321</v>
       </c>
@@ -39758,8 +40359,11 @@
       <c r="AO295">
         <v>0</v>
       </c>
+      <c r="AP295">
+        <v>0</v>
+      </c>
     </row>
-    <row r="296" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>322</v>
       </c>
@@ -39880,8 +40484,11 @@
       <c r="AO296">
         <v>0</v>
       </c>
+      <c r="AP296">
+        <v>0</v>
+      </c>
     </row>
-    <row r="297" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>323</v>
       </c>
@@ -40005,8 +40612,11 @@
       <c r="AO297" t="s">
         <v>308</v>
       </c>
+      <c r="AP297" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="298" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>324</v>
       </c>
@@ -40127,8 +40737,11 @@
       <c r="AO298">
         <v>6</v>
       </c>
+      <c r="AP298">
+        <v>6</v>
+      </c>
     </row>
-    <row r="299" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>325</v>
       </c>
@@ -40252,8 +40865,11 @@
       <c r="AO299" t="s">
         <v>308</v>
       </c>
+      <c r="AP299" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="300" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>326</v>
       </c>
@@ -40374,8 +40990,11 @@
       <c r="AO300">
         <v>0</v>
       </c>
+      <c r="AP300">
+        <v>0</v>
+      </c>
     </row>
-    <row r="301" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>327</v>
       </c>
@@ -40494,6 +41113,9 @@
         <v>6</v>
       </c>
       <c r="AO301">
+        <v>0</v>
+      </c>
+      <c r="AP301">
         <v>0</v>
       </c>
     </row>
@@ -42375,7 +42997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>343</v>
       </c>
@@ -42499,8 +43121,11 @@
       <c r="AO317" t="s">
         <v>308</v>
       </c>
+      <c r="AP317" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="318" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>344</v>
       </c>
@@ -42621,8 +43246,11 @@
       <c r="AO318">
         <v>0</v>
       </c>
+      <c r="AP318">
+        <v>0</v>
+      </c>
     </row>
-    <row r="319" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>345</v>
       </c>
@@ -42743,8 +43371,11 @@
       <c r="AO319">
         <v>0</v>
       </c>
+      <c r="AP319">
+        <v>0</v>
+      </c>
     </row>
-    <row r="320" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>346</v>
       </c>
@@ -42865,8 +43496,11 @@
       <c r="AO320">
         <v>0</v>
       </c>
+      <c r="AP320">
+        <v>0</v>
+      </c>
     </row>
-    <row r="321" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>347</v>
       </c>
@@ -42987,8 +43621,11 @@
       <c r="AO321">
         <v>0</v>
       </c>
+      <c r="AP321">
+        <v>0</v>
+      </c>
     </row>
-    <row r="322" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>348</v>
       </c>
@@ -43112,8 +43749,11 @@
       <c r="AO322" t="s">
         <v>308</v>
       </c>
+      <c r="AP322" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="323" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>350</v>
       </c>
@@ -43234,8 +43874,11 @@
       <c r="AO323">
         <v>0</v>
       </c>
+      <c r="AP323">
+        <v>0</v>
+      </c>
     </row>
-    <row r="324" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>351</v>
       </c>
@@ -43359,8 +44002,11 @@
       <c r="AO324" t="s">
         <v>308</v>
       </c>
+      <c r="AP324" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="325" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>353</v>
       </c>
@@ -43481,8 +44127,11 @@
       <c r="AO325">
         <v>6</v>
       </c>
+      <c r="AP325">
+        <v>6</v>
+      </c>
     </row>
-    <row r="326" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>354</v>
       </c>
@@ -43603,8 +44252,11 @@
       <c r="AO326">
         <v>0</v>
       </c>
+      <c r="AP326">
+        <v>0</v>
+      </c>
     </row>
-    <row r="327" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>355</v>
       </c>
@@ -43725,8 +44377,11 @@
       <c r="AO327">
         <v>0</v>
       </c>
+      <c r="AP327">
+        <v>0</v>
+      </c>
     </row>
-    <row r="328" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>356</v>
       </c>
@@ -43850,8 +44505,11 @@
       <c r="AO328" t="s">
         <v>308</v>
       </c>
+      <c r="AP328" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="329" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>357</v>
       </c>
@@ -43972,8 +44630,11 @@
       <c r="AO329">
         <v>0</v>
       </c>
+      <c r="AP329">
+        <v>0</v>
+      </c>
     </row>
-    <row r="330" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>358</v>
       </c>
@@ -44097,8 +44758,11 @@
       <c r="AO330" t="s">
         <v>308</v>
       </c>
+      <c r="AP330" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="331" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>359</v>
       </c>
@@ -44217,6 +44881,9 @@
         <v>308</v>
       </c>
       <c r="AO331" t="s">
+        <v>308</v>
+      </c>
+      <c r="AP331" t="s">
         <v>308</v>
       </c>
     </row>
@@ -48000,7 +48667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="362" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>390</v>
       </c>
@@ -48121,8 +48788,11 @@
       <c r="AO362">
         <v>0</v>
       </c>
+      <c r="AP362">
+        <v>0</v>
+      </c>
     </row>
-    <row r="363" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>393</v>
       </c>
@@ -48243,8 +48913,11 @@
       <c r="AO363">
         <v>0</v>
       </c>
+      <c r="AP363">
+        <v>0</v>
+      </c>
     </row>
-    <row r="364" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>394</v>
       </c>
@@ -48365,8 +49038,11 @@
       <c r="AO364">
         <v>0</v>
       </c>
+      <c r="AP364">
+        <v>0</v>
+      </c>
     </row>
-    <row r="365" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>395</v>
       </c>
@@ -48487,8 +49163,11 @@
       <c r="AO365">
         <v>0</v>
       </c>
+      <c r="AP365">
+        <v>0</v>
+      </c>
     </row>
-    <row r="366" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>396</v>
       </c>
@@ -48609,8 +49288,11 @@
       <c r="AO366">
         <v>0</v>
       </c>
+      <c r="AP366">
+        <v>0</v>
+      </c>
     </row>
-    <row r="367" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>397</v>
       </c>
@@ -48731,8 +49413,11 @@
       <c r="AO367">
         <v>0</v>
       </c>
+      <c r="AP367">
+        <v>0</v>
+      </c>
     </row>
-    <row r="368" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>398</v>
       </c>
@@ -48853,8 +49538,11 @@
       <c r="AO368">
         <v>0</v>
       </c>
+      <c r="AP368">
+        <v>0</v>
+      </c>
     </row>
-    <row r="369" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>399</v>
       </c>
@@ -48978,8 +49666,11 @@
       <c r="AO369">
         <v>0</v>
       </c>
+      <c r="AP369">
+        <v>0</v>
+      </c>
     </row>
-    <row r="370" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>400</v>
       </c>
@@ -49100,8 +49791,11 @@
       <c r="AO370">
         <v>0</v>
       </c>
+      <c r="AP370">
+        <v>0</v>
+      </c>
     </row>
-    <row r="371" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>401</v>
       </c>
@@ -49222,8 +49916,11 @@
       <c r="AO371">
         <v>0</v>
       </c>
+      <c r="AP371">
+        <v>0</v>
+      </c>
     </row>
-    <row r="372" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>402</v>
       </c>
@@ -49344,8 +50041,11 @@
       <c r="AO372">
         <v>0</v>
       </c>
+      <c r="AP372">
+        <v>0</v>
+      </c>
     </row>
-    <row r="373" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>403</v>
       </c>
@@ -49469,8 +50169,11 @@
       <c r="AO373">
         <v>0</v>
       </c>
+      <c r="AP373">
+        <v>0</v>
+      </c>
     </row>
-    <row r="374" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>404</v>
       </c>
@@ -49591,8 +50294,11 @@
       <c r="AO374">
         <v>0</v>
       </c>
+      <c r="AP374">
+        <v>0</v>
+      </c>
     </row>
-    <row r="375" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>405</v>
       </c>
@@ -49713,8 +50419,11 @@
       <c r="AO375">
         <v>0</v>
       </c>
+      <c r="AP375">
+        <v>0</v>
+      </c>
     </row>
-    <row r="376" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>406</v>
       </c>
@@ -49835,8 +50544,11 @@
       <c r="AO376">
         <v>0</v>
       </c>
+      <c r="AP376">
+        <v>0</v>
+      </c>
     </row>
-    <row r="377" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>407</v>
       </c>
@@ -49957,8 +50669,11 @@
       <c r="AO377">
         <v>0</v>
       </c>
+      <c r="AP377">
+        <v>0</v>
+      </c>
     </row>
-    <row r="378" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>408</v>
       </c>
@@ -50079,8 +50794,11 @@
       <c r="AO378">
         <v>0</v>
       </c>
+      <c r="AP378">
+        <v>0</v>
+      </c>
     </row>
-    <row r="379" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>409</v>
       </c>
@@ -50201,8 +50919,11 @@
       <c r="AO379">
         <v>0</v>
       </c>
+      <c r="AP379">
+        <v>0</v>
+      </c>
     </row>
-    <row r="380" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>410</v>
       </c>
@@ -50326,8 +51047,11 @@
       <c r="AO380">
         <v>0</v>
       </c>
+      <c r="AP380">
+        <v>0</v>
+      </c>
     </row>
-    <row r="381" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>412</v>
       </c>
@@ -50448,8 +51172,11 @@
       <c r="AO381">
         <v>0</v>
       </c>
+      <c r="AP381">
+        <v>0</v>
+      </c>
     </row>
-    <row r="382" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>413</v>
       </c>
@@ -50570,8 +51297,11 @@
       <c r="AO382">
         <v>0</v>
       </c>
+      <c r="AP382">
+        <v>0</v>
+      </c>
     </row>
-    <row r="383" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>414</v>
       </c>
@@ -50692,8 +51422,11 @@
       <c r="AO383">
         <v>0</v>
       </c>
+      <c r="AP383">
+        <v>0</v>
+      </c>
     </row>
-    <row r="384" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>415</v>
       </c>
@@ -50814,8 +51547,11 @@
       <c r="AO384">
         <v>0</v>
       </c>
+      <c r="AP384">
+        <v>0</v>
+      </c>
     </row>
-    <row r="385" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>416</v>
       </c>
@@ -50936,8 +51672,11 @@
       <c r="AO385">
         <v>0</v>
       </c>
+      <c r="AP385">
+        <v>0</v>
+      </c>
     </row>
-    <row r="386" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>417</v>
       </c>
@@ -51061,8 +51800,11 @@
       <c r="AO386">
         <v>0</v>
       </c>
+      <c r="AP386">
+        <v>0</v>
+      </c>
     </row>
-    <row r="387" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>418</v>
       </c>
@@ -51183,8 +51925,11 @@
       <c r="AO387" t="s">
         <v>308</v>
       </c>
+      <c r="AP387" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="388" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>419</v>
       </c>
@@ -51305,8 +52050,11 @@
       <c r="AO388">
         <v>0</v>
       </c>
+      <c r="AP388">
+        <v>0</v>
+      </c>
     </row>
-    <row r="389" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>420</v>
       </c>
@@ -51427,8 +52175,11 @@
       <c r="AO389">
         <v>0</v>
       </c>
+      <c r="AP389">
+        <v>0</v>
+      </c>
     </row>
-    <row r="390" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>421</v>
       </c>
@@ -51549,8 +52300,11 @@
       <c r="AO390">
         <v>0</v>
       </c>
+      <c r="AP390">
+        <v>0</v>
+      </c>
     </row>
-    <row r="391" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>422</v>
       </c>
@@ -51672,6 +52426,9 @@
         <v>308</v>
       </c>
       <c r="AO391" t="s">
+        <v>308</v>
+      </c>
+      <c r="AP391" t="s">
         <v>308</v>
       </c>
     </row>
@@ -53562,7 +54319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>439</v>
       </c>
@@ -53687,7 +54444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>440</v>
       </c>
@@ -53812,7 +54569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>441</v>
       </c>
@@ -53937,7 +54694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>442</v>
       </c>
@@ -54062,7 +54819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>443</v>
       </c>
@@ -54187,7 +54944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>444</v>
       </c>
@@ -54312,7 +55069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>445</v>
       </c>
@@ -54437,7 +55194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>446</v>
       </c>
@@ -54562,7 +55319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>447</v>
       </c>
@@ -54687,7 +55444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>448</v>
       </c>
@@ -54812,7 +55569,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="417" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>449</v>
       </c>
@@ -54940,7 +55697,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="418" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>450</v>
       </c>
@@ -55065,7 +55822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>451</v>
       </c>
@@ -55190,7 +55947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>452</v>
       </c>
@@ -55315,7 +56072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>453</v>
       </c>
@@ -59208,7 +59965,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="452" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
         <v>487</v>
       </c>
@@ -59329,8 +60086,11 @@
       <c r="AO452">
         <v>0</v>
       </c>
+      <c r="AP452">
+        <v>0</v>
+      </c>
     </row>
-    <row r="453" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>490</v>
       </c>
@@ -59451,8 +60211,11 @@
       <c r="AO453">
         <v>6</v>
       </c>
+      <c r="AP453">
+        <v>0</v>
+      </c>
     </row>
-    <row r="454" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
         <v>491</v>
       </c>
@@ -59573,8 +60336,11 @@
       <c r="AO454">
         <v>0</v>
       </c>
+      <c r="AP454">
+        <v>0</v>
+      </c>
     </row>
-    <row r="455" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>492</v>
       </c>
@@ -59695,8 +60461,11 @@
       <c r="AO455">
         <v>0</v>
       </c>
+      <c r="AP455">
+        <v>0</v>
+      </c>
     </row>
-    <row r="456" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
         <v>493</v>
       </c>
@@ -59817,8 +60586,11 @@
       <c r="AO456">
         <v>0</v>
       </c>
+      <c r="AP456">
+        <v>0</v>
+      </c>
     </row>
-    <row r="457" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>494</v>
       </c>
@@ -59942,8 +60714,11 @@
       <c r="AO457">
         <v>0</v>
       </c>
+      <c r="AP457" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="458" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
         <v>495</v>
       </c>
@@ -60064,8 +60839,11 @@
       <c r="AO458">
         <v>6</v>
       </c>
+      <c r="AP458" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="459" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>496</v>
       </c>
@@ -60186,8 +60964,11 @@
       <c r="AO459">
         <v>0</v>
       </c>
+      <c r="AP459" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="460" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
         <v>497</v>
       </c>
@@ -60308,8 +61089,11 @@
       <c r="AO460">
         <v>0</v>
       </c>
+      <c r="AP460" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="461" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
         <v>498</v>
       </c>
@@ -60430,8 +61214,11 @@
       <c r="AO461">
         <v>0</v>
       </c>
+      <c r="AP461" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="462" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
         <v>499</v>
       </c>
@@ -60552,8 +61339,11 @@
       <c r="AO462">
         <v>0</v>
       </c>
+      <c r="AP462" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="463" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
         <v>500</v>
       </c>
@@ -60674,8 +61464,11 @@
       <c r="AO463">
         <v>6</v>
       </c>
+      <c r="AP463" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="464" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
         <v>501</v>
       </c>
@@ -60796,8 +61589,11 @@
       <c r="AO464">
         <v>6</v>
       </c>
+      <c r="AP464" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="465" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>502</v>
       </c>
@@ -60918,8 +61714,11 @@
       <c r="AO465">
         <v>0</v>
       </c>
+      <c r="AP465" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="466" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>503</v>
       </c>
@@ -61040,8 +61839,11 @@
       <c r="AO466">
         <v>6</v>
       </c>
+      <c r="AP466" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="467" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
         <v>504</v>
       </c>
@@ -61162,8 +61964,11 @@
       <c r="AO467">
         <v>0</v>
       </c>
+      <c r="AP467" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="468" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>505</v>
       </c>
@@ -61287,8 +62092,11 @@
       <c r="AO468" s="2">
         <v>0</v>
       </c>
+      <c r="AP468" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="469" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
         <v>506</v>
       </c>
@@ -61412,8 +62220,11 @@
       <c r="AO469" s="2">
         <v>0</v>
       </c>
+      <c r="AP469" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="470" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>507</v>
       </c>
@@ -61534,8 +62345,11 @@
       <c r="AO470" s="2">
         <v>0</v>
       </c>
+      <c r="AP470" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="471" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
         <v>508</v>
       </c>
@@ -61656,8 +62470,11 @@
       <c r="AO471" s="2">
         <v>0</v>
       </c>
+      <c r="AP471" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="472" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>509</v>
       </c>
@@ -61778,8 +62595,11 @@
       <c r="AO472" s="2">
         <v>0</v>
       </c>
+      <c r="AP472" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="473" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
         <v>510</v>
       </c>
@@ -61900,8 +62720,11 @@
       <c r="AO473" s="2">
         <v>6</v>
       </c>
+      <c r="AP473" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="474" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>511</v>
       </c>
@@ -62022,8 +62845,11 @@
       <c r="AO474" s="2">
         <v>0</v>
       </c>
+      <c r="AP474" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="475" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
         <v>512</v>
       </c>
@@ -62147,8 +62973,11 @@
       <c r="AO475" s="2">
         <v>0</v>
       </c>
+      <c r="AP475" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="476" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
         <v>513</v>
       </c>
@@ -62269,8 +63098,11 @@
       <c r="AO476" s="2">
         <v>0</v>
       </c>
+      <c r="AP476" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="477" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
         <v>514</v>
       </c>
@@ -62391,8 +63223,11 @@
       <c r="AO477" s="2">
         <v>0</v>
       </c>
+      <c r="AP477" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="478" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
         <v>515</v>
       </c>
@@ -62513,8 +63348,11 @@
       <c r="AO478" s="2">
         <v>0</v>
       </c>
+      <c r="AP478" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="479" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
         <v>516</v>
       </c>
@@ -62635,8 +63473,11 @@
       <c r="AO479" s="2">
         <v>6</v>
       </c>
+      <c r="AP479" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="480" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
         <v>517</v>
       </c>
@@ -62757,8 +63598,11 @@
       <c r="AO480" s="2">
         <v>0</v>
       </c>
+      <c r="AP480" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="481" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>518</v>
       </c>
@@ -62877,6 +63721,9 @@
         <v>6</v>
       </c>
       <c r="AO481" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP481" s="2">
         <v>0</v>
       </c>
     </row>
@@ -64761,7 +65608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
         <v>534</v>
       </c>
@@ -64882,8 +65729,11 @@
       <c r="AO497" s="2">
         <v>0</v>
       </c>
+      <c r="AP497" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="498" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
         <v>535</v>
       </c>
@@ -65004,8 +65854,11 @@
       <c r="AO498" s="2">
         <v>0</v>
       </c>
+      <c r="AP498" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="499" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
         <v>536</v>
       </c>
@@ -65126,8 +65979,11 @@
       <c r="AO499" s="2">
         <v>0</v>
       </c>
+      <c r="AP499" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="500" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
         <v>537</v>
       </c>
@@ -65248,8 +66104,11 @@
       <c r="AO500" s="2">
         <v>0</v>
       </c>
+      <c r="AP500" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="501" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
         <v>538</v>
       </c>
@@ -65370,8 +66229,11 @@
       <c r="AO501" s="2">
         <v>0</v>
       </c>
+      <c r="AP501" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="502" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
         <v>539</v>
       </c>
@@ -65492,8 +66354,11 @@
       <c r="AO502" s="2">
         <v>0</v>
       </c>
+      <c r="AP502" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="503" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
         <v>540</v>
       </c>
@@ -65614,8 +66479,11 @@
       <c r="AO503" s="2">
         <v>0</v>
       </c>
+      <c r="AP503" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="504" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
         <v>541</v>
       </c>
@@ -65736,8 +66604,11 @@
       <c r="AO504" s="2">
         <v>0</v>
       </c>
+      <c r="AP504" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="505" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
         <v>542</v>
       </c>
@@ -65858,8 +66729,11 @@
       <c r="AO505" s="2">
         <v>0</v>
       </c>
+      <c r="AP505" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="506" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
         <v>543</v>
       </c>
@@ -65980,8 +66854,11 @@
       <c r="AO506" s="2">
         <v>0</v>
       </c>
+      <c r="AP506" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="507" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
         <v>544</v>
       </c>
@@ -66102,8 +66979,11 @@
       <c r="AO507" s="2">
         <v>0</v>
       </c>
+      <c r="AP507" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="508" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A508" t="s">
         <v>545</v>
       </c>
@@ -66224,8 +67104,11 @@
       <c r="AO508" s="2">
         <v>0</v>
       </c>
+      <c r="AP508" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="509" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
         <v>546</v>
       </c>
@@ -66346,8 +67229,11 @@
       <c r="AO509" s="2">
         <v>0</v>
       </c>
+      <c r="AP509" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="510" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A510" t="s">
         <v>547</v>
       </c>
@@ -66468,8 +67354,11 @@
       <c r="AO510" s="2">
         <v>0</v>
       </c>
+      <c r="AP510" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="511" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
         <v>548</v>
       </c>
@@ -66588,6 +67477,9 @@
         <v>0</v>
       </c>
       <c r="AO511" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP511" s="2">
         <v>0</v>
       </c>
     </row>
@@ -70359,7 +71251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="542" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>580</v>
       </c>
@@ -70481,7 +71373,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="543" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
         <v>583</v>
       </c>
@@ -70600,7 +71492,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="544" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>584</v>
       </c>
@@ -70722,7 +71614,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="545" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="545" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A545" t="s">
         <v>585</v>
       </c>
@@ -70841,7 +71733,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="546" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
         <v>586</v>
       </c>
@@ -70960,7 +71852,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="547" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="547" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
         <v>587</v>
       </c>
@@ -71079,7 +71971,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="548" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="548" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
         <v>588</v>
       </c>
@@ -71198,7 +72090,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="549" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="549" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A549" t="s">
         <v>589</v>
       </c>
@@ -71317,7 +72209,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="550" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A550" t="s">
         <v>590</v>
       </c>
@@ -71436,7 +72328,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="551" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A551" t="s">
         <v>591</v>
       </c>
@@ -71555,7 +72447,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="552" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="552" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A552" t="s">
         <v>592</v>
       </c>
@@ -71674,7 +72566,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="553" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="553" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A553" t="s">
         <v>593</v>
       </c>
@@ -71793,7 +72685,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="554" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A554" t="s">
         <v>594</v>
       </c>
@@ -71915,7 +72807,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="555" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="555" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A555" t="s">
         <v>595</v>
       </c>
@@ -72034,7 +72926,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="556" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="556" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A556" t="s">
         <v>596</v>
       </c>
@@ -72153,7 +73045,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="557" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="557" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A557" t="s">
         <v>597</v>
       </c>
@@ -72269,7 +73161,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="558" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A558" t="s">
         <v>598</v>
       </c>
@@ -72388,7 +73280,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="559" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A559" t="s">
         <v>599</v>
       </c>
@@ -72507,7 +73399,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="560" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="560" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A560" t="s">
         <v>600</v>
       </c>
@@ -72626,7 +73518,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="561" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
         <v>601</v>
       </c>
@@ -72745,7 +73637,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="562" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
         <v>602</v>
       </c>
@@ -72864,7 +73756,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="563" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
         <v>603</v>
       </c>
@@ -72983,7 +73875,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="564" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A564" t="s">
         <v>604</v>
       </c>
@@ -73102,7 +73994,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="565" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A565" t="s">
         <v>605</v>
       </c>
@@ -73221,7 +74113,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="566" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A566" t="s">
         <v>606</v>
       </c>
@@ -73340,7 +74232,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="567" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
         <v>607</v>
       </c>
@@ -73459,7 +74351,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="568" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A568" t="s">
         <v>608</v>
       </c>
@@ -73578,7 +74470,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="569" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
         <v>609</v>
       </c>
@@ -73697,7 +74589,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="570" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A570" t="s">
         <v>610</v>
       </c>
@@ -73816,7 +74708,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="571" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
         <v>611</v>
       </c>
@@ -75729,7 +76621,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="587" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
         <v>627</v>
       </c>
@@ -75848,7 +76740,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="588" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A588" t="s">
         <v>628</v>
       </c>
@@ -75967,7 +76859,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="589" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A589" t="s">
         <v>629</v>
       </c>
@@ -76086,7 +76978,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="590" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A590" t="s">
         <v>630</v>
       </c>
@@ -76208,7 +77100,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="591" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A591" t="s">
         <v>631</v>
       </c>
@@ -76327,7 +77219,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="592" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="592" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A592" t="s">
         <v>632</v>
       </c>
@@ -76446,7 +77338,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="593" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A593" t="s">
         <v>633</v>
       </c>
@@ -76565,7 +77457,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="594" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="594" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A594" t="s">
         <v>634</v>
       </c>
@@ -76684,7 +77576,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="595" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
         <v>635</v>
       </c>
@@ -76803,7 +77695,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="596" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A596" t="s">
         <v>636</v>
       </c>
@@ -76922,7 +77814,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="597" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="597" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A597" t="s">
         <v>637</v>
       </c>
@@ -77041,7 +77933,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="598" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A598" t="s">
         <v>638</v>
       </c>
@@ -77160,7 +78052,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="599" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
         <v>639</v>
       </c>
@@ -77279,7 +78171,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="600" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A600" t="s">
         <v>640</v>
       </c>
@@ -77398,7 +78290,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="601" spans="1:40" hidden="1" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A601" t="s">
         <v>641</v>
       </c>

</xml_diff>

<commit_message>
budset and senescence for greenhouse
</commit_message>
<xml_diff>
--- a/data/monitoring_phenology/2024_budburst_to_budset.xlsx
+++ b/data/monitoring_phenology/2024_budburst_to_budset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/data/monitoring_phenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED53541-5B4D-0346-80D6-94A16A039E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAE0FA8-0D02-0047-A25C-812DAE4F0E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phenological_monitoring" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5404" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5420" uniqueCount="745">
   <si>
     <t>tree_ID</t>
   </si>
@@ -3535,11 +3535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP631"/>
+  <dimension ref="A1:AQ631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A538" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AO547" sqref="AO547"/>
+    <sheetView tabSelected="1" topLeftCell="A537" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AR272" sqref="AR272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3551,7 +3551,7 @@
     <col min="30" max="30" width="4.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3678,8 +3678,11 @@
       <c r="AP1" s="3">
         <v>283</v>
       </c>
+      <c r="AQ1" s="3">
+        <v>290</v>
+      </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3806,8 +3809,11 @@
       <c r="AP2">
         <v>6</v>
       </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3931,8 +3937,11 @@
       <c r="AP3">
         <v>6</v>
       </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4056,8 +4065,11 @@
       <c r="AP4">
         <v>6</v>
       </c>
+      <c r="AQ4">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -4181,8 +4193,11 @@
       <c r="AP5">
         <v>6</v>
       </c>
+      <c r="AQ5">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -4306,8 +4321,11 @@
       <c r="AP6">
         <v>6</v>
       </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -4431,8 +4449,11 @@
       <c r="AP7">
         <v>0</v>
       </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -4556,8 +4577,11 @@
       <c r="AP8">
         <v>0</v>
       </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -4681,8 +4705,11 @@
       <c r="AP9">
         <v>0</v>
       </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -4806,8 +4833,11 @@
       <c r="AP10">
         <v>0</v>
       </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -4934,8 +4964,11 @@
       <c r="AP11">
         <v>6</v>
       </c>
+      <c r="AQ11">
+        <v>6</v>
+      </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -5059,8 +5092,11 @@
       <c r="AP12">
         <v>0</v>
       </c>
+      <c r="AQ12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -5184,8 +5220,11 @@
       <c r="AP13">
         <v>6</v>
       </c>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -5309,8 +5348,11 @@
       <c r="AP14">
         <v>6</v>
       </c>
+      <c r="AQ14">
+        <v>6</v>
+      </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -5434,8 +5476,11 @@
       <c r="AP15">
         <v>6</v>
       </c>
+      <c r="AQ15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -5559,8 +5604,11 @@
       <c r="AP16">
         <v>0</v>
       </c>
+      <c r="AQ16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -5684,8 +5732,11 @@
       <c r="AP17">
         <v>0</v>
       </c>
+      <c r="AQ17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -5809,8 +5860,11 @@
       <c r="AP18">
         <v>0</v>
       </c>
+      <c r="AQ18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -5934,8 +5988,11 @@
       <c r="AP19">
         <v>6</v>
       </c>
+      <c r="AQ19">
+        <v>6</v>
+      </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -6059,8 +6116,11 @@
       <c r="AP20">
         <v>6</v>
       </c>
+      <c r="AQ20">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -6184,8 +6244,11 @@
       <c r="AP21">
         <v>0</v>
       </c>
+      <c r="AQ21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -6312,8 +6375,11 @@
       <c r="AP22">
         <v>6</v>
       </c>
+      <c r="AQ22">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -6437,8 +6503,11 @@
       <c r="AP23">
         <v>6</v>
       </c>
+      <c r="AQ23">
+        <v>6</v>
+      </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -6562,8 +6631,11 @@
       <c r="AP24">
         <v>0</v>
       </c>
+      <c r="AQ24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -6687,8 +6759,11 @@
       <c r="AP25">
         <v>0</v>
       </c>
+      <c r="AQ25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -6812,8 +6887,11 @@
       <c r="AP26">
         <v>6</v>
       </c>
+      <c r="AQ26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -6937,8 +7015,11 @@
       <c r="AP27">
         <v>6</v>
       </c>
+      <c r="AQ27">
+        <v>6</v>
+      </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -7065,8 +7146,11 @@
       <c r="AP28">
         <v>0</v>
       </c>
+      <c r="AQ28">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -7193,8 +7277,11 @@
       <c r="AP29" t="s">
         <v>308</v>
       </c>
+      <c r="AQ29" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -7318,8 +7405,11 @@
       <c r="AP30">
         <v>0</v>
       </c>
+      <c r="AQ30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -7443,8 +7533,11 @@
       <c r="AP31">
         <v>0</v>
       </c>
+      <c r="AQ31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -7569,7 +7662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -7694,7 +7787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -7819,7 +7912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -7944,7 +8037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -8069,7 +8162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -8194,7 +8287,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -8319,7 +8412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -8444,7 +8537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -8569,7 +8662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -8694,7 +8787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -8822,7 +8915,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -8947,7 +9040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -9072,7 +9165,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -9197,7 +9290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -9322,7 +9415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -9446,8 +9539,11 @@
       <c r="AP47">
         <v>0</v>
       </c>
+      <c r="AQ47">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -9571,8 +9667,11 @@
       <c r="AP48">
         <v>0</v>
       </c>
+      <c r="AQ48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -9696,8 +9795,11 @@
       <c r="AP49">
         <v>6</v>
       </c>
+      <c r="AQ49">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -9821,8 +9923,11 @@
       <c r="AP50">
         <v>6</v>
       </c>
+      <c r="AQ50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -9946,8 +10051,11 @@
       <c r="AP51">
         <v>0</v>
       </c>
+      <c r="AQ51">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -10071,8 +10179,11 @@
       <c r="AP52">
         <v>0</v>
       </c>
+      <c r="AQ52">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -10196,8 +10307,11 @@
       <c r="AP53">
         <v>6</v>
       </c>
+      <c r="AQ53">
+        <v>6</v>
+      </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -10321,8 +10435,11 @@
       <c r="AP54">
         <v>0</v>
       </c>
+      <c r="AQ54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -10449,8 +10566,11 @@
       <c r="AP55">
         <v>0</v>
       </c>
+      <c r="AQ55">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -10577,8 +10697,11 @@
       <c r="AP56">
         <v>0</v>
       </c>
+      <c r="AQ56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -10705,8 +10828,11 @@
       <c r="AP57">
         <v>0</v>
       </c>
+      <c r="AQ57">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -10830,8 +10956,11 @@
       <c r="AP58">
         <v>0</v>
       </c>
+      <c r="AQ58">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -10955,8 +11084,11 @@
       <c r="AP59" t="s">
         <v>308</v>
       </c>
+      <c r="AQ59" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -11080,8 +11212,11 @@
       <c r="AP60">
         <v>0</v>
       </c>
+      <c r="AQ60">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -11205,8 +11340,11 @@
       <c r="AP61">
         <v>0</v>
       </c>
+      <c r="AQ61">
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -11331,7 +11469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -11456,7 +11594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -13584,7 +13722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>94</v>
       </c>
@@ -13709,7 +13847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>95</v>
       </c>
@@ -13834,7 +13972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>96</v>
       </c>
@@ -13959,7 +14097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>97</v>
       </c>
@@ -14084,7 +14222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>98</v>
       </c>
@@ -14209,7 +14347,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>99</v>
       </c>
@@ -14334,7 +14472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>100</v>
       </c>
@@ -14459,7 +14597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>101</v>
       </c>
@@ -14584,7 +14722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>102</v>
       </c>
@@ -14709,7 +14847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>103</v>
       </c>
@@ -14834,7 +14972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>104</v>
       </c>
@@ -14959,7 +15097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>105</v>
       </c>
@@ -15083,8 +15221,11 @@
       <c r="AP92" s="2">
         <v>6</v>
       </c>
+      <c r="AQ92">
+        <v>6</v>
+      </c>
     </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -15208,8 +15349,11 @@
       <c r="AP93" s="2">
         <v>6</v>
       </c>
+      <c r="AQ93">
+        <v>0</v>
+      </c>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -15331,10 +15475,13 @@
         <v>0</v>
       </c>
       <c r="AP94" s="2">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="AQ94">
+        <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -15461,8 +15608,11 @@
       <c r="AP95" s="2">
         <v>0</v>
       </c>
+      <c r="AQ95">
+        <v>0</v>
+      </c>
     </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>112</v>
       </c>
@@ -15586,8 +15736,11 @@
       <c r="AP96" s="2">
         <v>0</v>
       </c>
+      <c r="AQ96">
+        <v>0</v>
+      </c>
     </row>
-    <row r="97" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>113</v>
       </c>
@@ -15711,8 +15864,11 @@
       <c r="AP97" s="2">
         <v>0</v>
       </c>
+      <c r="AQ97" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="98" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>114</v>
       </c>
@@ -15836,8 +15992,11 @@
       <c r="AP98" s="2">
         <v>0</v>
       </c>
+      <c r="AQ98" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="99" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>115</v>
       </c>
@@ -15961,8 +16120,11 @@
       <c r="AP99" s="2">
         <v>6</v>
       </c>
+      <c r="AQ99" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="100" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>116</v>
       </c>
@@ -16086,8 +16248,11 @@
       <c r="AP100" s="2">
         <v>0</v>
       </c>
+      <c r="AQ100" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="101" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>117</v>
       </c>
@@ -16211,8 +16376,11 @@
       <c r="AP101" s="2">
         <v>6</v>
       </c>
+      <c r="AQ101" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="102" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>118</v>
       </c>
@@ -16336,8 +16504,11 @@
       <c r="AP102" s="2">
         <v>6</v>
       </c>
+      <c r="AQ102" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="103" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>119</v>
       </c>
@@ -16461,8 +16632,11 @@
       <c r="AP103" s="2">
         <v>6</v>
       </c>
+      <c r="AQ103" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="104" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>120</v>
       </c>
@@ -16586,8 +16760,11 @@
       <c r="AP104" s="2">
         <v>0</v>
       </c>
+      <c r="AQ104" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="105" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>121</v>
       </c>
@@ -16711,8 +16888,11 @@
       <c r="AP105" s="2">
         <v>6</v>
       </c>
+      <c r="AQ105" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="106" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>122</v>
       </c>
@@ -16836,8 +17016,11 @@
       <c r="AP106" s="2">
         <v>0</v>
       </c>
+      <c r="AQ106" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="107" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -16961,8 +17144,11 @@
       <c r="AP107" s="2">
         <v>6</v>
       </c>
+      <c r="AQ107" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="108" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>124</v>
       </c>
@@ -17086,8 +17272,11 @@
       <c r="AP108" s="2">
         <v>6</v>
       </c>
+      <c r="AQ108" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="109" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>125</v>
       </c>
@@ -17214,8 +17403,11 @@
       <c r="AP109" s="2">
         <v>0</v>
       </c>
+      <c r="AQ109" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="110" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -17339,8 +17531,11 @@
       <c r="AP110" s="2">
         <v>6</v>
       </c>
+      <c r="AQ110" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="111" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>127</v>
       </c>
@@ -17467,8 +17662,11 @@
       <c r="AP111" s="2">
         <v>6</v>
       </c>
+      <c r="AQ111" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="112" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>128</v>
       </c>
@@ -17592,8 +17790,11 @@
       <c r="AP112" s="2">
         <v>0</v>
       </c>
+      <c r="AQ112" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="113" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -17717,8 +17918,11 @@
       <c r="AP113" t="s">
         <v>308</v>
       </c>
+      <c r="AQ113" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="114" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -17842,8 +18046,11 @@
       <c r="AP114" s="2">
         <v>0</v>
       </c>
+      <c r="AQ114" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="115" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>131</v>
       </c>
@@ -17967,8 +18174,11 @@
       <c r="AP115" s="2">
         <v>6</v>
       </c>
+      <c r="AQ115" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="116" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>132</v>
       </c>
@@ -18092,8 +18302,11 @@
       <c r="AP116" s="2">
         <v>0</v>
       </c>
+      <c r="AQ116" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="117" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>133</v>
       </c>
@@ -18217,8 +18430,11 @@
       <c r="AP117" s="2">
         <v>6</v>
       </c>
+      <c r="AQ117" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="118" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>134</v>
       </c>
@@ -18342,8 +18558,11 @@
       <c r="AP118" s="2">
         <v>6</v>
       </c>
+      <c r="AQ118" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="119" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -18467,8 +18686,11 @@
       <c r="AP119" s="2">
         <v>0</v>
       </c>
+      <c r="AQ119" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="120" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>136</v>
       </c>
@@ -18592,8 +18814,11 @@
       <c r="AP120" s="2">
         <v>6</v>
       </c>
+      <c r="AQ120" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="121" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>137</v>
       </c>
@@ -18720,8 +18945,11 @@
       <c r="AP121" s="2">
         <v>6</v>
       </c>
+      <c r="AQ121" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="122" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>138</v>
       </c>
@@ -18846,7 +19074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>139</v>
       </c>
@@ -18971,7 +19199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>140</v>
       </c>
@@ -19096,7 +19324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>141</v>
       </c>
@@ -19221,7 +19449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>142</v>
       </c>
@@ -19346,7 +19574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="127" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>143</v>
       </c>
@@ -19471,7 +19699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>144</v>
       </c>
@@ -19596,7 +19824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>145</v>
       </c>
@@ -19721,7 +19949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>146</v>
       </c>
@@ -19846,7 +20074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="131" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>147</v>
       </c>
@@ -19974,7 +20202,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="132" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>148</v>
       </c>
@@ -20099,7 +20327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>149</v>
       </c>
@@ -20224,7 +20452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>150</v>
       </c>
@@ -20349,7 +20577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>151</v>
       </c>
@@ -20474,7 +20702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>152</v>
       </c>
@@ -20599,7 +20827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>153</v>
       </c>
@@ -20726,8 +20954,11 @@
       <c r="AP137">
         <v>6</v>
       </c>
+      <c r="AQ137">
+        <v>6</v>
+      </c>
     </row>
-    <row r="138" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>154</v>
       </c>
@@ -20851,8 +21082,11 @@
       <c r="AP138">
         <v>6</v>
       </c>
+      <c r="AQ138">
+        <v>0</v>
+      </c>
     </row>
-    <row r="139" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>155</v>
       </c>
@@ -20976,8 +21210,11 @@
       <c r="AP139">
         <v>6</v>
       </c>
+      <c r="AQ139">
+        <v>6</v>
+      </c>
     </row>
-    <row r="140" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>156</v>
       </c>
@@ -21101,8 +21338,11 @@
       <c r="AP140">
         <v>0</v>
       </c>
+      <c r="AQ140">
+        <v>0</v>
+      </c>
     </row>
-    <row r="141" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>157</v>
       </c>
@@ -21226,8 +21466,11 @@
       <c r="AP141">
         <v>0</v>
       </c>
+      <c r="AQ141">
+        <v>0</v>
+      </c>
     </row>
-    <row r="142" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>158</v>
       </c>
@@ -21351,8 +21594,11 @@
       <c r="AP142">
         <v>0</v>
       </c>
+      <c r="AQ142">
+        <v>0</v>
+      </c>
     </row>
-    <row r="143" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>159</v>
       </c>
@@ -21476,8 +21722,11 @@
       <c r="AP143">
         <v>0</v>
       </c>
+      <c r="AQ143">
+        <v>0</v>
+      </c>
     </row>
-    <row r="144" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>160</v>
       </c>
@@ -21601,8 +21850,11 @@
       <c r="AP144">
         <v>0</v>
       </c>
+      <c r="AQ144">
+        <v>0</v>
+      </c>
     </row>
-    <row r="145" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>161</v>
       </c>
@@ -21726,8 +21978,11 @@
       <c r="AP145">
         <v>0</v>
       </c>
+      <c r="AQ145">
+        <v>0</v>
+      </c>
     </row>
-    <row r="146" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>162</v>
       </c>
@@ -21851,8 +22106,11 @@
       <c r="AP146">
         <v>6</v>
       </c>
+      <c r="AQ146">
+        <v>6</v>
+      </c>
     </row>
-    <row r="147" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>163</v>
       </c>
@@ -21976,8 +22234,11 @@
       <c r="AP147">
         <v>0</v>
       </c>
+      <c r="AQ147">
+        <v>0</v>
+      </c>
     </row>
-    <row r="148" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>164</v>
       </c>
@@ -22104,8 +22365,11 @@
       <c r="AP148">
         <v>6</v>
       </c>
+      <c r="AQ148">
+        <v>0</v>
+      </c>
     </row>
-    <row r="149" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>165</v>
       </c>
@@ -22229,8 +22493,11 @@
       <c r="AP149">
         <v>0</v>
       </c>
+      <c r="AQ149">
+        <v>0</v>
+      </c>
     </row>
-    <row r="150" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>166</v>
       </c>
@@ -22357,8 +22624,11 @@
       <c r="AP150">
         <v>6</v>
       </c>
+      <c r="AQ150">
+        <v>6</v>
+      </c>
     </row>
-    <row r="151" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>167</v>
       </c>
@@ -22482,8 +22752,11 @@
       <c r="AP151">
         <v>0</v>
       </c>
+      <c r="AQ151">
+        <v>0</v>
+      </c>
     </row>
-    <row r="152" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>168</v>
       </c>
@@ -22608,7 +22881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>169</v>
       </c>
@@ -22733,7 +23006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>170</v>
       </c>
@@ -22858,7 +23131,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>171</v>
       </c>
@@ -22983,7 +23256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:43" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>172</v>
       </c>
@@ -23108,7 +23381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>173</v>
       </c>
@@ -23233,7 +23506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>174</v>
       </c>
@@ -23358,7 +23631,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>175</v>
       </c>
@@ -23483,7 +23756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>176</v>
       </c>
@@ -35497,7 +35770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>278</v>
       </c>
@@ -35620,7 +35893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>279</v>
       </c>
@@ -35743,7 +36016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>280</v>
       </c>
@@ -35866,7 +36139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>281</v>
       </c>
@@ -35989,7 +36262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>282</v>
       </c>
@@ -36112,7 +36385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>283</v>
       </c>
@@ -36235,7 +36508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>284</v>
       </c>
@@ -36358,7 +36631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>285</v>
       </c>
@@ -36481,7 +36754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>286</v>
       </c>
@@ -36604,7 +36877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>287</v>
       </c>
@@ -36727,7 +37000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>288</v>
       </c>
@@ -36850,7 +37123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>289</v>
       </c>
@@ -36973,7 +37246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>290</v>
       </c>
@@ -37096,7 +37369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>291</v>
       </c>
@@ -37219,7 +37492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>292</v>
       </c>
@@ -37342,7 +37615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>293</v>
       </c>
@@ -37469,8 +37742,11 @@
       <c r="AP272" t="s">
         <v>308</v>
       </c>
+      <c r="AQ272" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="273" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>296</v>
       </c>
@@ -37594,8 +37870,11 @@
       <c r="AP273">
         <v>0</v>
       </c>
+      <c r="AQ273">
+        <v>0</v>
+      </c>
     </row>
-    <row r="274" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>297</v>
       </c>
@@ -37719,8 +37998,11 @@
       <c r="AP274">
         <v>0</v>
       </c>
+      <c r="AQ274">
+        <v>0</v>
+      </c>
     </row>
-    <row r="275" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>298</v>
       </c>
@@ -37847,8 +38129,11 @@
       <c r="AP275" t="s">
         <v>308</v>
       </c>
+      <c r="AQ275" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="276" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>299</v>
       </c>
@@ -37975,8 +38260,11 @@
       <c r="AP276">
         <v>0</v>
       </c>
+      <c r="AQ276">
+        <v>0</v>
+      </c>
     </row>
-    <row r="277" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>300</v>
       </c>
@@ -38100,8 +38388,11 @@
       <c r="AP277">
         <v>0</v>
       </c>
+      <c r="AQ277">
+        <v>0</v>
+      </c>
     </row>
-    <row r="278" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>301</v>
       </c>
@@ -38225,8 +38516,11 @@
       <c r="AP278">
         <v>0</v>
       </c>
+      <c r="AQ278">
+        <v>0</v>
+      </c>
     </row>
-    <row r="279" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>302</v>
       </c>
@@ -38353,8 +38647,11 @@
       <c r="AP279" t="s">
         <v>308</v>
       </c>
+      <c r="AQ279" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="280" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>303</v>
       </c>
@@ -38478,8 +38775,11 @@
       <c r="AP280">
         <v>0</v>
       </c>
+      <c r="AQ280">
+        <v>0</v>
+      </c>
     </row>
-    <row r="281" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>304</v>
       </c>
@@ -38603,8 +38903,11 @@
       <c r="AP281">
         <v>0</v>
       </c>
+      <c r="AQ281">
+        <v>0</v>
+      </c>
     </row>
-    <row r="282" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>305</v>
       </c>
@@ -38731,8 +39034,11 @@
       <c r="AP282" t="s">
         <v>308</v>
       </c>
+      <c r="AQ282" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="283" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>306</v>
       </c>
@@ -38859,8 +39165,11 @@
       <c r="AP283" t="s">
         <v>308</v>
       </c>
+      <c r="AQ283" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="284" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>309</v>
       </c>
@@ -38984,8 +39293,11 @@
       <c r="AP284">
         <v>0</v>
       </c>
+      <c r="AQ284">
+        <v>0</v>
+      </c>
     </row>
-    <row r="285" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>310</v>
       </c>
@@ -39109,8 +39421,11 @@
       <c r="AP285">
         <v>0</v>
       </c>
+      <c r="AQ285">
+        <v>0</v>
+      </c>
     </row>
-    <row r="286" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>311</v>
       </c>
@@ -39234,8 +39549,11 @@
       <c r="AP286">
         <v>0</v>
       </c>
+      <c r="AQ286">
+        <v>0</v>
+      </c>
     </row>
-    <row r="287" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>312</v>
       </c>
@@ -39359,8 +39677,11 @@
       <c r="AP287">
         <v>0</v>
       </c>
+      <c r="AQ287">
+        <v>0</v>
+      </c>
     </row>
-    <row r="288" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>313</v>
       </c>
@@ -39484,8 +39805,11 @@
       <c r="AP288">
         <v>0</v>
       </c>
+      <c r="AQ288">
+        <v>0</v>
+      </c>
     </row>
-    <row r="289" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>314</v>
       </c>
@@ -39609,8 +39933,11 @@
       <c r="AP289">
         <v>0</v>
       </c>
+      <c r="AQ289">
+        <v>0</v>
+      </c>
     </row>
-    <row r="290" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>315</v>
       </c>
@@ -39734,8 +40061,11 @@
       <c r="AP290">
         <v>0</v>
       </c>
+      <c r="AQ290">
+        <v>0</v>
+      </c>
     </row>
-    <row r="291" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>316</v>
       </c>
@@ -39859,8 +40189,11 @@
       <c r="AP291">
         <v>0</v>
       </c>
+      <c r="AQ291">
+        <v>0</v>
+      </c>
     </row>
-    <row r="292" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>317</v>
       </c>
@@ -39984,8 +40317,11 @@
       <c r="AP292">
         <v>0</v>
       </c>
+      <c r="AQ292">
+        <v>0</v>
+      </c>
     </row>
-    <row r="293" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>318</v>
       </c>
@@ -40109,8 +40445,11 @@
       <c r="AP293">
         <v>0</v>
       </c>
+      <c r="AQ293">
+        <v>0</v>
+      </c>
     </row>
-    <row r="294" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>319</v>
       </c>
@@ -40237,8 +40576,11 @@
       <c r="AP294">
         <v>0</v>
       </c>
+      <c r="AQ294">
+        <v>0</v>
+      </c>
     </row>
-    <row r="295" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>321</v>
       </c>
@@ -40362,8 +40704,11 @@
       <c r="AP295">
         <v>0</v>
       </c>
+      <c r="AQ295">
+        <v>0</v>
+      </c>
     </row>
-    <row r="296" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>322</v>
       </c>
@@ -40487,8 +40832,11 @@
       <c r="AP296">
         <v>0</v>
       </c>
+      <c r="AQ296">
+        <v>0</v>
+      </c>
     </row>
-    <row r="297" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>323</v>
       </c>
@@ -40615,8 +40963,11 @@
       <c r="AP297" t="s">
         <v>308</v>
       </c>
+      <c r="AQ297" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="298" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>324</v>
       </c>
@@ -40740,8 +41091,11 @@
       <c r="AP298">
         <v>6</v>
       </c>
+      <c r="AQ298">
+        <v>6</v>
+      </c>
     </row>
-    <row r="299" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>325</v>
       </c>
@@ -40868,8 +41222,11 @@
       <c r="AP299" t="s">
         <v>308</v>
       </c>
+      <c r="AQ299" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="300" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>326</v>
       </c>
@@ -40993,8 +41350,11 @@
       <c r="AP300">
         <v>0</v>
       </c>
+      <c r="AQ300">
+        <v>0</v>
+      </c>
     </row>
-    <row r="301" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>327</v>
       </c>
@@ -41118,8 +41478,11 @@
       <c r="AP301">
         <v>0</v>
       </c>
+      <c r="AQ301">
+        <v>0</v>
+      </c>
     </row>
-    <row r="302" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>328</v>
       </c>
@@ -41244,7 +41607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>329</v>
       </c>
@@ -41369,7 +41732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>330</v>
       </c>
@@ -41494,7 +41857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>331</v>
       </c>
@@ -41619,7 +41982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>332</v>
       </c>
@@ -41744,7 +42107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>333</v>
       </c>
@@ -41869,7 +42232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>334</v>
       </c>
@@ -41994,7 +42357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>335</v>
       </c>
@@ -42119,7 +42482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>336</v>
       </c>
@@ -42244,7 +42607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>337</v>
       </c>
@@ -42369,7 +42732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>338</v>
       </c>
@@ -42494,7 +42857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>339</v>
       </c>
@@ -42619,7 +42982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>340</v>
       </c>
@@ -42744,7 +43107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>341</v>
       </c>
@@ -42869,7 +43232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>342</v>
       </c>
@@ -42997,7 +43360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>343</v>
       </c>
@@ -43124,8 +43487,11 @@
       <c r="AP317" t="s">
         <v>308</v>
       </c>
+      <c r="AQ317" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="318" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>344</v>
       </c>
@@ -43249,8 +43615,11 @@
       <c r="AP318">
         <v>0</v>
       </c>
+      <c r="AQ318">
+        <v>0</v>
+      </c>
     </row>
-    <row r="319" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>345</v>
       </c>
@@ -43374,8 +43743,11 @@
       <c r="AP319">
         <v>0</v>
       </c>
+      <c r="AQ319">
+        <v>0</v>
+      </c>
     </row>
-    <row r="320" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>346</v>
       </c>
@@ -43499,8 +43871,11 @@
       <c r="AP320">
         <v>0</v>
       </c>
+      <c r="AQ320">
+        <v>0</v>
+      </c>
     </row>
-    <row r="321" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>347</v>
       </c>
@@ -43624,8 +43999,11 @@
       <c r="AP321">
         <v>0</v>
       </c>
+      <c r="AQ321">
+        <v>0</v>
+      </c>
     </row>
-    <row r="322" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>348</v>
       </c>
@@ -43752,8 +44130,11 @@
       <c r="AP322" t="s">
         <v>308</v>
       </c>
+      <c r="AQ322" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="323" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>350</v>
       </c>
@@ -43877,8 +44258,11 @@
       <c r="AP323">
         <v>0</v>
       </c>
+      <c r="AQ323">
+        <v>0</v>
+      </c>
     </row>
-    <row r="324" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>351</v>
       </c>
@@ -44005,8 +44389,11 @@
       <c r="AP324" t="s">
         <v>308</v>
       </c>
+      <c r="AQ324" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="325" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>353</v>
       </c>
@@ -44130,8 +44517,11 @@
       <c r="AP325">
         <v>6</v>
       </c>
+      <c r="AQ325">
+        <v>0</v>
+      </c>
     </row>
-    <row r="326" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>354</v>
       </c>
@@ -44255,8 +44645,11 @@
       <c r="AP326">
         <v>0</v>
       </c>
+      <c r="AQ326">
+        <v>0</v>
+      </c>
     </row>
-    <row r="327" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>355</v>
       </c>
@@ -44380,8 +44773,11 @@
       <c r="AP327">
         <v>0</v>
       </c>
+      <c r="AQ327">
+        <v>0</v>
+      </c>
     </row>
-    <row r="328" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>356</v>
       </c>
@@ -44508,8 +44904,11 @@
       <c r="AP328" t="s">
         <v>308</v>
       </c>
+      <c r="AQ328" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="329" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>357</v>
       </c>
@@ -44633,8 +45032,11 @@
       <c r="AP329">
         <v>0</v>
       </c>
+      <c r="AQ329">
+        <v>0</v>
+      </c>
     </row>
-    <row r="330" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>358</v>
       </c>
@@ -44761,8 +45163,11 @@
       <c r="AP330" t="s">
         <v>308</v>
       </c>
+      <c r="AQ330" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="331" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>359</v>
       </c>
@@ -44886,8 +45291,11 @@
       <c r="AP331" t="s">
         <v>308</v>
       </c>
+      <c r="AQ331" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="332" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>360</v>
       </c>
@@ -45012,7 +45420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>361</v>
       </c>
@@ -45137,7 +45545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>362</v>
       </c>
@@ -45265,7 +45673,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="335" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>363</v>
       </c>
@@ -45393,7 +45801,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="336" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>364</v>
       </c>

</xml_diff>

<commit_message>
senescence and budset cc
</commit_message>
<xml_diff>
--- a/data/monitoring_phenology/2024_budburst_to_budset.xlsx
+++ b/data/monitoring_phenology/2024_budburst_to_budset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/data/monitoring_phenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAE0FA8-0D02-0047-A25C-812DAE4F0E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5871E1-4B64-384A-A44E-BA57010A4721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phenological_monitoring" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5420" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5449" uniqueCount="746">
   <si>
     <t>tree_ID</t>
   </si>
@@ -2273,6 +2273,9 @@
   <si>
     <t>doy276: seems like it flushed and starts to set bud again</t>
   </si>
+  <si>
+    <t>doy290: bud broken</t>
+  </si>
 </sst>
 </file>
 
@@ -3537,9 +3540,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A537" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AR272" sqref="AR272"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AQ137" sqref="AQ137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7661,6 +7664,9 @@
       <c r="AP32">
         <v>6</v>
       </c>
+      <c r="AQ32">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -7786,6 +7792,9 @@
       <c r="AP33">
         <v>6</v>
       </c>
+      <c r="AQ33">
+        <v>6</v>
+      </c>
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -7911,6 +7920,9 @@
       <c r="AP34">
         <v>5</v>
       </c>
+      <c r="AQ34">
+        <v>6</v>
+      </c>
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -8036,6 +8048,9 @@
       <c r="AP35">
         <v>6</v>
       </c>
+      <c r="AQ35">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -8161,6 +8176,9 @@
       <c r="AP36">
         <v>6</v>
       </c>
+      <c r="AQ36">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -8286,6 +8304,9 @@
       <c r="AP37">
         <v>6</v>
       </c>
+      <c r="AQ37">
+        <v>6</v>
+      </c>
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -8411,6 +8432,9 @@
       <c r="AP38">
         <v>6</v>
       </c>
+      <c r="AQ38">
+        <v>6</v>
+      </c>
     </row>
     <row r="39" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -8536,6 +8560,9 @@
       <c r="AP39">
         <v>6</v>
       </c>
+      <c r="AQ39">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -8661,6 +8688,9 @@
       <c r="AP40">
         <v>6</v>
       </c>
+      <c r="AQ40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -8786,6 +8816,9 @@
       <c r="AP41">
         <v>0</v>
       </c>
+      <c r="AQ41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -8914,6 +8947,9 @@
       <c r="AP42">
         <v>6</v>
       </c>
+      <c r="AQ42">
+        <v>6</v>
+      </c>
     </row>
     <row r="43" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -9039,6 +9075,9 @@
       <c r="AP43">
         <v>6</v>
       </c>
+      <c r="AQ43">
+        <v>6</v>
+      </c>
     </row>
     <row r="44" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -9164,6 +9203,9 @@
       <c r="AP44">
         <v>6</v>
       </c>
+      <c r="AQ44">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -9289,6 +9331,9 @@
       <c r="AP45">
         <v>6</v>
       </c>
+      <c r="AQ45">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -9414,6 +9459,9 @@
       <c r="AP46">
         <v>6</v>
       </c>
+      <c r="AQ46">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -11468,6 +11516,9 @@
       <c r="AP62">
         <v>6</v>
       </c>
+      <c r="AQ62">
+        <v>6</v>
+      </c>
     </row>
     <row r="63" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
@@ -11593,6 +11644,9 @@
       <c r="AP63">
         <v>6</v>
       </c>
+      <c r="AQ63">
+        <v>6</v>
+      </c>
     </row>
     <row r="64" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
@@ -11718,8 +11772,11 @@
       <c r="AP64">
         <v>6</v>
       </c>
+      <c r="AQ64">
+        <v>6</v>
+      </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -11843,8 +11900,11 @@
       <c r="AP65">
         <v>0</v>
       </c>
+      <c r="AQ65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -11968,8 +12028,11 @@
       <c r="AP66">
         <v>5</v>
       </c>
+      <c r="AQ66">
+        <v>6</v>
+      </c>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -12093,8 +12156,11 @@
       <c r="AP67">
         <v>6</v>
       </c>
+      <c r="AQ67">
+        <v>6</v>
+      </c>
     </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -12218,8 +12284,11 @@
       <c r="AP68">
         <v>6</v>
       </c>
+      <c r="AQ68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>81</v>
       </c>
@@ -12343,8 +12412,11 @@
       <c r="AP69">
         <v>0</v>
       </c>
+      <c r="AQ69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -12468,8 +12540,11 @@
       <c r="AP70">
         <v>6</v>
       </c>
+      <c r="AQ70">
+        <v>6</v>
+      </c>
     </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -12596,8 +12671,11 @@
       <c r="AP71" t="s">
         <v>308</v>
       </c>
+      <c r="AQ71" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>84</v>
       </c>
@@ -12721,8 +12799,11 @@
       <c r="AP72">
         <v>6</v>
       </c>
+      <c r="AQ72">
+        <v>6</v>
+      </c>
     </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -12846,8 +12927,11 @@
       <c r="AP73">
         <v>0</v>
       </c>
+      <c r="AQ73">
+        <v>0</v>
+      </c>
     </row>
-    <row r="74" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>86</v>
       </c>
@@ -12971,8 +13055,11 @@
       <c r="AP74">
         <v>6</v>
       </c>
+      <c r="AQ74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -12988,6 +13075,9 @@
       <c r="E75" t="s">
         <v>9</v>
       </c>
+      <c r="F75" t="s">
+        <v>745</v>
+      </c>
       <c r="G75" t="s">
         <v>10</v>
       </c>
@@ -13096,8 +13186,11 @@
       <c r="AP75">
         <v>6</v>
       </c>
+      <c r="AQ75" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -13221,8 +13314,11 @@
       <c r="AP76">
         <v>0</v>
       </c>
+      <c r="AQ76">
+        <v>0</v>
+      </c>
     </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>89</v>
       </c>
@@ -13346,8 +13442,11 @@
       <c r="AP77">
         <v>0</v>
       </c>
+      <c r="AQ77">
+        <v>0</v>
+      </c>
     </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>91</v>
       </c>
@@ -13471,8 +13570,11 @@
       <c r="AP78" s="2">
         <v>6</v>
       </c>
+      <c r="AQ78" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>92</v>
       </c>
@@ -13596,8 +13698,11 @@
       <c r="AP79" s="2">
         <v>6</v>
       </c>
+      <c r="AQ79" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="80" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>93</v>
       </c>
@@ -13719,6 +13824,9 @@
         <v>6</v>
       </c>
       <c r="AP80" s="2">
+        <v>6</v>
+      </c>
+      <c r="AQ80" s="2">
         <v>6</v>
       </c>
     </row>
@@ -13846,6 +13954,9 @@
       <c r="AP81" s="2">
         <v>6</v>
       </c>
+      <c r="AQ81" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
@@ -13971,6 +14082,9 @@
       <c r="AP82" s="2">
         <v>6</v>
       </c>
+      <c r="AQ82" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="83" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
@@ -14096,6 +14210,9 @@
       <c r="AP83" s="2">
         <v>6</v>
       </c>
+      <c r="AQ83" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="84" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
@@ -14221,6 +14338,9 @@
       <c r="AP84" s="2">
         <v>6</v>
       </c>
+      <c r="AQ84" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
@@ -14346,6 +14466,9 @@
       <c r="AP85" s="2">
         <v>6</v>
       </c>
+      <c r="AQ85" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="86" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
@@ -14471,6 +14594,9 @@
       <c r="AP86" s="2">
         <v>6</v>
       </c>
+      <c r="AQ86" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="87" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
@@ -14596,6 +14722,9 @@
       <c r="AP87" s="2">
         <v>6</v>
       </c>
+      <c r="AQ87" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="88" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
@@ -14721,6 +14850,9 @@
       <c r="AP88" s="2">
         <v>6</v>
       </c>
+      <c r="AQ88" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="89" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
@@ -14846,6 +14978,9 @@
       <c r="AP89" s="2">
         <v>6</v>
       </c>
+      <c r="AQ89" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
@@ -14971,6 +15106,9 @@
       <c r="AP90" s="2">
         <v>6</v>
       </c>
+      <c r="AQ90" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="91" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
@@ -15096,6 +15234,9 @@
       <c r="AP91" s="2">
         <v>6</v>
       </c>
+      <c r="AQ91" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="92" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
@@ -19073,6 +19214,9 @@
       <c r="AP122">
         <v>0</v>
       </c>
+      <c r="AQ122" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
@@ -19198,6 +19342,9 @@
       <c r="AP123">
         <v>0</v>
       </c>
+      <c r="AQ123" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
@@ -19323,6 +19470,9 @@
       <c r="AP124">
         <v>0</v>
       </c>
+      <c r="AQ124" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
@@ -19448,6 +19598,9 @@
       <c r="AP125">
         <v>6</v>
       </c>
+      <c r="AQ125" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="126" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
@@ -19573,6 +19726,9 @@
       <c r="AP126">
         <v>6</v>
       </c>
+      <c r="AQ126" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="127" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
@@ -19698,6 +19854,9 @@
       <c r="AP127">
         <v>6</v>
       </c>
+      <c r="AQ127" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
@@ -19823,6 +19982,9 @@
       <c r="AP128">
         <v>6</v>
       </c>
+      <c r="AQ128" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="129" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
@@ -19948,6 +20110,9 @@
       <c r="AP129">
         <v>0</v>
       </c>
+      <c r="AQ129" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="130" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
@@ -20073,6 +20238,9 @@
       <c r="AP130">
         <v>6</v>
       </c>
+      <c r="AQ130" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
@@ -20201,6 +20369,9 @@
       <c r="AP131" t="s">
         <v>308</v>
       </c>
+      <c r="AQ131" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="132" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
@@ -20326,6 +20497,9 @@
       <c r="AP132">
         <v>0</v>
       </c>
+      <c r="AQ132" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
@@ -20451,6 +20625,9 @@
       <c r="AP133">
         <v>6</v>
       </c>
+      <c r="AQ133" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="134" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
@@ -20576,6 +20753,9 @@
       <c r="AP134">
         <v>6</v>
       </c>
+      <c r="AQ134" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="135" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
@@ -20701,6 +20881,9 @@
       <c r="AP135">
         <v>0</v>
       </c>
+      <c r="AQ135" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
@@ -20826,6 +21009,9 @@
       <c r="AP136">
         <v>6</v>
       </c>
+      <c r="AQ136" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="137" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
@@ -25887,7 +26073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>193</v>
       </c>
@@ -26012,7 +26198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>194</v>
       </c>
@@ -26137,7 +26323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>195</v>
       </c>
@@ -26262,7 +26448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>196</v>
       </c>
@@ -26387,7 +26573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>197</v>
       </c>
@@ -26512,7 +26698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>198</v>
       </c>
@@ -26634,8 +26820,11 @@
       <c r="AP182">
         <v>0</v>
       </c>
+      <c r="AQ182">
+        <v>0</v>
+      </c>
     </row>
-    <row r="183" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>201</v>
       </c>
@@ -26757,8 +26946,11 @@
       <c r="AP183">
         <v>0</v>
       </c>
+      <c r="AQ183">
+        <v>0</v>
+      </c>
     </row>
-    <row r="184" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>202</v>
       </c>
@@ -26880,8 +27072,11 @@
       <c r="AP184">
         <v>0</v>
       </c>
+      <c r="AQ184">
+        <v>0</v>
+      </c>
     </row>
-    <row r="185" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>203</v>
       </c>
@@ -27003,8 +27198,11 @@
       <c r="AP185">
         <v>0</v>
       </c>
+      <c r="AQ185">
+        <v>0</v>
+      </c>
     </row>
-    <row r="186" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>204</v>
       </c>
@@ -27129,8 +27327,11 @@
       <c r="AP186">
         <v>0</v>
       </c>
+      <c r="AQ186">
+        <v>0</v>
+      </c>
     </row>
-    <row r="187" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>206</v>
       </c>
@@ -27252,8 +27453,11 @@
       <c r="AP187">
         <v>0</v>
       </c>
+      <c r="AQ187">
+        <v>0</v>
+      </c>
     </row>
-    <row r="188" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>207</v>
       </c>
@@ -27375,8 +27579,11 @@
       <c r="AP188">
         <v>0</v>
       </c>
+      <c r="AQ188">
+        <v>0</v>
+      </c>
     </row>
-    <row r="189" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>208</v>
       </c>
@@ -27498,8 +27705,11 @@
       <c r="AP189">
         <v>0</v>
       </c>
+      <c r="AQ189">
+        <v>0</v>
+      </c>
     </row>
-    <row r="190" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>209</v>
       </c>
@@ -27624,8 +27834,11 @@
       <c r="AP190">
         <v>0</v>
       </c>
+      <c r="AQ190">
+        <v>0</v>
+      </c>
     </row>
-    <row r="191" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>210</v>
       </c>
@@ -27747,8 +27960,11 @@
       <c r="AP191">
         <v>0</v>
       </c>
+      <c r="AQ191">
+        <v>0</v>
+      </c>
     </row>
-    <row r="192" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>211</v>
       </c>
@@ -27870,8 +28086,11 @@
       <c r="AP192">
         <v>0</v>
       </c>
+      <c r="AQ192">
+        <v>0</v>
+      </c>
     </row>
-    <row r="193" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>212</v>
       </c>
@@ -27993,8 +28212,11 @@
       <c r="AP193">
         <v>0</v>
       </c>
+      <c r="AQ193">
+        <v>0</v>
+      </c>
     </row>
-    <row r="194" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>213</v>
       </c>
@@ -28119,8 +28341,11 @@
       <c r="AP194">
         <v>0</v>
       </c>
+      <c r="AQ194">
+        <v>0</v>
+      </c>
     </row>
-    <row r="195" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>215</v>
       </c>
@@ -28242,8 +28467,11 @@
       <c r="AP195">
         <v>0</v>
       </c>
+      <c r="AQ195">
+        <v>0</v>
+      </c>
     </row>
-    <row r="196" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>216</v>
       </c>
@@ -28365,8 +28593,11 @@
       <c r="AP196">
         <v>0</v>
       </c>
+      <c r="AQ196">
+        <v>0</v>
+      </c>
     </row>
-    <row r="197" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>217</v>
       </c>
@@ -28488,8 +28719,11 @@
       <c r="AP197">
         <v>0</v>
       </c>
+      <c r="AQ197">
+        <v>0</v>
+      </c>
     </row>
-    <row r="198" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>218</v>
       </c>
@@ -28614,8 +28848,11 @@
       <c r="AP198">
         <v>0</v>
       </c>
+      <c r="AQ198">
+        <v>0</v>
+      </c>
     </row>
-    <row r="199" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>220</v>
       </c>
@@ -28737,8 +28974,11 @@
       <c r="AP199">
         <v>0</v>
       </c>
+      <c r="AQ199">
+        <v>0</v>
+      </c>
     </row>
-    <row r="200" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>221</v>
       </c>
@@ -28863,8 +29103,11 @@
       <c r="AP200">
         <v>0</v>
       </c>
+      <c r="AQ200">
+        <v>0</v>
+      </c>
     </row>
-    <row r="201" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>222</v>
       </c>
@@ -28986,8 +29229,11 @@
       <c r="AP201">
         <v>0</v>
       </c>
+      <c r="AQ201">
+        <v>0</v>
+      </c>
     </row>
-    <row r="202" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>223</v>
       </c>
@@ -29109,8 +29355,11 @@
       <c r="AP202">
         <v>0</v>
       </c>
+      <c r="AQ202">
+        <v>0</v>
+      </c>
     </row>
-    <row r="203" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>224</v>
       </c>
@@ -29232,8 +29481,11 @@
       <c r="AP203">
         <v>0</v>
       </c>
+      <c r="AQ203">
+        <v>0</v>
+      </c>
     </row>
-    <row r="204" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>225</v>
       </c>
@@ -29355,8 +29607,11 @@
       <c r="AP204">
         <v>0</v>
       </c>
+      <c r="AQ204">
+        <v>0</v>
+      </c>
     </row>
-    <row r="205" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>226</v>
       </c>
@@ -29481,8 +29736,11 @@
       <c r="AP205">
         <v>0</v>
       </c>
+      <c r="AQ205">
+        <v>0</v>
+      </c>
     </row>
-    <row r="206" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>227</v>
       </c>
@@ -29604,8 +29862,11 @@
       <c r="AP206">
         <v>0</v>
       </c>
+      <c r="AQ206">
+        <v>0</v>
+      </c>
     </row>
-    <row r="207" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>228</v>
       </c>
@@ -29727,8 +29988,11 @@
       <c r="AP207">
         <v>0</v>
       </c>
+      <c r="AQ207">
+        <v>0</v>
+      </c>
     </row>
-    <row r="208" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>229</v>
       </c>
@@ -29853,8 +30117,11 @@
       <c r="AP208">
         <v>0</v>
       </c>
+      <c r="AQ208">
+        <v>0</v>
+      </c>
     </row>
-    <row r="209" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>230</v>
       </c>
@@ -29976,8 +30243,11 @@
       <c r="AP209">
         <v>0</v>
       </c>
+      <c r="AQ209">
+        <v>0</v>
+      </c>
     </row>
-    <row r="210" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>231</v>
       </c>
@@ -30099,8 +30369,11 @@
       <c r="AP210">
         <v>0</v>
       </c>
+      <c r="AQ210">
+        <v>0</v>
+      </c>
     </row>
-    <row r="211" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>232</v>
       </c>
@@ -30225,8 +30498,11 @@
       <c r="AP211">
         <v>0</v>
       </c>
+      <c r="AQ211">
+        <v>0</v>
+      </c>
     </row>
-    <row r="212" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>233</v>
       </c>
@@ -30348,8 +30624,11 @@
       <c r="AP212">
         <v>0</v>
       </c>
+      <c r="AQ212">
+        <v>0</v>
+      </c>
     </row>
-    <row r="213" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>234</v>
       </c>
@@ -30471,8 +30750,11 @@
       <c r="AP213">
         <v>0</v>
       </c>
+      <c r="AQ213">
+        <v>0</v>
+      </c>
     </row>
-    <row r="214" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>235</v>
       </c>
@@ -30594,8 +30876,11 @@
       <c r="AP214">
         <v>0</v>
       </c>
+      <c r="AQ214">
+        <v>0</v>
+      </c>
     </row>
-    <row r="215" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>236</v>
       </c>
@@ -30717,8 +31002,11 @@
       <c r="AP215">
         <v>0</v>
       </c>
+      <c r="AQ215">
+        <v>0</v>
+      </c>
     </row>
-    <row r="216" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>237</v>
       </c>
@@ -30843,8 +31131,11 @@
       <c r="AP216">
         <v>0</v>
       </c>
+      <c r="AQ216">
+        <v>0</v>
+      </c>
     </row>
-    <row r="217" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>238</v>
       </c>
@@ -30966,8 +31257,11 @@
       <c r="AP217">
         <v>0</v>
       </c>
+      <c r="AQ217">
+        <v>0</v>
+      </c>
     </row>
-    <row r="218" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>239</v>
       </c>
@@ -31089,8 +31383,11 @@
       <c r="AP218">
         <v>0</v>
       </c>
+      <c r="AQ218">
+        <v>0</v>
+      </c>
     </row>
-    <row r="219" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>240</v>
       </c>
@@ -31212,8 +31509,11 @@
       <c r="AP219">
         <v>0</v>
       </c>
+      <c r="AQ219">
+        <v>0</v>
+      </c>
     </row>
-    <row r="220" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>241</v>
       </c>
@@ -31335,8 +31635,11 @@
       <c r="AP220">
         <v>0</v>
       </c>
+      <c r="AQ220">
+        <v>0</v>
+      </c>
     </row>
-    <row r="221" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>242</v>
       </c>
@@ -31458,8 +31761,11 @@
       <c r="AP221" t="s">
         <v>308</v>
       </c>
+      <c r="AQ221" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="222" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>243</v>
       </c>
@@ -31581,8 +31887,11 @@
       <c r="AP222">
         <v>0</v>
       </c>
+      <c r="AQ222">
+        <v>0</v>
+      </c>
     </row>
-    <row r="223" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>244</v>
       </c>
@@ -31707,8 +32016,11 @@
       <c r="AP223">
         <v>0</v>
       </c>
+      <c r="AQ223">
+        <v>0</v>
+      </c>
     </row>
-    <row r="224" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>245</v>
       </c>
@@ -31830,8 +32142,11 @@
       <c r="AP224">
         <v>0</v>
       </c>
+      <c r="AQ224">
+        <v>0</v>
+      </c>
     </row>
-    <row r="225" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>246</v>
       </c>
@@ -31956,8 +32271,11 @@
       <c r="AP225">
         <v>0</v>
       </c>
+      <c r="AQ225">
+        <v>0</v>
+      </c>
     </row>
-    <row r="226" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>247</v>
       </c>
@@ -32079,8 +32397,11 @@
       <c r="AP226">
         <v>0</v>
       </c>
+      <c r="AQ226">
+        <v>0</v>
+      </c>
     </row>
-    <row r="227" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>248</v>
       </c>
@@ -32202,8 +32523,11 @@
       <c r="AP227">
         <v>0</v>
       </c>
+      <c r="AQ227">
+        <v>0</v>
+      </c>
     </row>
-    <row r="228" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>249</v>
       </c>
@@ -32325,8 +32649,11 @@
       <c r="AP228">
         <v>0</v>
       </c>
+      <c r="AQ228">
+        <v>0</v>
+      </c>
     </row>
-    <row r="229" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>250</v>
       </c>
@@ -32448,8 +32775,11 @@
       <c r="AP229">
         <v>0</v>
       </c>
+      <c r="AQ229">
+        <v>0</v>
+      </c>
     </row>
-    <row r="230" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>251</v>
       </c>
@@ -32571,8 +32901,11 @@
       <c r="AP230">
         <v>0</v>
       </c>
+      <c r="AQ230">
+        <v>0</v>
+      </c>
     </row>
-    <row r="231" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>252</v>
       </c>
@@ -32694,8 +33027,11 @@
       <c r="AP231">
         <v>0</v>
       </c>
+      <c r="AQ231">
+        <v>0</v>
+      </c>
     </row>
-    <row r="232" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>253</v>
       </c>
@@ -32817,8 +33153,11 @@
       <c r="AP232">
         <v>0</v>
       </c>
+      <c r="AQ232">
+        <v>0</v>
+      </c>
     </row>
-    <row r="233" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>254</v>
       </c>
@@ -32940,8 +33279,11 @@
       <c r="AP233">
         <v>0</v>
       </c>
+      <c r="AQ233">
+        <v>0</v>
+      </c>
     </row>
-    <row r="234" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>255</v>
       </c>
@@ -33063,8 +33405,11 @@
       <c r="AP234">
         <v>0</v>
       </c>
+      <c r="AQ234">
+        <v>0</v>
+      </c>
     </row>
-    <row r="235" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>256</v>
       </c>
@@ -33186,8 +33531,11 @@
       <c r="AP235">
         <v>0</v>
       </c>
+      <c r="AQ235">
+        <v>0</v>
+      </c>
     </row>
-    <row r="236" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>257</v>
       </c>
@@ -33309,8 +33657,11 @@
       <c r="AP236">
         <v>0</v>
       </c>
+      <c r="AQ236">
+        <v>0</v>
+      </c>
     </row>
-    <row r="237" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>258</v>
       </c>
@@ -33432,8 +33783,11 @@
       <c r="AP237">
         <v>0</v>
       </c>
+      <c r="AQ237">
+        <v>0</v>
+      </c>
     </row>
-    <row r="238" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>259</v>
       </c>
@@ -33555,8 +33909,11 @@
       <c r="AP238">
         <v>0</v>
       </c>
+      <c r="AQ238">
+        <v>0</v>
+      </c>
     </row>
-    <row r="239" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>260</v>
       </c>
@@ -33678,8 +34035,11 @@
       <c r="AP239">
         <v>0</v>
       </c>
+      <c r="AQ239">
+        <v>0</v>
+      </c>
     </row>
-    <row r="240" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>261</v>
       </c>
@@ -33801,8 +34161,11 @@
       <c r="AP240">
         <v>0</v>
       </c>
+      <c r="AQ240">
+        <v>0</v>
+      </c>
     </row>
-    <row r="241" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>262</v>
       </c>
@@ -33924,8 +34287,11 @@
       <c r="AP241">
         <v>0</v>
       </c>
+      <c r="AQ241">
+        <v>0</v>
+      </c>
     </row>
-    <row r="242" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>263</v>
       </c>
@@ -34047,8 +34413,11 @@
       <c r="AP242">
         <v>0</v>
       </c>
+      <c r="AQ242">
+        <v>0</v>
+      </c>
     </row>
-    <row r="243" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>264</v>
       </c>
@@ -34170,8 +34539,11 @@
       <c r="AP243">
         <v>0</v>
       </c>
+      <c r="AQ243">
+        <v>0</v>
+      </c>
     </row>
-    <row r="244" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>265</v>
       </c>
@@ -34293,8 +34665,11 @@
       <c r="AP244">
         <v>0</v>
       </c>
+      <c r="AQ244">
+        <v>0</v>
+      </c>
     </row>
-    <row r="245" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>266</v>
       </c>
@@ -34416,8 +34791,11 @@
       <c r="AP245">
         <v>0</v>
       </c>
+      <c r="AQ245">
+        <v>0</v>
+      </c>
     </row>
-    <row r="246" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>267</v>
       </c>
@@ -34539,8 +34917,11 @@
       <c r="AP246">
         <v>0</v>
       </c>
+      <c r="AQ246">
+        <v>0</v>
+      </c>
     </row>
-    <row r="247" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>268</v>
       </c>
@@ -34662,8 +35043,11 @@
       <c r="AP247">
         <v>0</v>
       </c>
+      <c r="AQ247">
+        <v>0</v>
+      </c>
     </row>
-    <row r="248" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>269</v>
       </c>
@@ -34785,8 +35169,11 @@
       <c r="AP248">
         <v>0</v>
       </c>
+      <c r="AQ248">
+        <v>0</v>
+      </c>
     </row>
-    <row r="249" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>270</v>
       </c>
@@ -34908,8 +35295,11 @@
       <c r="AP249">
         <v>0</v>
       </c>
+      <c r="AQ249">
+        <v>0</v>
+      </c>
     </row>
-    <row r="250" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>271</v>
       </c>
@@ -35031,8 +35421,11 @@
       <c r="AP250">
         <v>0</v>
       </c>
+      <c r="AQ250">
+        <v>0</v>
+      </c>
     </row>
-    <row r="251" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>272</v>
       </c>
@@ -35154,8 +35547,11 @@
       <c r="AP251">
         <v>0</v>
       </c>
+      <c r="AQ251">
+        <v>0</v>
+      </c>
     </row>
-    <row r="252" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>273</v>
       </c>
@@ -35277,8 +35673,11 @@
       <c r="AP252">
         <v>0</v>
       </c>
+      <c r="AQ252">
+        <v>0</v>
+      </c>
     </row>
-    <row r="253" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>274</v>
       </c>
@@ -35400,8 +35799,11 @@
       <c r="AP253">
         <v>0</v>
       </c>
+      <c r="AQ253">
+        <v>0</v>
+      </c>
     </row>
-    <row r="254" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>275</v>
       </c>
@@ -35523,8 +35925,11 @@
       <c r="AP254">
         <v>0</v>
       </c>
+      <c r="AQ254">
+        <v>0</v>
+      </c>
     </row>
-    <row r="255" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>276</v>
       </c>
@@ -35646,8 +36051,11 @@
       <c r="AP255">
         <v>0</v>
       </c>
+      <c r="AQ255">
+        <v>0</v>
+      </c>
     </row>
-    <row r="256" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>277</v>
       </c>
@@ -35767,6 +36175,9 @@
         <v>0</v>
       </c>
       <c r="AP256">
+        <v>0</v>
+      </c>
+      <c r="AQ256">
         <v>0</v>
       </c>
     </row>
@@ -35892,6 +36303,9 @@
       <c r="AP257">
         <v>0</v>
       </c>
+      <c r="AQ257">
+        <v>0</v>
+      </c>
     </row>
     <row r="258" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
@@ -36015,6 +36429,9 @@
       <c r="AP258">
         <v>0</v>
       </c>
+      <c r="AQ258">
+        <v>0</v>
+      </c>
     </row>
     <row r="259" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
@@ -36138,6 +36555,9 @@
       <c r="AP259">
         <v>0</v>
       </c>
+      <c r="AQ259">
+        <v>0</v>
+      </c>
     </row>
     <row r="260" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
@@ -36261,6 +36681,9 @@
       <c r="AP260">
         <v>0</v>
       </c>
+      <c r="AQ260">
+        <v>0</v>
+      </c>
     </row>
     <row r="261" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
@@ -36384,6 +36807,9 @@
       <c r="AP261">
         <v>0</v>
       </c>
+      <c r="AQ261">
+        <v>0</v>
+      </c>
     </row>
     <row r="262" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
@@ -36507,6 +36933,9 @@
       <c r="AP262">
         <v>0</v>
       </c>
+      <c r="AQ262">
+        <v>0</v>
+      </c>
     </row>
     <row r="263" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
@@ -36630,6 +37059,9 @@
       <c r="AP263">
         <v>0</v>
       </c>
+      <c r="AQ263">
+        <v>0</v>
+      </c>
     </row>
     <row r="264" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
@@ -36753,6 +37185,9 @@
       <c r="AP264">
         <v>0</v>
       </c>
+      <c r="AQ264">
+        <v>0</v>
+      </c>
     </row>
     <row r="265" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
@@ -36876,6 +37311,9 @@
       <c r="AP265">
         <v>0</v>
       </c>
+      <c r="AQ265">
+        <v>0</v>
+      </c>
     </row>
     <row r="266" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
@@ -36999,6 +37437,9 @@
       <c r="AP266">
         <v>0</v>
       </c>
+      <c r="AQ266">
+        <v>0</v>
+      </c>
     </row>
     <row r="267" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
@@ -37122,6 +37563,9 @@
       <c r="AP267">
         <v>0</v>
       </c>
+      <c r="AQ267">
+        <v>0</v>
+      </c>
     </row>
     <row r="268" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
@@ -37245,6 +37689,9 @@
       <c r="AP268">
         <v>0</v>
       </c>
+      <c r="AQ268">
+        <v>0</v>
+      </c>
     </row>
     <row r="269" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
@@ -37368,6 +37815,9 @@
       <c r="AP269">
         <v>0</v>
       </c>
+      <c r="AQ269">
+        <v>0</v>
+      </c>
     </row>
     <row r="270" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
@@ -37491,6 +37941,9 @@
       <c r="AP270">
         <v>0</v>
       </c>
+      <c r="AQ270">
+        <v>0</v>
+      </c>
     </row>
     <row r="271" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
@@ -37614,6 +38067,9 @@
       <c r="AP271">
         <v>0</v>
       </c>
+      <c r="AQ271">
+        <v>0</v>
+      </c>
     </row>
     <row r="272" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
@@ -41606,6 +42062,9 @@
       <c r="AP302">
         <v>0</v>
       </c>
+      <c r="AQ302">
+        <v>0</v>
+      </c>
     </row>
     <row r="303" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
@@ -41731,6 +42190,9 @@
       <c r="AP303">
         <v>0</v>
       </c>
+      <c r="AQ303">
+        <v>0</v>
+      </c>
     </row>
     <row r="304" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
@@ -41856,6 +42318,9 @@
       <c r="AP304">
         <v>0</v>
       </c>
+      <c r="AQ304">
+        <v>0</v>
+      </c>
     </row>
     <row r="305" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
@@ -41981,6 +42446,9 @@
       <c r="AP305">
         <v>0</v>
       </c>
+      <c r="AQ305">
+        <v>0</v>
+      </c>
     </row>
     <row r="306" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
@@ -42106,6 +42574,9 @@
       <c r="AP306">
         <v>0</v>
       </c>
+      <c r="AQ306">
+        <v>0</v>
+      </c>
     </row>
     <row r="307" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
@@ -42231,6 +42702,9 @@
       <c r="AP307">
         <v>0</v>
       </c>
+      <c r="AQ307">
+        <v>0</v>
+      </c>
     </row>
     <row r="308" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
@@ -42356,6 +42830,9 @@
       <c r="AP308">
         <v>0</v>
       </c>
+      <c r="AQ308">
+        <v>0</v>
+      </c>
     </row>
     <row r="309" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
@@ -42481,6 +42958,9 @@
       <c r="AP309">
         <v>0</v>
       </c>
+      <c r="AQ309">
+        <v>0</v>
+      </c>
     </row>
     <row r="310" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
@@ -42606,6 +43086,9 @@
       <c r="AP310">
         <v>0</v>
       </c>
+      <c r="AQ310">
+        <v>0</v>
+      </c>
     </row>
     <row r="311" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
@@ -42731,6 +43214,9 @@
       <c r="AP311">
         <v>0</v>
       </c>
+      <c r="AQ311">
+        <v>0</v>
+      </c>
     </row>
     <row r="312" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
@@ -42856,6 +43342,9 @@
       <c r="AP312">
         <v>0</v>
       </c>
+      <c r="AQ312">
+        <v>0</v>
+      </c>
     </row>
     <row r="313" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
@@ -42981,6 +43470,9 @@
       <c r="AP313">
         <v>0</v>
       </c>
+      <c r="AQ313">
+        <v>0</v>
+      </c>
     </row>
     <row r="314" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
@@ -43106,6 +43598,9 @@
       <c r="AP314">
         <v>0</v>
       </c>
+      <c r="AQ314">
+        <v>0</v>
+      </c>
     </row>
     <row r="315" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
@@ -43231,6 +43726,9 @@
       <c r="AP315">
         <v>0</v>
       </c>
+      <c r="AQ315">
+        <v>0</v>
+      </c>
     </row>
     <row r="316" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
@@ -43359,6 +43857,9 @@
       <c r="AP316">
         <v>0</v>
       </c>
+      <c r="AQ316">
+        <v>0</v>
+      </c>
     </row>
     <row r="317" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
@@ -45419,6 +45920,9 @@
       <c r="AP332">
         <v>0</v>
       </c>
+      <c r="AQ332">
+        <v>0</v>
+      </c>
     </row>
     <row r="333" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
@@ -45544,6 +46048,9 @@
       <c r="AP333">
         <v>0</v>
       </c>
+      <c r="AQ333">
+        <v>0</v>
+      </c>
     </row>
     <row r="334" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
@@ -45672,6 +46179,9 @@
       <c r="AP334" t="s">
         <v>308</v>
       </c>
+      <c r="AQ334" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="335" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
@@ -45800,6 +46310,9 @@
       <c r="AP335" t="s">
         <v>308</v>
       </c>
+      <c r="AQ335" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="336" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
@@ -45925,8 +46438,11 @@
       <c r="AP336">
         <v>0</v>
       </c>
+      <c r="AQ336">
+        <v>0</v>
+      </c>
     </row>
-    <row r="337" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>365</v>
       </c>
@@ -46053,8 +46569,11 @@
       <c r="AP337" t="s">
         <v>308</v>
       </c>
+      <c r="AQ337" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="338" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>366</v>
       </c>
@@ -46178,8 +46697,11 @@
       <c r="AP338">
         <v>0</v>
       </c>
+      <c r="AQ338">
+        <v>0</v>
+      </c>
     </row>
-    <row r="339" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>367</v>
       </c>
@@ -46303,8 +46825,11 @@
       <c r="AP339">
         <v>0</v>
       </c>
+      <c r="AQ339">
+        <v>0</v>
+      </c>
     </row>
-    <row r="340" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>368</v>
       </c>
@@ -46428,8 +46953,11 @@
       <c r="AP340">
         <v>0</v>
       </c>
+      <c r="AQ340">
+        <v>0</v>
+      </c>
     </row>
-    <row r="341" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>369</v>
       </c>
@@ -46553,8 +47081,11 @@
       <c r="AP341">
         <v>0</v>
       </c>
+      <c r="AQ341">
+        <v>0</v>
+      </c>
     </row>
-    <row r="342" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>370</v>
       </c>
@@ -46681,8 +47212,11 @@
       <c r="AP342" t="s">
         <v>308</v>
       </c>
+      <c r="AQ342" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="343" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>371</v>
       </c>
@@ -46809,8 +47343,11 @@
       <c r="AP343" t="s">
         <v>308</v>
       </c>
+      <c r="AQ343" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="344" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>372</v>
       </c>
@@ -46937,8 +47474,11 @@
       <c r="AP344">
         <v>0</v>
       </c>
+      <c r="AQ344">
+        <v>0</v>
+      </c>
     </row>
-    <row r="345" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>373</v>
       </c>
@@ -47062,8 +47602,11 @@
       <c r="AP345" t="s">
         <v>308</v>
       </c>
+      <c r="AQ345" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="346" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>374</v>
       </c>
@@ -47187,8 +47730,11 @@
       <c r="AP346">
         <v>0</v>
       </c>
+      <c r="AQ346">
+        <v>0</v>
+      </c>
     </row>
-    <row r="347" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>375</v>
       </c>
@@ -47312,8 +47858,11 @@
       <c r="AP347">
         <v>6</v>
       </c>
+      <c r="AQ347">
+        <v>6</v>
+      </c>
     </row>
-    <row r="348" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>376</v>
       </c>
@@ -47440,8 +47989,11 @@
       <c r="AP348">
         <v>6</v>
       </c>
+      <c r="AQ348">
+        <v>6</v>
+      </c>
     </row>
-    <row r="349" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>377</v>
       </c>
@@ -47565,8 +48117,11 @@
       <c r="AP349">
         <v>0</v>
       </c>
+      <c r="AQ349">
+        <v>0</v>
+      </c>
     </row>
-    <row r="350" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>378</v>
       </c>
@@ -47690,8 +48245,11 @@
       <c r="AP350" t="s">
         <v>308</v>
       </c>
+      <c r="AQ350" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="351" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>379</v>
       </c>
@@ -47815,8 +48373,11 @@
       <c r="AP351">
         <v>0</v>
       </c>
+      <c r="AQ351">
+        <v>0</v>
+      </c>
     </row>
-    <row r="352" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>380</v>
       </c>
@@ -47943,8 +48504,11 @@
       <c r="AP352">
         <v>6</v>
       </c>
+      <c r="AQ352">
+        <v>0</v>
+      </c>
     </row>
-    <row r="353" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>381</v>
       </c>
@@ -48068,8 +48632,11 @@
       <c r="AP353">
         <v>6</v>
       </c>
+      <c r="AQ353">
+        <v>0</v>
+      </c>
     </row>
-    <row r="354" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>382</v>
       </c>
@@ -48193,8 +48760,11 @@
       <c r="AP354">
         <v>0</v>
       </c>
+      <c r="AQ354">
+        <v>0</v>
+      </c>
     </row>
-    <row r="355" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>383</v>
       </c>
@@ -48321,8 +48891,11 @@
       <c r="AP355" t="s">
         <v>308</v>
       </c>
+      <c r="AQ355" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="356" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>384</v>
       </c>
@@ -48446,8 +49019,11 @@
       <c r="AP356">
         <v>0</v>
       </c>
+      <c r="AQ356">
+        <v>0</v>
+      </c>
     </row>
-    <row r="357" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>385</v>
       </c>
@@ -48571,8 +49147,11 @@
       <c r="AP357">
         <v>0</v>
       </c>
+      <c r="AQ357">
+        <v>0</v>
+      </c>
     </row>
-    <row r="358" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>386</v>
       </c>
@@ -48696,8 +49275,11 @@
       <c r="AP358">
         <v>0</v>
       </c>
+      <c r="AQ358">
+        <v>0</v>
+      </c>
     </row>
-    <row r="359" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>387</v>
       </c>
@@ -48824,8 +49406,11 @@
       <c r="AP359" t="s">
         <v>308</v>
       </c>
+      <c r="AQ359" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="360" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>388</v>
       </c>
@@ -48949,8 +49534,11 @@
       <c r="AP360">
         <v>0</v>
       </c>
+      <c r="AQ360">
+        <v>0</v>
+      </c>
     </row>
-    <row r="361" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>389</v>
       </c>
@@ -49074,8 +49662,14 @@
       <c r="AO361">
         <v>5</v>
       </c>
+      <c r="AP361">
+        <v>6</v>
+      </c>
+      <c r="AQ361">
+        <v>6</v>
+      </c>
     </row>
-    <row r="362" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>390</v>
       </c>
@@ -49199,8 +49793,11 @@
       <c r="AP362">
         <v>0</v>
       </c>
+      <c r="AQ362">
+        <v>0</v>
+      </c>
     </row>
-    <row r="363" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>393</v>
       </c>
@@ -49324,8 +49921,11 @@
       <c r="AP363">
         <v>0</v>
       </c>
+      <c r="AQ363">
+        <v>0</v>
+      </c>
     </row>
-    <row r="364" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>394</v>
       </c>
@@ -49449,8 +50049,11 @@
       <c r="AP364">
         <v>0</v>
       </c>
+      <c r="AQ364">
+        <v>0</v>
+      </c>
     </row>
-    <row r="365" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>395</v>
       </c>
@@ -49574,8 +50177,11 @@
       <c r="AP365">
         <v>0</v>
       </c>
+      <c r="AQ365">
+        <v>0</v>
+      </c>
     </row>
-    <row r="366" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>396</v>
       </c>
@@ -49699,8 +50305,11 @@
       <c r="AP366">
         <v>0</v>
       </c>
+      <c r="AQ366">
+        <v>0</v>
+      </c>
     </row>
-    <row r="367" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>397</v>
       </c>
@@ -49824,8 +50433,11 @@
       <c r="AP367">
         <v>0</v>
       </c>
+      <c r="AQ367">
+        <v>0</v>
+      </c>
     </row>
-    <row r="368" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>398</v>
       </c>
@@ -49949,8 +50561,11 @@
       <c r="AP368">
         <v>0</v>
       </c>
+      <c r="AQ368">
+        <v>0</v>
+      </c>
     </row>
-    <row r="369" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>399</v>
       </c>
@@ -50077,8 +50692,11 @@
       <c r="AP369">
         <v>0</v>
       </c>
+      <c r="AQ369">
+        <v>0</v>
+      </c>
     </row>
-    <row r="370" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>400</v>
       </c>
@@ -50202,8 +50820,11 @@
       <c r="AP370">
         <v>0</v>
       </c>
+      <c r="AQ370">
+        <v>0</v>
+      </c>
     </row>
-    <row r="371" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>401</v>
       </c>
@@ -50327,8 +50948,11 @@
       <c r="AP371">
         <v>0</v>
       </c>
+      <c r="AQ371">
+        <v>0</v>
+      </c>
     </row>
-    <row r="372" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>402</v>
       </c>
@@ -50452,8 +51076,11 @@
       <c r="AP372">
         <v>0</v>
       </c>
+      <c r="AQ372">
+        <v>0</v>
+      </c>
     </row>
-    <row r="373" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>403</v>
       </c>
@@ -50580,8 +51207,11 @@
       <c r="AP373">
         <v>0</v>
       </c>
+      <c r="AQ373">
+        <v>0</v>
+      </c>
     </row>
-    <row r="374" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>404</v>
       </c>
@@ -50705,8 +51335,11 @@
       <c r="AP374">
         <v>0</v>
       </c>
+      <c r="AQ374">
+        <v>0</v>
+      </c>
     </row>
-    <row r="375" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>405</v>
       </c>
@@ -50830,8 +51463,11 @@
       <c r="AP375">
         <v>0</v>
       </c>
+      <c r="AQ375">
+        <v>0</v>
+      </c>
     </row>
-    <row r="376" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>406</v>
       </c>
@@ -50955,8 +51591,11 @@
       <c r="AP376">
         <v>0</v>
       </c>
+      <c r="AQ376">
+        <v>0</v>
+      </c>
     </row>
-    <row r="377" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>407</v>
       </c>
@@ -51080,8 +51719,11 @@
       <c r="AP377">
         <v>0</v>
       </c>
+      <c r="AQ377">
+        <v>0</v>
+      </c>
     </row>
-    <row r="378" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>408</v>
       </c>
@@ -51205,8 +51847,11 @@
       <c r="AP378">
         <v>0</v>
       </c>
+      <c r="AQ378">
+        <v>0</v>
+      </c>
     </row>
-    <row r="379" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>409</v>
       </c>
@@ -51330,8 +51975,11 @@
       <c r="AP379">
         <v>0</v>
       </c>
+      <c r="AQ379">
+        <v>0</v>
+      </c>
     </row>
-    <row r="380" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>410</v>
       </c>
@@ -51458,8 +52106,11 @@
       <c r="AP380">
         <v>0</v>
       </c>
+      <c r="AQ380">
+        <v>0</v>
+      </c>
     </row>
-    <row r="381" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>412</v>
       </c>
@@ -51583,8 +52234,11 @@
       <c r="AP381">
         <v>0</v>
       </c>
+      <c r="AQ381">
+        <v>0</v>
+      </c>
     </row>
-    <row r="382" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>413</v>
       </c>
@@ -51708,8 +52362,11 @@
       <c r="AP382">
         <v>0</v>
       </c>
+      <c r="AQ382">
+        <v>0</v>
+      </c>
     </row>
-    <row r="383" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>414</v>
       </c>
@@ -51833,8 +52490,11 @@
       <c r="AP383">
         <v>0</v>
       </c>
+      <c r="AQ383">
+        <v>0</v>
+      </c>
     </row>
-    <row r="384" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>415</v>
       </c>
@@ -51958,8 +52618,11 @@
       <c r="AP384">
         <v>0</v>
       </c>
+      <c r="AQ384">
+        <v>0</v>
+      </c>
     </row>
-    <row r="385" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>416</v>
       </c>
@@ -52083,8 +52746,11 @@
       <c r="AP385">
         <v>0</v>
       </c>
+      <c r="AQ385">
+        <v>0</v>
+      </c>
     </row>
-    <row r="386" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>417</v>
       </c>
@@ -52211,8 +52877,11 @@
       <c r="AP386">
         <v>0</v>
       </c>
+      <c r="AQ386">
+        <v>0</v>
+      </c>
     </row>
-    <row r="387" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>418</v>
       </c>
@@ -52336,8 +53005,11 @@
       <c r="AP387" t="s">
         <v>308</v>
       </c>
+      <c r="AQ387" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="388" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>419</v>
       </c>
@@ -52461,8 +53133,11 @@
       <c r="AP388">
         <v>0</v>
       </c>
+      <c r="AQ388">
+        <v>0</v>
+      </c>
     </row>
-    <row r="389" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>420</v>
       </c>
@@ -52586,8 +53261,11 @@
       <c r="AP389">
         <v>0</v>
       </c>
+      <c r="AQ389">
+        <v>0</v>
+      </c>
     </row>
-    <row r="390" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>421</v>
       </c>
@@ -52711,8 +53389,11 @@
       <c r="AP390">
         <v>0</v>
       </c>
+      <c r="AQ390">
+        <v>0</v>
+      </c>
     </row>
-    <row r="391" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>422</v>
       </c>
@@ -52839,8 +53520,11 @@
       <c r="AP391" t="s">
         <v>308</v>
       </c>
+      <c r="AQ391" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="392" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>423</v>
       </c>
@@ -52967,8 +53651,11 @@
       <c r="AP392">
         <v>0</v>
       </c>
+      <c r="AQ392">
+        <v>0</v>
+      </c>
     </row>
-    <row r="393" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>424</v>
       </c>
@@ -53092,8 +53779,11 @@
       <c r="AP393">
         <v>0</v>
       </c>
+      <c r="AQ393">
+        <v>0</v>
+      </c>
     </row>
-    <row r="394" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>425</v>
       </c>
@@ -53217,8 +53907,11 @@
       <c r="AP394">
         <v>0</v>
       </c>
+      <c r="AQ394">
+        <v>0</v>
+      </c>
     </row>
-    <row r="395" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>426</v>
       </c>
@@ -53342,8 +54035,11 @@
       <c r="AP395">
         <v>0</v>
       </c>
+      <c r="AQ395">
+        <v>0</v>
+      </c>
     </row>
-    <row r="396" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>427</v>
       </c>
@@ -53467,8 +54163,11 @@
       <c r="AP396">
         <v>0</v>
       </c>
+      <c r="AQ396">
+        <v>0</v>
+      </c>
     </row>
-    <row r="397" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>428</v>
       </c>
@@ -53592,8 +54291,11 @@
       <c r="AP397">
         <v>0</v>
       </c>
+      <c r="AQ397">
+        <v>0</v>
+      </c>
     </row>
-    <row r="398" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>429</v>
       </c>
@@ -53717,8 +54419,11 @@
       <c r="AP398">
         <v>0</v>
       </c>
+      <c r="AQ398">
+        <v>0</v>
+      </c>
     </row>
-    <row r="399" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>430</v>
       </c>
@@ -53845,8 +54550,11 @@
       <c r="AP399">
         <v>0</v>
       </c>
+      <c r="AQ399">
+        <v>0</v>
+      </c>
     </row>
-    <row r="400" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>431</v>
       </c>
@@ -53970,8 +54678,11 @@
       <c r="AP400">
         <v>0</v>
       </c>
+      <c r="AQ400">
+        <v>0</v>
+      </c>
     </row>
-    <row r="401" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>432</v>
       </c>
@@ -54095,8 +54806,11 @@
       <c r="AP401">
         <v>0</v>
       </c>
+      <c r="AQ401">
+        <v>0</v>
+      </c>
     </row>
-    <row r="402" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>433</v>
       </c>
@@ -54223,8 +54937,11 @@
       <c r="AP402" t="s">
         <v>308</v>
       </c>
+      <c r="AQ402" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="403" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>434</v>
       </c>
@@ -54348,8 +55065,11 @@
       <c r="AP403">
         <v>0</v>
       </c>
+      <c r="AQ403">
+        <v>0</v>
+      </c>
     </row>
-    <row r="404" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>435</v>
       </c>
@@ -54476,8 +55196,11 @@
       <c r="AP404">
         <v>0</v>
       </c>
+      <c r="AQ404">
+        <v>0</v>
+      </c>
     </row>
-    <row r="405" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>437</v>
       </c>
@@ -54601,8 +55324,11 @@
       <c r="AP405">
         <v>0</v>
       </c>
+      <c r="AQ405">
+        <v>0</v>
+      </c>
     </row>
-    <row r="406" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>438</v>
       </c>
@@ -54726,8 +55452,11 @@
       <c r="AP406">
         <v>0</v>
       </c>
+      <c r="AQ406">
+        <v>0</v>
+      </c>
     </row>
-    <row r="407" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>439</v>
       </c>
@@ -54851,8 +55580,11 @@
       <c r="AP407">
         <v>0</v>
       </c>
+      <c r="AQ407">
+        <v>0</v>
+      </c>
     </row>
-    <row r="408" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>440</v>
       </c>
@@ -54976,8 +55708,11 @@
       <c r="AP408">
         <v>0</v>
       </c>
+      <c r="AQ408">
+        <v>0</v>
+      </c>
     </row>
-    <row r="409" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>441</v>
       </c>
@@ -55101,8 +55836,11 @@
       <c r="AP409">
         <v>0</v>
       </c>
+      <c r="AQ409">
+        <v>0</v>
+      </c>
     </row>
-    <row r="410" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>442</v>
       </c>
@@ -55226,8 +55964,11 @@
       <c r="AP410">
         <v>0</v>
       </c>
+      <c r="AQ410">
+        <v>0</v>
+      </c>
     </row>
-    <row r="411" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>443</v>
       </c>
@@ -55351,8 +56092,11 @@
       <c r="AP411">
         <v>0</v>
       </c>
+      <c r="AQ411">
+        <v>0</v>
+      </c>
     </row>
-    <row r="412" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>444</v>
       </c>
@@ -55476,8 +56220,11 @@
       <c r="AP412">
         <v>0</v>
       </c>
+      <c r="AQ412">
+        <v>0</v>
+      </c>
     </row>
-    <row r="413" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>445</v>
       </c>
@@ -55601,8 +56348,11 @@
       <c r="AP413">
         <v>0</v>
       </c>
+      <c r="AQ413">
+        <v>0</v>
+      </c>
     </row>
-    <row r="414" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>446</v>
       </c>
@@ -55726,8 +56476,11 @@
       <c r="AP414">
         <v>0</v>
       </c>
+      <c r="AQ414">
+        <v>0</v>
+      </c>
     </row>
-    <row r="415" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>447</v>
       </c>
@@ -55851,8 +56604,11 @@
       <c r="AP415">
         <v>0</v>
       </c>
+      <c r="AQ415">
+        <v>0</v>
+      </c>
     </row>
-    <row r="416" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>448</v>
       </c>
@@ -55976,8 +56732,11 @@
       <c r="AP416" t="s">
         <v>308</v>
       </c>
+      <c r="AQ416" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="417" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>449</v>
       </c>
@@ -56104,8 +56863,11 @@
       <c r="AP417" t="s">
         <v>308</v>
       </c>
+      <c r="AQ417" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="418" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>450</v>
       </c>
@@ -56229,8 +56991,11 @@
       <c r="AP418">
         <v>0</v>
       </c>
+      <c r="AQ418">
+        <v>0</v>
+      </c>
     </row>
-    <row r="419" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>451</v>
       </c>
@@ -56354,8 +57119,11 @@
       <c r="AP419">
         <v>0</v>
       </c>
+      <c r="AQ419">
+        <v>0</v>
+      </c>
     </row>
-    <row r="420" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>452</v>
       </c>
@@ -56479,8 +57247,11 @@
       <c r="AP420">
         <v>0</v>
       </c>
+      <c r="AQ420">
+        <v>0</v>
+      </c>
     </row>
-    <row r="421" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>453</v>
       </c>
@@ -56607,8 +57378,11 @@
       <c r="AP421" t="s">
         <v>308</v>
       </c>
+      <c r="AQ421" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="422" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>454</v>
       </c>
@@ -56732,8 +57506,11 @@
       <c r="AP422">
         <v>0</v>
       </c>
+      <c r="AQ422">
+        <v>0</v>
+      </c>
     </row>
-    <row r="423" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>455</v>
       </c>
@@ -56860,8 +57637,11 @@
       <c r="AP423" t="s">
         <v>308</v>
       </c>
+      <c r="AQ423" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="424" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>457</v>
       </c>
@@ -56985,8 +57765,11 @@
       <c r="AP424">
         <v>0</v>
       </c>
+      <c r="AQ424">
+        <v>0</v>
+      </c>
     </row>
-    <row r="425" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>458</v>
       </c>
@@ -57110,8 +57893,11 @@
       <c r="AP425">
         <v>0</v>
       </c>
+      <c r="AQ425">
+        <v>0</v>
+      </c>
     </row>
-    <row r="426" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>459</v>
       </c>
@@ -57235,8 +58021,11 @@
       <c r="AP426" t="s">
         <v>308</v>
       </c>
+      <c r="AQ426" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="427" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>460</v>
       </c>
@@ -57360,8 +58149,11 @@
       <c r="AP427">
         <v>0</v>
       </c>
+      <c r="AQ427">
+        <v>0</v>
+      </c>
     </row>
-    <row r="428" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>461</v>
       </c>
@@ -57485,8 +58277,11 @@
       <c r="AP428">
         <v>0</v>
       </c>
+      <c r="AQ428">
+        <v>0</v>
+      </c>
     </row>
-    <row r="429" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>462</v>
       </c>
@@ -57613,8 +58408,11 @@
       <c r="AP429">
         <v>0</v>
       </c>
+      <c r="AQ429">
+        <v>0</v>
+      </c>
     </row>
-    <row r="430" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>464</v>
       </c>
@@ -57738,8 +58536,11 @@
       <c r="AP430">
         <v>0</v>
       </c>
+      <c r="AQ430">
+        <v>0</v>
+      </c>
     </row>
-    <row r="431" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>465</v>
       </c>
@@ -57866,8 +58667,11 @@
       <c r="AP431" t="s">
         <v>308</v>
       </c>
+      <c r="AQ431" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="432" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>466</v>
       </c>
@@ -57991,8 +58795,11 @@
       <c r="AP432">
         <v>0</v>
       </c>
+      <c r="AQ432">
+        <v>0</v>
+      </c>
     </row>
-    <row r="433" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>467</v>
       </c>
@@ -58116,8 +58923,11 @@
       <c r="AP433">
         <v>0</v>
       </c>
+      <c r="AQ433">
+        <v>0</v>
+      </c>
     </row>
-    <row r="434" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>468</v>
       </c>
@@ -58241,8 +59051,11 @@
       <c r="AP434">
         <v>0</v>
       </c>
+      <c r="AQ434">
+        <v>0</v>
+      </c>
     </row>
-    <row r="435" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>469</v>
       </c>
@@ -58366,8 +59179,11 @@
       <c r="AP435">
         <v>0</v>
       </c>
+      <c r="AQ435">
+        <v>0</v>
+      </c>
     </row>
-    <row r="436" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>470</v>
       </c>
@@ -58491,8 +59307,11 @@
       <c r="AP436">
         <v>0</v>
       </c>
+      <c r="AQ436">
+        <v>0</v>
+      </c>
     </row>
-    <row r="437" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>471</v>
       </c>
@@ -58616,8 +59435,11 @@
       <c r="AP437">
         <v>0</v>
       </c>
+      <c r="AQ437">
+        <v>0</v>
+      </c>
     </row>
-    <row r="438" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>472</v>
       </c>
@@ -58738,8 +59560,11 @@
       <c r="AP438">
         <v>0</v>
       </c>
+      <c r="AQ438">
+        <v>0</v>
+      </c>
     </row>
-    <row r="439" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>473</v>
       </c>
@@ -58863,8 +59688,11 @@
       <c r="AP439">
         <v>0</v>
       </c>
+      <c r="AQ439">
+        <v>0</v>
+      </c>
     </row>
-    <row r="440" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>474</v>
       </c>
@@ -58988,8 +59816,11 @@
       <c r="AP440">
         <v>0</v>
       </c>
+      <c r="AQ440">
+        <v>0</v>
+      </c>
     </row>
-    <row r="441" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>475</v>
       </c>
@@ -59113,8 +59944,11 @@
       <c r="AP441">
         <v>0</v>
       </c>
+      <c r="AQ441">
+        <v>0</v>
+      </c>
     </row>
-    <row r="442" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>476</v>
       </c>
@@ -59241,8 +60075,11 @@
       <c r="AP442" t="s">
         <v>308</v>
       </c>
+      <c r="AQ442" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="443" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>478</v>
       </c>
@@ -59366,8 +60203,11 @@
       <c r="AP443">
         <v>0</v>
       </c>
+      <c r="AQ443">
+        <v>0</v>
+      </c>
     </row>
-    <row r="444" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
         <v>479</v>
       </c>
@@ -59494,8 +60334,11 @@
       <c r="AP444" t="s">
         <v>308</v>
       </c>
+      <c r="AQ444" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="445" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
         <v>480</v>
       </c>
@@ -59619,8 +60462,11 @@
       <c r="AP445">
         <v>0</v>
       </c>
+      <c r="AQ445">
+        <v>0</v>
+      </c>
     </row>
-    <row r="446" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
         <v>481</v>
       </c>
@@ -59744,8 +60590,11 @@
       <c r="AP446">
         <v>0</v>
       </c>
+      <c r="AQ446">
+        <v>0</v>
+      </c>
     </row>
-    <row r="447" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>482</v>
       </c>
@@ -59869,8 +60718,11 @@
       <c r="AP447">
         <v>0</v>
       </c>
+      <c r="AQ447">
+        <v>0</v>
+      </c>
     </row>
-    <row r="448" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
         <v>483</v>
       </c>
@@ -59994,8 +60846,11 @@
       <c r="AP448">
         <v>0</v>
       </c>
+      <c r="AQ448">
+        <v>0</v>
+      </c>
     </row>
-    <row r="449" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>484</v>
       </c>
@@ -60119,8 +60974,11 @@
       <c r="AP449">
         <v>0</v>
       </c>
+      <c r="AQ449">
+        <v>0</v>
+      </c>
     </row>
-    <row r="450" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>485</v>
       </c>
@@ -60244,8 +61102,11 @@
       <c r="AP450">
         <v>0</v>
       </c>
+      <c r="AQ450">
+        <v>0</v>
+      </c>
     </row>
-    <row r="451" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>486</v>
       </c>
@@ -60372,8 +61233,11 @@
       <c r="AP451" t="s">
         <v>308</v>
       </c>
+      <c r="AQ451" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="452" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
         <v>487</v>
       </c>
@@ -60497,8 +61361,11 @@
       <c r="AP452">
         <v>0</v>
       </c>
+      <c r="AQ452">
+        <v>0</v>
+      </c>
     </row>
-    <row r="453" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>490</v>
       </c>
@@ -60622,8 +61489,11 @@
       <c r="AP453">
         <v>0</v>
       </c>
+      <c r="AQ453">
+        <v>0</v>
+      </c>
     </row>
-    <row r="454" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
         <v>491</v>
       </c>
@@ -60747,8 +61617,11 @@
       <c r="AP454">
         <v>0</v>
       </c>
+      <c r="AQ454">
+        <v>0</v>
+      </c>
     </row>
-    <row r="455" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>492</v>
       </c>
@@ -60872,8 +61745,11 @@
       <c r="AP455">
         <v>0</v>
       </c>
+      <c r="AQ455">
+        <v>0</v>
+      </c>
     </row>
-    <row r="456" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
         <v>493</v>
       </c>
@@ -60997,8 +61873,11 @@
       <c r="AP456">
         <v>0</v>
       </c>
+      <c r="AQ456">
+        <v>0</v>
+      </c>
     </row>
-    <row r="457" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>494</v>
       </c>
@@ -61125,8 +62004,11 @@
       <c r="AP457" s="2">
         <v>0</v>
       </c>
+      <c r="AQ457" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="458" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
         <v>495</v>
       </c>
@@ -61250,8 +62132,11 @@
       <c r="AP458" s="2">
         <v>0</v>
       </c>
+      <c r="AQ458" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="459" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>496</v>
       </c>
@@ -61375,8 +62260,11 @@
       <c r="AP459" s="2">
         <v>0</v>
       </c>
+      <c r="AQ459" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="460" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
         <v>497</v>
       </c>
@@ -61500,8 +62388,11 @@
       <c r="AP460" s="2">
         <v>0</v>
       </c>
+      <c r="AQ460" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="461" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
         <v>498</v>
       </c>
@@ -61625,8 +62516,11 @@
       <c r="AP461" s="2">
         <v>0</v>
       </c>
+      <c r="AQ461" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="462" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
         <v>499</v>
       </c>
@@ -61750,8 +62644,11 @@
       <c r="AP462" s="2">
         <v>0</v>
       </c>
+      <c r="AQ462" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="463" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
         <v>500</v>
       </c>
@@ -61875,8 +62772,11 @@
       <c r="AP463" s="2">
         <v>0</v>
       </c>
+      <c r="AQ463" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="464" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
         <v>501</v>
       </c>
@@ -62000,8 +62900,11 @@
       <c r="AP464" s="2">
         <v>0</v>
       </c>
+      <c r="AQ464" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="465" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>502</v>
       </c>
@@ -62125,8 +63028,11 @@
       <c r="AP465" s="2">
         <v>0</v>
       </c>
+      <c r="AQ465" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="466" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>503</v>
       </c>
@@ -62250,8 +63156,11 @@
       <c r="AP466" s="2">
         <v>0</v>
       </c>
+      <c r="AQ466" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="467" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
         <v>504</v>
       </c>
@@ -62375,8 +63284,11 @@
       <c r="AP467" s="2">
         <v>0</v>
       </c>
+      <c r="AQ467" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="468" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>505</v>
       </c>
@@ -62503,8 +63415,11 @@
       <c r="AP468" s="2">
         <v>0</v>
       </c>
+      <c r="AQ468" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="469" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
         <v>506</v>
       </c>
@@ -62631,8 +63546,11 @@
       <c r="AP469" s="2">
         <v>0</v>
       </c>
+      <c r="AQ469" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="470" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>507</v>
       </c>
@@ -62756,8 +63674,11 @@
       <c r="AP470" s="2">
         <v>0</v>
       </c>
+      <c r="AQ470" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="471" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
         <v>508</v>
       </c>
@@ -62881,8 +63802,11 @@
       <c r="AP471" s="2">
         <v>0</v>
       </c>
+      <c r="AQ471" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="472" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>509</v>
       </c>
@@ -63006,8 +63930,11 @@
       <c r="AP472" s="2">
         <v>0</v>
       </c>
+      <c r="AQ472" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="473" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
         <v>510</v>
       </c>
@@ -63131,8 +64058,11 @@
       <c r="AP473" s="2">
         <v>0</v>
       </c>
+      <c r="AQ473" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="474" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>511</v>
       </c>
@@ -63256,8 +64186,11 @@
       <c r="AP474" s="2">
         <v>0</v>
       </c>
+      <c r="AQ474" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="475" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
         <v>512</v>
       </c>
@@ -63384,8 +64317,11 @@
       <c r="AP475" s="2">
         <v>0</v>
       </c>
+      <c r="AQ475" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="476" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
         <v>513</v>
       </c>
@@ -63509,8 +64445,11 @@
       <c r="AP476" s="2">
         <v>0</v>
       </c>
+      <c r="AQ476" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="477" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
         <v>514</v>
       </c>
@@ -63634,8 +64573,11 @@
       <c r="AP477" s="2">
         <v>0</v>
       </c>
+      <c r="AQ477" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="478" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
         <v>515</v>
       </c>
@@ -63759,8 +64701,11 @@
       <c r="AP478" s="2">
         <v>0</v>
       </c>
+      <c r="AQ478" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="479" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
         <v>516</v>
       </c>
@@ -63884,8 +64829,11 @@
       <c r="AP479" s="2">
         <v>0</v>
       </c>
+      <c r="AQ479" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="480" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
         <v>517</v>
       </c>
@@ -64009,8 +64957,11 @@
       <c r="AP480" s="2">
         <v>0</v>
       </c>
+      <c r="AQ480" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="481" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>518</v>
       </c>
@@ -64134,8 +65085,11 @@
       <c r="AP481" s="2">
         <v>0</v>
       </c>
+      <c r="AQ481" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="482" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
         <v>519</v>
       </c>
@@ -64259,8 +65213,11 @@
       <c r="AP482">
         <v>0</v>
       </c>
+      <c r="AQ482">
+        <v>0</v>
+      </c>
     </row>
-    <row r="483" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
         <v>520</v>
       </c>
@@ -64384,8 +65341,11 @@
       <c r="AP483">
         <v>0</v>
       </c>
+      <c r="AQ483">
+        <v>0</v>
+      </c>
     </row>
-    <row r="484" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>521</v>
       </c>
@@ -64509,8 +65469,11 @@
       <c r="AP484">
         <v>0</v>
       </c>
+      <c r="AQ484">
+        <v>0</v>
+      </c>
     </row>
-    <row r="485" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
         <v>522</v>
       </c>
@@ -64634,8 +65597,11 @@
       <c r="AP485">
         <v>0</v>
       </c>
+      <c r="AQ485">
+        <v>0</v>
+      </c>
     </row>
-    <row r="486" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>523</v>
       </c>
@@ -64759,8 +65725,11 @@
       <c r="AP486">
         <v>0</v>
       </c>
+      <c r="AQ486">
+        <v>0</v>
+      </c>
     </row>
-    <row r="487" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
         <v>524</v>
       </c>
@@ -64884,8 +65853,11 @@
       <c r="AP487">
         <v>0</v>
       </c>
+      <c r="AQ487">
+        <v>0</v>
+      </c>
     </row>
-    <row r="488" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
         <v>525</v>
       </c>
@@ -65012,8 +65984,11 @@
       <c r="AP488">
         <v>0</v>
       </c>
+      <c r="AQ488">
+        <v>0</v>
+      </c>
     </row>
-    <row r="489" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
         <v>526</v>
       </c>
@@ -65137,8 +66112,11 @@
       <c r="AP489">
         <v>0</v>
       </c>
+      <c r="AQ489">
+        <v>0</v>
+      </c>
     </row>
-    <row r="490" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
         <v>527</v>
       </c>
@@ -65262,8 +66240,11 @@
       <c r="AP490">
         <v>0</v>
       </c>
+      <c r="AQ490">
+        <v>0</v>
+      </c>
     </row>
-    <row r="491" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
         <v>528</v>
       </c>
@@ -65387,8 +66368,11 @@
       <c r="AP491">
         <v>0</v>
       </c>
+      <c r="AQ491">
+        <v>0</v>
+      </c>
     </row>
-    <row r="492" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
         <v>529</v>
       </c>
@@ -65512,8 +66496,11 @@
       <c r="AP492">
         <v>0</v>
       </c>
+      <c r="AQ492">
+        <v>0</v>
+      </c>
     </row>
-    <row r="493" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
         <v>530</v>
       </c>
@@ -65637,8 +66624,11 @@
       <c r="AP493">
         <v>0</v>
       </c>
+      <c r="AQ493">
+        <v>0</v>
+      </c>
     </row>
-    <row r="494" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
         <v>531</v>
       </c>
@@ -65762,8 +66752,11 @@
       <c r="AP494">
         <v>0</v>
       </c>
+      <c r="AQ494">
+        <v>0</v>
+      </c>
     </row>
-    <row r="495" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
         <v>532</v>
       </c>
@@ -65890,8 +66883,11 @@
       <c r="AP495" t="s">
         <v>308</v>
       </c>
+      <c r="AQ495" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="496" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
         <v>533</v>
       </c>
@@ -66015,8 +67011,11 @@
       <c r="AP496">
         <v>0</v>
       </c>
+      <c r="AQ496">
+        <v>0</v>
+      </c>
     </row>
-    <row r="497" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
         <v>534</v>
       </c>
@@ -66140,8 +67139,11 @@
       <c r="AP497" s="2">
         <v>0</v>
       </c>
+      <c r="AQ497" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="498" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
         <v>535</v>
       </c>
@@ -66265,8 +67267,11 @@
       <c r="AP498" s="2">
         <v>0</v>
       </c>
+      <c r="AQ498" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="499" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
         <v>536</v>
       </c>
@@ -66390,8 +67395,11 @@
       <c r="AP499" s="2">
         <v>0</v>
       </c>
+      <c r="AQ499" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="500" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
         <v>537</v>
       </c>
@@ -66515,8 +67523,11 @@
       <c r="AP500" s="2">
         <v>0</v>
       </c>
+      <c r="AQ500" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="501" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
         <v>538</v>
       </c>
@@ -66640,8 +67651,11 @@
       <c r="AP501" s="2">
         <v>0</v>
       </c>
+      <c r="AQ501" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="502" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
         <v>539</v>
       </c>
@@ -66765,8 +67779,11 @@
       <c r="AP502" s="2">
         <v>0</v>
       </c>
+      <c r="AQ502" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="503" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
         <v>540</v>
       </c>
@@ -66890,8 +67907,11 @@
       <c r="AP503" s="2">
         <v>0</v>
       </c>
+      <c r="AQ503" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="504" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
         <v>541</v>
       </c>
@@ -67015,8 +68035,11 @@
       <c r="AP504" s="2">
         <v>0</v>
       </c>
+      <c r="AQ504" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="505" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
         <v>542</v>
       </c>
@@ -67140,8 +68163,11 @@
       <c r="AP505" s="2">
         <v>0</v>
       </c>
+      <c r="AQ505" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="506" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
         <v>543</v>
       </c>
@@ -67265,8 +68291,11 @@
       <c r="AP506" s="2">
         <v>0</v>
       </c>
+      <c r="AQ506" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="507" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
         <v>544</v>
       </c>
@@ -67390,8 +68419,11 @@
       <c r="AP507" s="2">
         <v>0</v>
       </c>
+      <c r="AQ507" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="508" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A508" t="s">
         <v>545</v>
       </c>
@@ -67515,8 +68547,11 @@
       <c r="AP508" s="2">
         <v>0</v>
       </c>
+      <c r="AQ508" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="509" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
         <v>546</v>
       </c>
@@ -67640,8 +68675,11 @@
       <c r="AP509" s="2">
         <v>0</v>
       </c>
+      <c r="AQ509" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="510" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A510" t="s">
         <v>547</v>
       </c>
@@ -67765,8 +68803,11 @@
       <c r="AP510" s="2">
         <v>0</v>
       </c>
+      <c r="AQ510" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="511" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
         <v>548</v>
       </c>
@@ -67890,8 +68931,11 @@
       <c r="AP511" s="2">
         <v>0</v>
       </c>
+      <c r="AQ511" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="512" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A512" t="s">
         <v>549</v>
       </c>
@@ -68018,8 +69062,11 @@
       <c r="AP512">
         <v>0</v>
       </c>
+      <c r="AQ512">
+        <v>0</v>
+      </c>
     </row>
-    <row r="513" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
         <v>550</v>
       </c>
@@ -68143,8 +69190,11 @@
       <c r="AP513">
         <v>0</v>
       </c>
+      <c r="AQ513">
+        <v>0</v>
+      </c>
     </row>
-    <row r="514" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
         <v>551</v>
       </c>
@@ -68268,8 +69318,11 @@
       <c r="AP514">
         <v>0</v>
       </c>
+      <c r="AQ514">
+        <v>0</v>
+      </c>
     </row>
-    <row r="515" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
         <v>552</v>
       </c>
@@ -68393,8 +69446,11 @@
       <c r="AP515">
         <v>0</v>
       </c>
+      <c r="AQ515">
+        <v>0</v>
+      </c>
     </row>
-    <row r="516" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A516" t="s">
         <v>553</v>
       </c>
@@ -68518,8 +69574,11 @@
       <c r="AP516">
         <v>0</v>
       </c>
+      <c r="AQ516">
+        <v>0</v>
+      </c>
     </row>
-    <row r="517" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
         <v>554</v>
       </c>
@@ -68646,8 +69705,11 @@
       <c r="AP517" t="s">
         <v>308</v>
       </c>
+      <c r="AQ517" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="518" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A518" t="s">
         <v>555</v>
       </c>
@@ -68774,8 +69836,11 @@
       <c r="AP518" t="s">
         <v>308</v>
       </c>
+      <c r="AQ518" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="519" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A519" t="s">
         <v>557</v>
       </c>
@@ -68899,8 +69964,11 @@
       <c r="AP519">
         <v>0</v>
       </c>
+      <c r="AQ519">
+        <v>0</v>
+      </c>
     </row>
-    <row r="520" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A520" t="s">
         <v>558</v>
       </c>
@@ -69024,8 +70092,11 @@
       <c r="AP520">
         <v>0</v>
       </c>
+      <c r="AQ520">
+        <v>0</v>
+      </c>
     </row>
-    <row r="521" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A521" t="s">
         <v>559</v>
       </c>
@@ -69149,8 +70220,11 @@
       <c r="AP521">
         <v>0</v>
       </c>
+      <c r="AQ521">
+        <v>0</v>
+      </c>
     </row>
-    <row r="522" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
         <v>560</v>
       </c>
@@ -69274,8 +70348,11 @@
       <c r="AP522">
         <v>0</v>
       </c>
+      <c r="AQ522">
+        <v>0</v>
+      </c>
     </row>
-    <row r="523" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
         <v>561</v>
       </c>
@@ -69399,8 +70476,11 @@
       <c r="AP523">
         <v>0</v>
       </c>
+      <c r="AQ523">
+        <v>0</v>
+      </c>
     </row>
-    <row r="524" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
         <v>562</v>
       </c>
@@ -69524,8 +70604,11 @@
       <c r="AP524">
         <v>0</v>
       </c>
+      <c r="AQ524">
+        <v>0</v>
+      </c>
     </row>
-    <row r="525" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
         <v>563</v>
       </c>
@@ -69649,8 +70732,11 @@
       <c r="AP525">
         <v>0</v>
       </c>
+      <c r="AQ525">
+        <v>0</v>
+      </c>
     </row>
-    <row r="526" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="526" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A526" t="s">
         <v>564</v>
       </c>
@@ -69774,8 +70860,11 @@
       <c r="AP526">
         <v>0</v>
       </c>
+      <c r="AQ526">
+        <v>0</v>
+      </c>
     </row>
-    <row r="527" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="527" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
         <v>565</v>
       </c>
@@ -69899,8 +70988,11 @@
       <c r="AP527">
         <v>0</v>
       </c>
+      <c r="AQ527">
+        <v>0</v>
+      </c>
     </row>
-    <row r="528" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="528" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A528" t="s">
         <v>566</v>
       </c>
@@ -70027,8 +71119,11 @@
       <c r="AP528">
         <v>0</v>
       </c>
+      <c r="AQ528">
+        <v>0</v>
+      </c>
     </row>
-    <row r="529" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>567</v>
       </c>
@@ -70152,8 +71247,11 @@
       <c r="AP529">
         <v>0</v>
       </c>
+      <c r="AQ529">
+        <v>0</v>
+      </c>
     </row>
-    <row r="530" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A530" t="s">
         <v>568</v>
       </c>
@@ -70277,8 +71375,11 @@
       <c r="AP530">
         <v>0</v>
       </c>
+      <c r="AQ530">
+        <v>0</v>
+      </c>
     </row>
-    <row r="531" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
         <v>569</v>
       </c>
@@ -70405,8 +71506,11 @@
       <c r="AP531">
         <v>0</v>
       </c>
+      <c r="AQ531">
+        <v>0</v>
+      </c>
     </row>
-    <row r="532" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
         <v>570</v>
       </c>
@@ -70533,8 +71637,11 @@
       <c r="AP532">
         <v>0</v>
       </c>
+      <c r="AQ532">
+        <v>0</v>
+      </c>
     </row>
-    <row r="533" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
         <v>571</v>
       </c>
@@ -70658,8 +71765,11 @@
       <c r="AP533">
         <v>0</v>
       </c>
+      <c r="AQ533">
+        <v>0</v>
+      </c>
     </row>
-    <row r="534" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A534" t="s">
         <v>572</v>
       </c>
@@ -70783,8 +71893,11 @@
       <c r="AP534">
         <v>0</v>
       </c>
+      <c r="AQ534">
+        <v>0</v>
+      </c>
     </row>
-    <row r="535" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
         <v>573</v>
       </c>
@@ -70908,8 +72021,11 @@
       <c r="AP535">
         <v>0</v>
       </c>
+      <c r="AQ535">
+        <v>0</v>
+      </c>
     </row>
-    <row r="536" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>574</v>
       </c>
@@ -71033,8 +72149,11 @@
       <c r="AP536">
         <v>0</v>
       </c>
+      <c r="AQ536">
+        <v>0</v>
+      </c>
     </row>
-    <row r="537" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
         <v>575</v>
       </c>
@@ -71158,8 +72277,11 @@
       <c r="AP537">
         <v>0</v>
       </c>
+      <c r="AQ537">
+        <v>0</v>
+      </c>
     </row>
-    <row r="538" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
         <v>576</v>
       </c>
@@ -71283,8 +72405,11 @@
       <c r="AP538">
         <v>0</v>
       </c>
+      <c r="AQ538">
+        <v>0</v>
+      </c>
     </row>
-    <row r="539" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
         <v>577</v>
       </c>
@@ -71408,8 +72533,11 @@
       <c r="AP539">
         <v>0</v>
       </c>
+      <c r="AQ539">
+        <v>0</v>
+      </c>
     </row>
-    <row r="540" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>578</v>
       </c>
@@ -71533,8 +72661,11 @@
       <c r="AP540">
         <v>0</v>
       </c>
+      <c r="AQ540">
+        <v>0</v>
+      </c>
     </row>
-    <row r="541" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
         <v>579</v>
       </c>
@@ -71658,8 +72789,11 @@
       <c r="AP541">
         <v>0</v>
       </c>
+      <c r="AQ541">
+        <v>0</v>
+      </c>
     </row>
-    <row r="542" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>580</v>
       </c>
@@ -71781,7 +72915,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="543" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
         <v>583</v>
       </c>
@@ -71900,7 +73034,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="544" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>584</v>
       </c>

</xml_diff>

<commit_message>
addded readme for phenomonitoring and csv
</commit_message>
<xml_diff>
--- a/data/monitoring_phenology/2024_budburst_to_budset.xlsx
+++ b/data/monitoring_phenology/2024_budburst_to_budset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/data/monitoring_phenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DCE158-7E6D-AA46-9856-2340A00F6655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB68AC2-1087-724F-8E8B-7D6BAF56C3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="-2480" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phenological_monitoring" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5474" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5492" uniqueCount="746">
   <si>
     <t>tree_ID</t>
   </si>
@@ -2779,12 +2779,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -3549,9 +3548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AR122" sqref="AR122"/>
+    <sheetView tabSelected="1" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AS164" sqref="AS164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7900,7 +7899,7 @@
       <c r="AQ33">
         <v>6</v>
       </c>
-      <c r="AR33" s="4">
+      <c r="AR33">
         <v>0</v>
       </c>
     </row>
@@ -8031,7 +8030,7 @@
       <c r="AQ34">
         <v>6</v>
       </c>
-      <c r="AR34" s="4">
+      <c r="AR34">
         <v>6</v>
       </c>
     </row>
@@ -8162,7 +8161,7 @@
       <c r="AQ35">
         <v>0</v>
       </c>
-      <c r="AR35" s="4">
+      <c r="AR35">
         <v>0</v>
       </c>
     </row>
@@ -8293,7 +8292,7 @@
       <c r="AQ36">
         <v>0</v>
       </c>
-      <c r="AR36" s="4">
+      <c r="AR36">
         <v>0</v>
       </c>
     </row>
@@ -8424,7 +8423,7 @@
       <c r="AQ37">
         <v>6</v>
       </c>
-      <c r="AR37" s="4">
+      <c r="AR37">
         <v>0</v>
       </c>
     </row>
@@ -8555,7 +8554,7 @@
       <c r="AQ38">
         <v>6</v>
       </c>
-      <c r="AR38" s="4">
+      <c r="AR38">
         <v>0</v>
       </c>
     </row>
@@ -8686,7 +8685,7 @@
       <c r="AQ39">
         <v>0</v>
       </c>
-      <c r="AR39" s="4">
+      <c r="AR39">
         <v>0</v>
       </c>
     </row>
@@ -8817,7 +8816,7 @@
       <c r="AQ40">
         <v>0</v>
       </c>
-      <c r="AR40" s="4">
+      <c r="AR40">
         <v>0</v>
       </c>
     </row>
@@ -8948,7 +8947,7 @@
       <c r="AQ41">
         <v>0</v>
       </c>
-      <c r="AR41" s="4">
+      <c r="AR41">
         <v>0</v>
       </c>
     </row>
@@ -9082,7 +9081,7 @@
       <c r="AQ42">
         <v>6</v>
       </c>
-      <c r="AR42" s="4">
+      <c r="AR42">
         <v>6</v>
       </c>
     </row>
@@ -9213,7 +9212,7 @@
       <c r="AQ43">
         <v>6</v>
       </c>
-      <c r="AR43" s="4">
+      <c r="AR43">
         <v>0</v>
       </c>
     </row>
@@ -9344,7 +9343,7 @@
       <c r="AQ44">
         <v>0</v>
       </c>
-      <c r="AR44" s="4">
+      <c r="AR44">
         <v>0</v>
       </c>
     </row>
@@ -9475,7 +9474,7 @@
       <c r="AQ45">
         <v>6</v>
       </c>
-      <c r="AR45" s="4">
+      <c r="AR45">
         <v>0</v>
       </c>
     </row>
@@ -9606,7 +9605,7 @@
       <c r="AQ46">
         <v>0</v>
       </c>
-      <c r="AR46" s="4">
+      <c r="AR46">
         <v>0</v>
       </c>
     </row>
@@ -19589,6 +19588,9 @@
       <c r="AQ122" s="2">
         <v>0</v>
       </c>
+      <c r="AR122" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
@@ -19717,6 +19719,9 @@
       <c r="AQ123" s="2">
         <v>0</v>
       </c>
+      <c r="AR123" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
@@ -19845,6 +19850,9 @@
       <c r="AQ124" s="2">
         <v>0</v>
       </c>
+      <c r="AR124" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
@@ -19973,6 +19981,9 @@
       <c r="AQ125" s="2">
         <v>6</v>
       </c>
+      <c r="AR125" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="126" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
@@ -20101,6 +20112,9 @@
       <c r="AQ126" s="2">
         <v>0</v>
       </c>
+      <c r="AR126" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="127" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
@@ -20229,6 +20243,9 @@
       <c r="AQ127" s="2">
         <v>0</v>
       </c>
+      <c r="AR127" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
@@ -20357,6 +20374,9 @@
       <c r="AQ128" s="2">
         <v>6</v>
       </c>
+      <c r="AR128" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="129" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
@@ -20485,6 +20505,9 @@
       <c r="AQ129" s="2">
         <v>0</v>
       </c>
+      <c r="AR129" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="130" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
@@ -20613,6 +20636,9 @@
       <c r="AQ130" s="2">
         <v>0</v>
       </c>
+      <c r="AR130" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
@@ -20744,6 +20770,9 @@
       <c r="AQ131" t="s">
         <v>308</v>
       </c>
+      <c r="AR131" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="132" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
@@ -20872,6 +20901,9 @@
       <c r="AQ132" s="2">
         <v>0</v>
       </c>
+      <c r="AR132" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
@@ -21000,6 +21032,9 @@
       <c r="AQ133" s="2">
         <v>0</v>
       </c>
+      <c r="AR133" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="134" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
@@ -21128,6 +21163,9 @@
       <c r="AQ134" s="2">
         <v>6</v>
       </c>
+      <c r="AR134" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="135" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
@@ -21256,6 +21294,9 @@
       <c r="AQ135" s="2">
         <v>0</v>
       </c>
+      <c r="AR135" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
@@ -21384,6 +21425,9 @@
       <c r="AQ136" s="2">
         <v>6</v>
       </c>
+      <c r="AR136" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="137" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
@@ -21516,7 +21560,7 @@
         <v>6</v>
       </c>
       <c r="AR137">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
@@ -21778,7 +21822,7 @@
         <v>6</v>
       </c>
       <c r="AR139">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
@@ -22695,7 +22739,7 @@
         <v>6</v>
       </c>
       <c r="AR146">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
@@ -23225,7 +23269,7 @@
         <v>6</v>
       </c>
       <c r="AR150">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
@@ -23486,6 +23530,9 @@
       <c r="AQ152">
         <v>0</v>
       </c>
+      <c r="AR152">
+        <v>0</v>
+      </c>
     </row>
     <row r="153" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
@@ -23614,6 +23661,9 @@
       <c r="AQ153">
         <v>0</v>
       </c>
+      <c r="AR153">
+        <v>0</v>
+      </c>
     </row>
     <row r="154" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
@@ -23742,6 +23792,9 @@
       <c r="AQ154">
         <v>6</v>
       </c>
+      <c r="AR154">
+        <v>6</v>
+      </c>
     </row>
     <row r="155" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
@@ -23870,6 +23923,9 @@
       <c r="AQ155">
         <v>0</v>
       </c>
+      <c r="AR155">
+        <v>0</v>
+      </c>
     </row>
     <row r="156" spans="1:44" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
@@ -23998,6 +24054,9 @@
       <c r="AQ156">
         <v>0</v>
       </c>
+      <c r="AR156">
+        <v>0</v>
+      </c>
     </row>
     <row r="157" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
@@ -24126,6 +24185,9 @@
       <c r="AQ157">
         <v>0</v>
       </c>
+      <c r="AR157">
+        <v>0</v>
+      </c>
     </row>
     <row r="158" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
@@ -24254,6 +24316,9 @@
       <c r="AQ158">
         <v>6</v>
       </c>
+      <c r="AR158">
+        <v>0</v>
+      </c>
     </row>
     <row r="159" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
@@ -24382,6 +24447,9 @@
       <c r="AQ159">
         <v>0</v>
       </c>
+      <c r="AR159">
+        <v>0</v>
+      </c>
     </row>
     <row r="160" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
@@ -24510,8 +24578,11 @@
       <c r="AQ160">
         <v>0</v>
       </c>
+      <c r="AR160">
+        <v>0</v>
+      </c>
     </row>
-    <row r="161" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>177</v>
       </c>
@@ -24638,8 +24709,11 @@
       <c r="AQ161">
         <v>0</v>
       </c>
+      <c r="AR161">
+        <v>0</v>
+      </c>
     </row>
-    <row r="162" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>178</v>
       </c>
@@ -24769,8 +24843,11 @@
       <c r="AQ162">
         <v>6</v>
       </c>
+      <c r="AR162">
+        <v>6</v>
+      </c>
     </row>
-    <row r="163" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>179</v>
       </c>
@@ -24897,8 +24974,11 @@
       <c r="AQ163">
         <v>0</v>
       </c>
+      <c r="AR163">
+        <v>0</v>
+      </c>
     </row>
-    <row r="164" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>180</v>
       </c>
@@ -25028,8 +25108,11 @@
       <c r="AQ164">
         <v>5</v>
       </c>
+      <c r="AR164">
+        <v>6</v>
+      </c>
     </row>
-    <row r="165" spans="1:43" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:44" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>181</v>
       </c>
@@ -25156,8 +25239,11 @@
       <c r="AQ165">
         <v>0</v>
       </c>
+      <c r="AR165">
+        <v>0</v>
+      </c>
     </row>
-    <row r="166" spans="1:43" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:44" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>182</v>
       </c>
@@ -25284,8 +25370,11 @@
       <c r="AQ166">
         <v>0</v>
       </c>
+      <c r="AR166">
+        <v>0</v>
+      </c>
     </row>
-    <row r="167" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>183</v>
       </c>
@@ -25412,8 +25501,11 @@
       <c r="AQ167">
         <v>0</v>
       </c>
+      <c r="AR167">
+        <v>0</v>
+      </c>
     </row>
-    <row r="168" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>184</v>
       </c>
@@ -25540,8 +25632,11 @@
       <c r="AQ168">
         <v>0</v>
       </c>
+      <c r="AR168">
+        <v>0</v>
+      </c>
     </row>
-    <row r="169" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>185</v>
       </c>
@@ -25668,8 +25763,11 @@
       <c r="AQ169">
         <v>0</v>
       </c>
+      <c r="AR169">
+        <v>0</v>
+      </c>
     </row>
-    <row r="170" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>186</v>
       </c>
@@ -25796,8 +25894,11 @@
       <c r="AQ170">
         <v>0</v>
       </c>
+      <c r="AR170">
+        <v>0</v>
+      </c>
     </row>
-    <row r="171" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>187</v>
       </c>
@@ -25924,8 +26025,11 @@
       <c r="AQ171">
         <v>0</v>
       </c>
+      <c r="AR171">
+        <v>0</v>
+      </c>
     </row>
-    <row r="172" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>188</v>
       </c>
@@ -26052,8 +26156,11 @@
       <c r="AQ172">
         <v>0</v>
       </c>
+      <c r="AR172">
+        <v>0</v>
+      </c>
     </row>
-    <row r="173" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>189</v>
       </c>
@@ -26180,8 +26287,11 @@
       <c r="AQ173">
         <v>0</v>
       </c>
+      <c r="AR173">
+        <v>0</v>
+      </c>
     </row>
-    <row r="174" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>190</v>
       </c>
@@ -26308,8 +26418,11 @@
       <c r="AQ174">
         <v>0</v>
       </c>
+      <c r="AR174">
+        <v>0</v>
+      </c>
     </row>
-    <row r="175" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>191</v>
       </c>
@@ -26436,8 +26549,11 @@
       <c r="AQ175">
         <v>0</v>
       </c>
+      <c r="AR175">
+        <v>0</v>
+      </c>
     </row>
-    <row r="176" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>192</v>
       </c>
@@ -26562,6 +26678,9 @@
         <v>6</v>
       </c>
       <c r="AQ176">
+        <v>0</v>
+      </c>
+      <c r="AR176">
         <v>0</v>
       </c>
     </row>
@@ -26692,6 +26811,9 @@
       <c r="AQ177">
         <v>0</v>
       </c>
+      <c r="AR177">
+        <v>0</v>
+      </c>
     </row>
     <row r="178" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
@@ -26820,6 +26942,9 @@
       <c r="AQ178">
         <v>0</v>
       </c>
+      <c r="AR178">
+        <v>0</v>
+      </c>
     </row>
     <row r="179" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
@@ -26948,6 +27073,9 @@
       <c r="AQ179">
         <v>0</v>
       </c>
+      <c r="AR179">
+        <v>0</v>
+      </c>
     </row>
     <row r="180" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
@@ -27076,6 +27204,9 @@
       <c r="AQ180">
         <v>0</v>
       </c>
+      <c r="AR180">
+        <v>0</v>
+      </c>
     </row>
     <row r="181" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
@@ -27204,6 +27335,9 @@
       <c r="AQ181">
         <v>0</v>
       </c>
+      <c r="AR181">
+        <v>0</v>
+      </c>
     </row>
     <row r="182" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
@@ -35103,6 +35237,9 @@
       <c r="AQ242">
         <v>0</v>
       </c>
+      <c r="AR242">
+        <v>0</v>
+      </c>
     </row>
     <row r="243" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
@@ -35229,6 +35366,9 @@
       <c r="AQ243">
         <v>0</v>
       </c>
+      <c r="AR243">
+        <v>0</v>
+      </c>
     </row>
     <row r="244" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
@@ -35355,6 +35495,9 @@
       <c r="AQ244">
         <v>0</v>
       </c>
+      <c r="AR244">
+        <v>0</v>
+      </c>
     </row>
     <row r="245" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
@@ -35481,6 +35624,9 @@
       <c r="AQ245">
         <v>0</v>
       </c>
+      <c r="AR245">
+        <v>0</v>
+      </c>
     </row>
     <row r="246" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
@@ -35607,6 +35753,9 @@
       <c r="AQ246">
         <v>0</v>
       </c>
+      <c r="AR246">
+        <v>0</v>
+      </c>
     </row>
     <row r="247" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
@@ -35733,6 +35882,9 @@
       <c r="AQ247">
         <v>0</v>
       </c>
+      <c r="AR247">
+        <v>0</v>
+      </c>
     </row>
     <row r="248" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
@@ -35859,6 +36011,9 @@
       <c r="AQ248">
         <v>0</v>
       </c>
+      <c r="AR248">
+        <v>0</v>
+      </c>
     </row>
     <row r="249" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
@@ -35985,6 +36140,9 @@
       <c r="AQ249">
         <v>0</v>
       </c>
+      <c r="AR249">
+        <v>0</v>
+      </c>
     </row>
     <row r="250" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
@@ -36111,6 +36269,9 @@
       <c r="AQ250">
         <v>0</v>
       </c>
+      <c r="AR250">
+        <v>0</v>
+      </c>
     </row>
     <row r="251" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
@@ -36237,6 +36398,9 @@
       <c r="AQ251">
         <v>0</v>
       </c>
+      <c r="AR251">
+        <v>0</v>
+      </c>
     </row>
     <row r="252" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
@@ -36363,6 +36527,9 @@
       <c r="AQ252">
         <v>0</v>
       </c>
+      <c r="AR252">
+        <v>0</v>
+      </c>
     </row>
     <row r="253" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
@@ -36489,6 +36656,9 @@
       <c r="AQ253">
         <v>0</v>
       </c>
+      <c r="AR253">
+        <v>0</v>
+      </c>
     </row>
     <row r="254" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
@@ -36615,6 +36785,9 @@
       <c r="AQ254">
         <v>0</v>
       </c>
+      <c r="AR254">
+        <v>0</v>
+      </c>
     </row>
     <row r="255" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
@@ -36741,6 +36914,9 @@
       <c r="AQ255">
         <v>0</v>
       </c>
+      <c r="AR255">
+        <v>0</v>
+      </c>
     </row>
     <row r="256" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
@@ -36867,6 +37043,9 @@
       <c r="AQ256">
         <v>0</v>
       </c>
+      <c r="AR256">
+        <v>0</v>
+      </c>
     </row>
     <row r="257" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
@@ -36993,6 +37172,9 @@
       <c r="AQ257">
         <v>0</v>
       </c>
+      <c r="AR257">
+        <v>0</v>
+      </c>
     </row>
     <row r="258" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
@@ -37119,6 +37301,9 @@
       <c r="AQ258">
         <v>0</v>
       </c>
+      <c r="AR258">
+        <v>0</v>
+      </c>
     </row>
     <row r="259" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
@@ -37245,6 +37430,9 @@
       <c r="AQ259">
         <v>0</v>
       </c>
+      <c r="AR259">
+        <v>0</v>
+      </c>
     </row>
     <row r="260" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
@@ -37371,6 +37559,9 @@
       <c r="AQ260">
         <v>0</v>
       </c>
+      <c r="AR260">
+        <v>0</v>
+      </c>
     </row>
     <row r="261" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
@@ -37497,6 +37688,9 @@
       <c r="AQ261">
         <v>0</v>
       </c>
+      <c r="AR261">
+        <v>0</v>
+      </c>
     </row>
     <row r="262" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
@@ -37623,6 +37817,9 @@
       <c r="AQ262">
         <v>0</v>
       </c>
+      <c r="AR262">
+        <v>0</v>
+      </c>
     </row>
     <row r="263" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
@@ -37749,6 +37946,9 @@
       <c r="AQ263">
         <v>0</v>
       </c>
+      <c r="AR263">
+        <v>0</v>
+      </c>
     </row>
     <row r="264" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
@@ -37875,6 +38075,9 @@
       <c r="AQ264">
         <v>0</v>
       </c>
+      <c r="AR264">
+        <v>0</v>
+      </c>
     </row>
     <row r="265" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
@@ -38001,6 +38204,9 @@
       <c r="AQ265">
         <v>0</v>
       </c>
+      <c r="AR265">
+        <v>0</v>
+      </c>
     </row>
     <row r="266" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
@@ -38127,6 +38333,9 @@
       <c r="AQ266">
         <v>0</v>
       </c>
+      <c r="AR266">
+        <v>0</v>
+      </c>
     </row>
     <row r="267" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
@@ -38253,6 +38462,9 @@
       <c r="AQ267">
         <v>0</v>
       </c>
+      <c r="AR267">
+        <v>0</v>
+      </c>
     </row>
     <row r="268" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
@@ -38379,6 +38591,9 @@
       <c r="AQ268">
         <v>0</v>
       </c>
+      <c r="AR268">
+        <v>0</v>
+      </c>
     </row>
     <row r="269" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
@@ -38505,6 +38720,9 @@
       <c r="AQ269">
         <v>0</v>
       </c>
+      <c r="AR269">
+        <v>0</v>
+      </c>
     </row>
     <row r="270" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
@@ -38631,6 +38849,9 @@
       <c r="AQ270">
         <v>0</v>
       </c>
+      <c r="AR270">
+        <v>0</v>
+      </c>
     </row>
     <row r="271" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
@@ -38757,6 +38978,9 @@
       <c r="AQ271">
         <v>0</v>
       </c>
+      <c r="AR271">
+        <v>0</v>
+      </c>
     </row>
     <row r="272" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
@@ -46790,6 +47014,9 @@
       <c r="AQ332">
         <v>0</v>
       </c>
+      <c r="AR332">
+        <v>0</v>
+      </c>
     </row>
     <row r="333" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
@@ -46918,6 +47145,9 @@
       <c r="AQ333">
         <v>0</v>
       </c>
+      <c r="AR333">
+        <v>0</v>
+      </c>
     </row>
     <row r="334" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
@@ -47049,6 +47279,9 @@
       <c r="AQ334" t="s">
         <v>308</v>
       </c>
+      <c r="AR334" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="335" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
@@ -47180,6 +47413,9 @@
       <c r="AQ335" t="s">
         <v>308</v>
       </c>
+      <c r="AR335" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="336" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
@@ -47308,8 +47544,11 @@
       <c r="AQ336">
         <v>0</v>
       </c>
+      <c r="AR336">
+        <v>0</v>
+      </c>
     </row>
-    <row r="337" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>365</v>
       </c>
@@ -47439,8 +47678,11 @@
       <c r="AQ337" t="s">
         <v>308</v>
       </c>
+      <c r="AR337" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="338" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>366</v>
       </c>
@@ -47567,8 +47809,11 @@
       <c r="AQ338">
         <v>0</v>
       </c>
+      <c r="AR338">
+        <v>0</v>
+      </c>
     </row>
-    <row r="339" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>367</v>
       </c>
@@ -47695,8 +47940,11 @@
       <c r="AQ339">
         <v>0</v>
       </c>
+      <c r="AR339">
+        <v>0</v>
+      </c>
     </row>
-    <row r="340" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>368</v>
       </c>
@@ -47823,8 +48071,11 @@
       <c r="AQ340">
         <v>0</v>
       </c>
+      <c r="AR340">
+        <v>0</v>
+      </c>
     </row>
-    <row r="341" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>369</v>
       </c>
@@ -47951,8 +48202,11 @@
       <c r="AQ341">
         <v>0</v>
       </c>
+      <c r="AR341">
+        <v>0</v>
+      </c>
     </row>
-    <row r="342" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>370</v>
       </c>
@@ -48082,8 +48336,11 @@
       <c r="AQ342" t="s">
         <v>308</v>
       </c>
+      <c r="AR342" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="343" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>371</v>
       </c>
@@ -48213,8 +48470,11 @@
       <c r="AQ343" t="s">
         <v>308</v>
       </c>
+      <c r="AR343" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="344" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>372</v>
       </c>
@@ -48344,8 +48604,11 @@
       <c r="AQ344">
         <v>0</v>
       </c>
+      <c r="AR344">
+        <v>0</v>
+      </c>
     </row>
-    <row r="345" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>373</v>
       </c>
@@ -48472,8 +48735,11 @@
       <c r="AQ345" t="s">
         <v>308</v>
       </c>
+      <c r="AR345" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="346" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>374</v>
       </c>
@@ -48600,8 +48866,11 @@
       <c r="AQ346">
         <v>0</v>
       </c>
+      <c r="AR346">
+        <v>0</v>
+      </c>
     </row>
-    <row r="347" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>375</v>
       </c>
@@ -48728,8 +48997,11 @@
       <c r="AQ347">
         <v>6</v>
       </c>
+      <c r="AR347">
+        <v>0</v>
+      </c>
     </row>
-    <row r="348" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>376</v>
       </c>
@@ -48859,8 +49131,11 @@
       <c r="AQ348">
         <v>6</v>
       </c>
+      <c r="AR348">
+        <v>0</v>
+      </c>
     </row>
-    <row r="349" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>377</v>
       </c>
@@ -48987,8 +49262,11 @@
       <c r="AQ349">
         <v>0</v>
       </c>
+      <c r="AR349">
+        <v>0</v>
+      </c>
     </row>
-    <row r="350" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>378</v>
       </c>
@@ -49115,8 +49393,11 @@
       <c r="AQ350" t="s">
         <v>308</v>
       </c>
+      <c r="AR350" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="351" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>379</v>
       </c>
@@ -49243,8 +49524,11 @@
       <c r="AQ351">
         <v>0</v>
       </c>
+      <c r="AR351">
+        <v>0</v>
+      </c>
     </row>
-    <row r="352" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>380</v>
       </c>
@@ -49372,6 +49656,9 @@
         <v>6</v>
       </c>
       <c r="AQ352">
+        <v>0</v>
+      </c>
+      <c r="AR352">
         <v>0</v>
       </c>
     </row>
@@ -49502,6 +49789,9 @@
       <c r="AQ353">
         <v>0</v>
       </c>
+      <c r="AR353">
+        <v>0</v>
+      </c>
     </row>
     <row r="354" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
@@ -49630,6 +49920,9 @@
       <c r="AQ354">
         <v>0</v>
       </c>
+      <c r="AR354">
+        <v>0</v>
+      </c>
     </row>
     <row r="355" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
@@ -49761,6 +50054,9 @@
       <c r="AQ355" t="s">
         <v>308</v>
       </c>
+      <c r="AR355" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="356" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
@@ -49889,6 +50185,9 @@
       <c r="AQ356">
         <v>0</v>
       </c>
+      <c r="AR356">
+        <v>0</v>
+      </c>
     </row>
     <row r="357" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
@@ -50017,6 +50316,9 @@
       <c r="AQ357">
         <v>0</v>
       </c>
+      <c r="AR357">
+        <v>0</v>
+      </c>
     </row>
     <row r="358" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
@@ -50145,6 +50447,9 @@
       <c r="AQ358">
         <v>0</v>
       </c>
+      <c r="AR358">
+        <v>0</v>
+      </c>
     </row>
     <row r="359" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
@@ -50276,6 +50581,9 @@
       <c r="AQ359" t="s">
         <v>308</v>
       </c>
+      <c r="AR359" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="360" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
@@ -50404,6 +50712,9 @@
       <c r="AQ360">
         <v>0</v>
       </c>
+      <c r="AR360">
+        <v>0</v>
+      </c>
     </row>
     <row r="361" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
@@ -50535,6 +50846,9 @@
       <c r="AQ361">
         <v>6</v>
       </c>
+      <c r="AR361">
+        <v>0</v>
+      </c>
     </row>
     <row r="362" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
@@ -58556,6 +58870,9 @@
       <c r="AQ422">
         <v>0</v>
       </c>
+      <c r="AR422">
+        <v>0</v>
+      </c>
     </row>
     <row r="423" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
@@ -58687,6 +59004,9 @@
       <c r="AQ423" t="s">
         <v>308</v>
       </c>
+      <c r="AR423" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="424" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
@@ -58815,6 +59135,9 @@
       <c r="AQ424">
         <v>0</v>
       </c>
+      <c r="AR424">
+        <v>0</v>
+      </c>
     </row>
     <row r="425" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
@@ -58943,6 +59266,9 @@
       <c r="AQ425">
         <v>0</v>
       </c>
+      <c r="AR425">
+        <v>0</v>
+      </c>
     </row>
     <row r="426" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
@@ -59071,6 +59397,9 @@
       <c r="AQ426" t="s">
         <v>308</v>
       </c>
+      <c r="AR426" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="427" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
@@ -59199,6 +59528,9 @@
       <c r="AQ427">
         <v>0</v>
       </c>
+      <c r="AR427">
+        <v>0</v>
+      </c>
     </row>
     <row r="428" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
@@ -59327,6 +59659,9 @@
       <c r="AQ428">
         <v>0</v>
       </c>
+      <c r="AR428">
+        <v>0</v>
+      </c>
     </row>
     <row r="429" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
@@ -59458,6 +59793,9 @@
       <c r="AQ429">
         <v>0</v>
       </c>
+      <c r="AR429">
+        <v>0</v>
+      </c>
     </row>
     <row r="430" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
@@ -59586,6 +59924,9 @@
       <c r="AQ430">
         <v>0</v>
       </c>
+      <c r="AR430">
+        <v>0</v>
+      </c>
     </row>
     <row r="431" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
@@ -59717,6 +60058,9 @@
       <c r="AQ431" t="s">
         <v>308</v>
       </c>
+      <c r="AR431" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="432" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
@@ -59845,8 +60189,11 @@
       <c r="AQ432">
         <v>0</v>
       </c>
+      <c r="AR432">
+        <v>0</v>
+      </c>
     </row>
-    <row r="433" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>467</v>
       </c>
@@ -59973,8 +60320,11 @@
       <c r="AQ433">
         <v>0</v>
       </c>
+      <c r="AR433">
+        <v>0</v>
+      </c>
     </row>
-    <row r="434" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>468</v>
       </c>
@@ -60101,8 +60451,11 @@
       <c r="AQ434">
         <v>0</v>
       </c>
+      <c r="AR434">
+        <v>0</v>
+      </c>
     </row>
-    <row r="435" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>469</v>
       </c>
@@ -60229,8 +60582,11 @@
       <c r="AQ435">
         <v>0</v>
       </c>
+      <c r="AR435">
+        <v>0</v>
+      </c>
     </row>
-    <row r="436" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>470</v>
       </c>
@@ -60357,8 +60713,11 @@
       <c r="AQ436">
         <v>0</v>
       </c>
+      <c r="AR436">
+        <v>0</v>
+      </c>
     </row>
-    <row r="437" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>471</v>
       </c>
@@ -60485,8 +60844,11 @@
       <c r="AQ437">
         <v>0</v>
       </c>
+      <c r="AR437">
+        <v>0</v>
+      </c>
     </row>
-    <row r="438" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>472</v>
       </c>
@@ -60610,8 +60972,11 @@
       <c r="AQ438">
         <v>0</v>
       </c>
+      <c r="AR438">
+        <v>0</v>
+      </c>
     </row>
-    <row r="439" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>473</v>
       </c>
@@ -60738,8 +61103,11 @@
       <c r="AQ439">
         <v>0</v>
       </c>
+      <c r="AR439">
+        <v>0</v>
+      </c>
     </row>
-    <row r="440" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>474</v>
       </c>
@@ -60866,8 +61234,11 @@
       <c r="AQ440">
         <v>0</v>
       </c>
+      <c r="AR440">
+        <v>0</v>
+      </c>
     </row>
-    <row r="441" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>475</v>
       </c>
@@ -60994,8 +61365,11 @@
       <c r="AQ441">
         <v>0</v>
       </c>
+      <c r="AR441">
+        <v>0</v>
+      </c>
     </row>
-    <row r="442" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>476</v>
       </c>
@@ -61125,8 +61499,11 @@
       <c r="AQ442" t="s">
         <v>308</v>
       </c>
+      <c r="AR442" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="443" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>478</v>
       </c>
@@ -61253,8 +61630,11 @@
       <c r="AQ443">
         <v>0</v>
       </c>
+      <c r="AR443">
+        <v>0</v>
+      </c>
     </row>
-    <row r="444" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
         <v>479</v>
       </c>
@@ -61384,8 +61764,11 @@
       <c r="AQ444" t="s">
         <v>308</v>
       </c>
+      <c r="AR444" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="445" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
         <v>480</v>
       </c>
@@ -61512,8 +61895,11 @@
       <c r="AQ445">
         <v>0</v>
       </c>
+      <c r="AR445">
+        <v>0</v>
+      </c>
     </row>
-    <row r="446" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
         <v>481</v>
       </c>
@@ -61640,8 +62026,11 @@
       <c r="AQ446">
         <v>0</v>
       </c>
+      <c r="AR446">
+        <v>0</v>
+      </c>
     </row>
-    <row r="447" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>482</v>
       </c>
@@ -61768,8 +62157,11 @@
       <c r="AQ447">
         <v>0</v>
       </c>
+      <c r="AR447">
+        <v>0</v>
+      </c>
     </row>
-    <row r="448" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
         <v>483</v>
       </c>
@@ -61894,6 +62286,9 @@
         <v>0</v>
       </c>
       <c r="AQ448">
+        <v>0</v>
+      </c>
+      <c r="AR448">
         <v>0</v>
       </c>
     </row>
@@ -62024,6 +62419,9 @@
       <c r="AQ449">
         <v>0</v>
       </c>
+      <c r="AR449">
+        <v>0</v>
+      </c>
     </row>
     <row r="450" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
@@ -62152,6 +62550,9 @@
       <c r="AQ450">
         <v>0</v>
       </c>
+      <c r="AR450">
+        <v>0</v>
+      </c>
     </row>
     <row r="451" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
@@ -62283,6 +62684,9 @@
       <c r="AQ451" t="s">
         <v>308</v>
       </c>
+      <c r="AR451" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="452" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
@@ -70292,8 +70696,11 @@
       <c r="AQ512">
         <v>0</v>
       </c>
+      <c r="AR512">
+        <v>0</v>
+      </c>
     </row>
-    <row r="513" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
         <v>550</v>
       </c>
@@ -70420,8 +70827,11 @@
       <c r="AQ513">
         <v>0</v>
       </c>
+      <c r="AR513">
+        <v>0</v>
+      </c>
     </row>
-    <row r="514" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
         <v>551</v>
       </c>
@@ -70548,8 +70958,11 @@
       <c r="AQ514">
         <v>0</v>
       </c>
+      <c r="AR514">
+        <v>0</v>
+      </c>
     </row>
-    <row r="515" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
         <v>552</v>
       </c>
@@ -70676,8 +71089,11 @@
       <c r="AQ515">
         <v>0</v>
       </c>
+      <c r="AR515">
+        <v>0</v>
+      </c>
     </row>
-    <row r="516" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A516" t="s">
         <v>553</v>
       </c>
@@ -70804,8 +71220,11 @@
       <c r="AQ516">
         <v>0</v>
       </c>
+      <c r="AR516">
+        <v>0</v>
+      </c>
     </row>
-    <row r="517" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
         <v>554</v>
       </c>
@@ -70935,8 +71354,11 @@
       <c r="AQ517" t="s">
         <v>308</v>
       </c>
+      <c r="AR517" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="518" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A518" t="s">
         <v>555</v>
       </c>
@@ -71066,8 +71488,11 @@
       <c r="AQ518" t="s">
         <v>308</v>
       </c>
+      <c r="AR518" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="519" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A519" t="s">
         <v>557</v>
       </c>
@@ -71194,8 +71619,11 @@
       <c r="AQ519">
         <v>0</v>
       </c>
+      <c r="AR519">
+        <v>0</v>
+      </c>
     </row>
-    <row r="520" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A520" t="s">
         <v>558</v>
       </c>
@@ -71322,8 +71750,11 @@
       <c r="AQ520">
         <v>0</v>
       </c>
+      <c r="AR520">
+        <v>0</v>
+      </c>
     </row>
-    <row r="521" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A521" t="s">
         <v>559</v>
       </c>
@@ -71450,8 +71881,11 @@
       <c r="AQ521">
         <v>0</v>
       </c>
+      <c r="AR521">
+        <v>0</v>
+      </c>
     </row>
-    <row r="522" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
         <v>560</v>
       </c>
@@ -71578,8 +72012,11 @@
       <c r="AQ522">
         <v>0</v>
       </c>
+      <c r="AR522">
+        <v>0</v>
+      </c>
     </row>
-    <row r="523" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
         <v>561</v>
       </c>
@@ -71706,8 +72143,11 @@
       <c r="AQ523">
         <v>0</v>
       </c>
+      <c r="AR523">
+        <v>0</v>
+      </c>
     </row>
-    <row r="524" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
         <v>562</v>
       </c>
@@ -71834,8 +72274,11 @@
       <c r="AQ524">
         <v>0</v>
       </c>
+      <c r="AR524">
+        <v>0</v>
+      </c>
     </row>
-    <row r="525" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
         <v>563</v>
       </c>
@@ -71962,8 +72405,11 @@
       <c r="AQ525">
         <v>0</v>
       </c>
+      <c r="AR525">
+        <v>0</v>
+      </c>
     </row>
-    <row r="526" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="526" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A526" t="s">
         <v>564</v>
       </c>
@@ -72090,8 +72536,11 @@
       <c r="AQ526">
         <v>0</v>
       </c>
+      <c r="AR526">
+        <v>0</v>
+      </c>
     </row>
-    <row r="527" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="527" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
         <v>565</v>
       </c>
@@ -72218,8 +72667,11 @@
       <c r="AQ527">
         <v>0</v>
       </c>
+      <c r="AR527">
+        <v>0</v>
+      </c>
     </row>
-    <row r="528" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="528" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A528" t="s">
         <v>566</v>
       </c>
@@ -72349,8 +72801,11 @@
       <c r="AQ528">
         <v>0</v>
       </c>
+      <c r="AR528">
+        <v>0</v>
+      </c>
     </row>
-    <row r="529" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>567</v>
       </c>
@@ -72477,8 +72932,11 @@
       <c r="AQ529">
         <v>0</v>
       </c>
+      <c r="AR529">
+        <v>0</v>
+      </c>
     </row>
-    <row r="530" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A530" t="s">
         <v>568</v>
       </c>
@@ -72605,8 +73063,11 @@
       <c r="AQ530">
         <v>0</v>
       </c>
+      <c r="AR530">
+        <v>0</v>
+      </c>
     </row>
-    <row r="531" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
         <v>569</v>
       </c>
@@ -72736,8 +73197,11 @@
       <c r="AQ531">
         <v>0</v>
       </c>
+      <c r="AR531">
+        <v>0</v>
+      </c>
     </row>
-    <row r="532" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
         <v>570</v>
       </c>
@@ -72867,8 +73331,11 @@
       <c r="AQ532">
         <v>0</v>
       </c>
+      <c r="AR532">
+        <v>0</v>
+      </c>
     </row>
-    <row r="533" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
         <v>571</v>
       </c>
@@ -72995,8 +73462,11 @@
       <c r="AQ533">
         <v>0</v>
       </c>
+      <c r="AR533">
+        <v>0</v>
+      </c>
     </row>
-    <row r="534" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A534" t="s">
         <v>572</v>
       </c>
@@ -73123,8 +73593,11 @@
       <c r="AQ534">
         <v>0</v>
       </c>
+      <c r="AR534">
+        <v>0</v>
+      </c>
     </row>
-    <row r="535" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
         <v>573</v>
       </c>
@@ -73251,8 +73724,11 @@
       <c r="AQ535">
         <v>0</v>
       </c>
+      <c r="AR535">
+        <v>0</v>
+      </c>
     </row>
-    <row r="536" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>574</v>
       </c>
@@ -73379,8 +73855,11 @@
       <c r="AQ536">
         <v>0</v>
       </c>
+      <c r="AR536">
+        <v>0</v>
+      </c>
     </row>
-    <row r="537" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
         <v>575</v>
       </c>
@@ -73507,8 +73986,11 @@
       <c r="AQ537">
         <v>0</v>
       </c>
+      <c r="AR537">
+        <v>0</v>
+      </c>
     </row>
-    <row r="538" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
         <v>576</v>
       </c>
@@ -73635,8 +74117,11 @@
       <c r="AQ538">
         <v>0</v>
       </c>
+      <c r="AR538">
+        <v>0</v>
+      </c>
     </row>
-    <row r="539" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
         <v>577</v>
       </c>
@@ -73763,8 +74248,11 @@
       <c r="AQ539">
         <v>0</v>
       </c>
+      <c r="AR539">
+        <v>0</v>
+      </c>
     </row>
-    <row r="540" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>578</v>
       </c>
@@ -73891,8 +74379,11 @@
       <c r="AQ540">
         <v>0</v>
       </c>
+      <c r="AR540">
+        <v>0</v>
+      </c>
     </row>
-    <row r="541" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
         <v>579</v>
       </c>
@@ -74019,8 +74510,11 @@
       <c r="AQ541">
         <v>0</v>
       </c>
+      <c r="AR541">
+        <v>0</v>
+      </c>
     </row>
-    <row r="542" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>580</v>
       </c>
@@ -74142,7 +74636,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="543" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
         <v>583</v>
       </c>
@@ -74261,7 +74755,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="544" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>584</v>
       </c>

</xml_diff>